<commit_message>
Update Prosecution Case Query Results and Case Filing Decision Reporting SSPs for Hawaii requirements.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/ProsecutionCaseQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/ProsecutionCaseQueryResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="300" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="5680" yWindow="1780" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="378">
   <si>
     <t>ATN [Arrest Tracking Number]</t>
   </si>
@@ -451,12 +451,6 @@
     <t>Offense</t>
   </si>
   <si>
-    <t>Subject Residence</t>
-  </si>
-  <si>
-    <t>Case Initiating Party - Organization</t>
-  </si>
-  <si>
     <t>Statute Offense Identification</t>
   </si>
   <si>
@@ -466,15 +460,9 @@
     <t>Offense Location Description</t>
   </si>
   <si>
-    <t>Anchorage</t>
-  </si>
-  <si>
     <t>Sample Data</t>
   </si>
   <si>
-    <t>ACML Corporation</t>
-  </si>
-  <si>
     <t>123 N Oak Street Apt #5</t>
   </si>
   <si>
@@ -490,9 +478,6 @@
     <t>Forgerty</t>
   </si>
   <si>
-    <t>AK</t>
-  </si>
-  <si>
     <t>Charge Statute Code Jurisdiction</t>
   </si>
   <si>
@@ -508,9 +493,6 @@
     <t>Uniform Offense Code (UOCT or UMOT)</t>
   </si>
   <si>
-    <t>Prosecution Criminal Case Filing</t>
-  </si>
-  <si>
     <t>NIEM 3.1 Mapping</t>
   </si>
   <si>
@@ -526,12 +508,6 @@
     <t>CD12951</t>
   </si>
   <si>
-    <t>Case Filing Document Category</t>
-  </si>
-  <si>
-    <t>DCN</t>
-  </si>
-  <si>
     <t>Case Filing Date</t>
   </si>
   <si>
@@ -622,12 +598,6 @@
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonPassportIdentification/nc:IdentificationJurisdiction/nc:JurisdictionText</t>
   </si>
   <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonStateIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonStateIdentification/nc:IdentificationJurisdiction/nc:JurisdictionText</t>
-  </si>
-  <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/j:PersonAugmentation/j:DriverLicense/j:DriverLicenseIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -650,9 +620,6 @@
   </si>
   <si>
     <t>Mr</t>
-  </si>
-  <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:DocumentCategoryText</t>
   </si>
   <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:DocumentCreationDate/nc:Date</t>
@@ -867,9 +834,6 @@
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Offense/nc:ActivityDate/nc:Date</t>
   </si>
   <si>
-    <t>Offense Date</t>
-  </si>
-  <si>
     <t>2016-09-12</t>
   </si>
   <si>
@@ -901,13 +865,304 @@
   </si>
   <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest/pcq-res-ext:ArrestTrackingNumberIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Court</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Case Type</t>
+  </si>
+  <si>
+    <t>Extended Case Title</t>
+  </si>
+  <si>
+    <t>Party ID</t>
+  </si>
+  <si>
+    <t>Name Suffix</t>
+  </si>
+  <si>
+    <t>Juvenile Indicator</t>
+  </si>
+  <si>
+    <t>Confidential Indicator</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Eye Color</t>
+  </si>
+  <si>
+    <t>Hair Color</t>
+  </si>
+  <si>
+    <t>SSN</t>
+  </si>
+  <si>
+    <t>Party Role</t>
+  </si>
+  <si>
+    <t>Apt/Unit Number</t>
+  </si>
+  <si>
+    <t>Country Text</t>
+  </si>
+  <si>
+    <t>Home Phone</t>
+  </si>
+  <si>
+    <t>Business Phone</t>
+  </si>
+  <si>
+    <t>Cell Phone</t>
+  </si>
+  <si>
+    <t>Subject (PersonResidence or Organization Location)</t>
+  </si>
+  <si>
+    <t>Alias First Name</t>
+  </si>
+  <si>
+    <t>Alias Middle Name</t>
+  </si>
+  <si>
+    <t>Alias Last Name</t>
+  </si>
+  <si>
+    <t>Alternate Name</t>
+  </si>
+  <si>
+    <t>Arrest Date</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>Agency Name</t>
+  </si>
+  <si>
+    <t>Booking Agency</t>
+  </si>
+  <si>
+    <t>Booking Number</t>
+  </si>
+  <si>
+    <t>Booking ID</t>
+  </si>
+  <si>
+    <t>Offender Tracking Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Number </t>
+  </si>
+  <si>
+    <t>Violation Category Text</t>
+  </si>
+  <si>
+    <t>Change to Date/Time</t>
+  </si>
+  <si>
+    <t>Violation Description</t>
+  </si>
+  <si>
+    <t>CDL</t>
+  </si>
+  <si>
+    <t>HAZ</t>
+  </si>
+  <si>
+    <t>CMV</t>
+  </si>
+  <si>
+    <t>Filing Party</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>DocumentType</t>
+  </si>
+  <si>
+    <t>Type of document</t>
+  </si>
+  <si>
+    <t>Document category</t>
+  </si>
+  <si>
+    <t>Case Filing Document Category Name</t>
+  </si>
+  <si>
+    <t>Document Category Description Text</t>
+  </si>
+  <si>
+    <t>Case Title Text</t>
+  </si>
+  <si>
+    <t>Jr</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonName/nc:PersonNameSuffixText</t>
+  </si>
+  <si>
+    <t>Use nc:VehicleAugmentation</t>
+  </si>
+  <si>
+    <t>Use j:driverLicenseAugmentation</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/j:PersonAugmentation/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/j:PersonAugmentation/j:PersonStateFingerprintIdentification/nc:IdentificationJurisdictionText/nc:IdentificationText</t>
+  </si>
+  <si>
+    <t>State vs.</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>INH</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>Party Unique ID</t>
+  </si>
+  <si>
+    <t>2016-09-12T04:30:00</t>
+  </si>
+  <si>
+    <t>Offense Date/Time</t>
+  </si>
+  <si>
+    <t>Height Unit</t>
+  </si>
+  <si>
+    <t>Weight Unit</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>LBR</t>
+  </si>
+  <si>
+    <t>SSN12345</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Defendant Party - Person</t>
+  </si>
+  <si>
+    <t>Defendant Party - Organization</t>
+  </si>
+  <si>
+    <t>Defendant Org</t>
+  </si>
+  <si>
+    <t>ACME Corporation</t>
+  </si>
+  <si>
+    <t>35765</t>
+  </si>
+  <si>
+    <t>Contact Information</t>
+  </si>
+  <si>
+    <t>Defendant@flores.com</t>
+  </si>
+  <si>
+    <t>(453) 213-0324</t>
+  </si>
+  <si>
+    <t>(456) 212-0290</t>
+  </si>
+  <si>
+    <t>(456) 121-2345</t>
+  </si>
+  <si>
+    <t>NEED TO CHECK FOR HI INFORMATION</t>
+  </si>
+  <si>
+    <t>Apt #3</t>
+  </si>
+  <si>
+    <t>21905</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Honolulu</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>B1234567</t>
+  </si>
+  <si>
+    <t>Levitt County Jail</t>
+  </si>
+  <si>
+    <t>I4567789</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Identified Person Tracking Identification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge Count Number </t>
+  </si>
+  <si>
+    <t>Charge Description Text</t>
+  </si>
+  <si>
+    <t>Charge Category Description Text</t>
+  </si>
+  <si>
+    <t>Vehicle CMV Indicator</t>
+  </si>
+  <si>
+    <t>Charge Category</t>
+  </si>
+  <si>
+    <t>Charge Description</t>
+  </si>
+  <si>
+    <t>Indicator ?</t>
+  </si>
+  <si>
+    <t>UPDATE MAPPING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1077,8 +1332,13 @@
       <sz val="12"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1163,6 +1423,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1201,7 +1473,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1343,8 +1615,70 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1457,8 +1791,50 @@
     <xf numFmtId="0" fontId="26" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="203">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -1543,6 +1919,37 @@
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -1594,6 +2001,37 @@
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="90"/>
@@ -1898,1082 +2336,1585 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.1640625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="23" style="25" customWidth="1"/>
-    <col min="3" max="3" width="77.5" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="20.5" style="15" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="23" style="25" customWidth="1"/>
+    <col min="4" max="4" width="77.5" style="13" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="B2" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="37"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28">
+      <c r="B6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28">
+      <c r="B7" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="26"/>
+    </row>
+    <row r="9" spans="1:4" ht="28">
+      <c r="B9" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>306</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28">
+      <c r="B11" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="42">
+      <c r="B12" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28">
+      <c r="B13" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="42">
+      <c r="B14" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="98">
+      <c r="B15" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A16" s="41"/>
+      <c r="B16" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="B17" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="1:4" s="2" customFormat="1">
+      <c r="A18" s="41" t="s">
+        <v>315</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>342</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A19" s="41"/>
+      <c r="B19" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="2" customFormat="1" ht="42">
+      <c r="A20" s="41"/>
+      <c r="B20" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="26"/>
+    </row>
+    <row r="22" spans="1:4" s="2" customFormat="1">
+      <c r="A22" s="41"/>
+      <c r="B22" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A23" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="2" customFormat="1" ht="42">
+      <c r="A24" s="41"/>
+      <c r="B24" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A25" s="41"/>
+      <c r="B25" s="30" t="s">
+        <v>325</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="2" customFormat="1">
+      <c r="A26" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>326</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:4" s="2" customFormat="1">
+      <c r="A27" s="41" t="s">
+        <v>320</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A28" s="41"/>
+      <c r="B28" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A29" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A30" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A31" s="41"/>
+      <c r="B31" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A32" s="41"/>
+      <c r="B32" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="2" customFormat="1">
+      <c r="A33" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="B33" s="45" t="s">
+        <v>327</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="B34" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A35" s="41"/>
+      <c r="B35" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="B36" s="48" t="s">
+        <v>370</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>372</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>371</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A39" s="41"/>
+      <c r="B39" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A40" s="41"/>
+      <c r="B40" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="2" customFormat="1" ht="42">
+      <c r="A41" s="41"/>
+      <c r="B41" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A42" s="41"/>
+      <c r="B42" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="2" customFormat="1">
+      <c r="A43" s="41"/>
+      <c r="B43" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43" s="17"/>
+    </row>
+    <row r="44" spans="1:4" s="2" customFormat="1" ht="42">
+      <c r="A44" s="41"/>
+      <c r="B44" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="2" customFormat="1" ht="42">
+      <c r="A45" s="41"/>
+      <c r="B45" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="2" customFormat="1" ht="42">
+      <c r="A46" s="41"/>
+      <c r="B46" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="2" customFormat="1" ht="28">
+      <c r="A47" s="41"/>
+      <c r="B47" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="2" customFormat="1" ht="56">
+      <c r="A48" s="41"/>
+      <c r="B48" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A49" s="41"/>
+      <c r="B49" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="2" customFormat="1" ht="38" customHeight="1">
+      <c r="A50" s="41"/>
+      <c r="B50" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="B51" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="26"/>
+    </row>
+    <row r="52" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A52" s="41"/>
+      <c r="B52" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A53" s="41"/>
+      <c r="B53" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A54" s="41"/>
+      <c r="B54" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A55" s="41" t="s">
+        <v>286</v>
+      </c>
+      <c r="B55" s="45"/>
+      <c r="C55" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="2" customFormat="1">
+      <c r="A56" s="41" t="s">
+        <v>305</v>
+      </c>
+      <c r="B56" s="45" t="s">
+        <v>302</v>
+      </c>
+      <c r="C56" s="20"/>
+      <c r="D56" s="17"/>
+    </row>
+    <row r="57" spans="1:9" s="2" customFormat="1">
+      <c r="A57" s="41"/>
+      <c r="B57" s="45" t="s">
+        <v>303</v>
+      </c>
+      <c r="C57" s="20"/>
+      <c r="D57" s="17"/>
+    </row>
+    <row r="58" spans="1:9" s="2" customFormat="1">
+      <c r="A58" s="41"/>
+      <c r="B58" s="45" t="s">
+        <v>304</v>
+      </c>
+      <c r="C58" s="20"/>
+      <c r="D58" s="17"/>
+    </row>
+    <row r="59" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A59" s="41"/>
+      <c r="B59" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A60" s="41"/>
+      <c r="B60" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A61" s="41"/>
+      <c r="B61" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="2" customFormat="1">
+      <c r="A62" s="41" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15">
-      <c r="A2" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="3" spans="1:3" s="16" customFormat="1">
-      <c r="A3" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28">
-      <c r="A7" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28">
-      <c r="A8" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="26"/>
-    </row>
-    <row r="10" spans="1:3" ht="28">
-      <c r="A10" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28">
-      <c r="A11" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="C11" s="16" t="s">
+      <c r="B62" s="45" t="s">
+        <v>340</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="D62" s="17"/>
+    </row>
+    <row r="63" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A63" s="41"/>
+      <c r="B63" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="2" customFormat="1" ht="56">
+      <c r="A64" s="41"/>
+      <c r="B64" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="2" customFormat="1" ht="56">
+      <c r="A65" s="41"/>
+      <c r="B65" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="2" customFormat="1" ht="56">
+      <c r="A66" s="41"/>
+      <c r="B66" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="2" customFormat="1">
+      <c r="A67" s="41" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="42">
-      <c r="A12" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="C12" s="16" t="s">
+      <c r="B67" s="45" t="s">
+        <v>287</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="D67" s="17"/>
+    </row>
+    <row r="68" spans="1:8" s="2" customFormat="1">
+      <c r="A68" s="41" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="28">
-      <c r="A13" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="C13" s="16" t="s">
+      <c r="B68" s="45" t="s">
+        <v>288</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="D68" s="17"/>
+    </row>
+    <row r="69" spans="1:8" s="2" customFormat="1">
+      <c r="A69" s="41" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="42">
-      <c r="A14" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="B69" s="45" t="s">
+        <v>289</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="D69" s="17"/>
+    </row>
+    <row r="70" spans="1:8" s="2" customFormat="1">
+      <c r="A70" s="41" t="s">
+        <v>343</v>
+      </c>
+      <c r="B70" s="45" t="s">
+        <v>343</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="D70" s="17"/>
+    </row>
+    <row r="71" spans="1:8" s="2" customFormat="1">
+      <c r="A71" s="41" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="98">
-      <c r="A15" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" ht="28">
-      <c r="A16" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="C16" s="16" t="s">
+      <c r="B71" s="45" t="s">
+        <v>290</v>
+      </c>
+      <c r="C71" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="D71" s="17"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="B72" s="47" t="s">
+        <v>344</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="2" customFormat="1">
+      <c r="A73" s="41" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="26"/>
-    </row>
-    <row r="18" spans="1:3" s="2" customFormat="1">
-      <c r="A18" s="29" t="s">
-        <v>281</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" ht="28">
-      <c r="A19" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" ht="42">
-      <c r="A20" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="26"/>
-    </row>
-    <row r="22" spans="1:3" s="2" customFormat="1">
-      <c r="A22" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="2" customFormat="1" ht="28">
-      <c r="A23" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="2" customFormat="1" ht="42">
-      <c r="A24" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="2" customFormat="1" ht="28">
-      <c r="A25" s="30" t="s">
-        <v>168</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="2" customFormat="1" ht="28">
-      <c r="A26" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="2" customFormat="1" ht="28">
-      <c r="A27" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="2" customFormat="1" ht="28">
-      <c r="A28" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="2" customFormat="1" ht="28">
-      <c r="A29" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="2" customFormat="1" ht="28">
-      <c r="A30" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="26"/>
-    </row>
-    <row r="32" spans="1:3" s="2" customFormat="1" ht="28">
-      <c r="A32" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="2" customFormat="1" ht="28">
-      <c r="A33" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" ht="28">
-      <c r="A34" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="2" customFormat="1" ht="42">
-      <c r="A35" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="2" customFormat="1" ht="28">
-      <c r="A36" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="2" customFormat="1">
-      <c r="A37" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="C37" s="17"/>
-    </row>
-    <row r="38" spans="1:8" s="2" customFormat="1" ht="42">
-      <c r="A38" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="2" customFormat="1" ht="42">
-      <c r="A39" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="2" customFormat="1" ht="42">
-      <c r="A40" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="2" customFormat="1" ht="28">
-      <c r="A41" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="2" customFormat="1" ht="56">
-      <c r="A42" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="2" customFormat="1" ht="42">
-      <c r="A43" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" ht="38" customHeight="1">
-      <c r="A44" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="27" t="s">
+      <c r="B73" s="46" t="s">
+        <v>292</v>
+      </c>
+      <c r="C73" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="D73" s="17"/>
+    </row>
+    <row r="74" spans="1:8" s="2" customFormat="1">
+      <c r="A74" s="41" t="s">
+        <v>293</v>
+      </c>
+      <c r="B74" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="C74" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="D74" s="17"/>
+    </row>
+    <row r="75" spans="1:8" s="2" customFormat="1">
+      <c r="A75" s="41" t="s">
+        <v>294</v>
+      </c>
+      <c r="B75" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="C75" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="D75" s="17"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B76" s="48" t="s">
+        <v>369</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="2" customFormat="1">
+      <c r="A77" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="B77" s="45" t="s">
+        <v>295</v>
+      </c>
+      <c r="C77" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="26"/>
-    </row>
-    <row r="46" spans="1:8" s="2" customFormat="1" ht="42">
-      <c r="A46" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="2" customFormat="1" ht="42">
-      <c r="A47" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="2" customFormat="1" ht="42">
-      <c r="A48" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="2" customFormat="1" ht="42">
-      <c r="A49" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="2" customFormat="1" ht="42">
-      <c r="A50" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="2" customFormat="1" ht="42">
-      <c r="A51" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" s="2" customFormat="1" ht="42">
-      <c r="A52" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" s="2" customFormat="1" ht="42">
-      <c r="A53" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B53" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" s="2" customFormat="1" ht="56">
-      <c r="A54" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" s="2" customFormat="1" ht="56">
-      <c r="A55" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B55" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B56" s="19"/>
-      <c r="C56" s="26"/>
-    </row>
-    <row r="57" spans="1:7" ht="42">
-      <c r="A57" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B57" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="42">
-      <c r="A58" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B58" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="42">
-      <c r="A59" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B59" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-    </row>
-    <row r="60" spans="1:7" ht="42">
-      <c r="A60" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="B60" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-    </row>
-    <row r="61" spans="1:7" ht="56">
-      <c r="A61" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="C61" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-    </row>
-    <row r="62" spans="1:7" ht="56">
-      <c r="A62" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-    </row>
-    <row r="63" spans="1:7" ht="42">
-      <c r="A63" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="B64" s="19"/>
-      <c r="C64" s="26"/>
-    </row>
-    <row r="65" spans="1:7" ht="42">
-      <c r="A65" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="42">
-      <c r="A66" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="C66" s="16" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="42">
-      <c r="A67" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="C67" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-    </row>
-    <row r="68" spans="1:7" ht="42">
-      <c r="A68" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="B68" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C68" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-    </row>
-    <row r="69" spans="1:7" ht="42">
-      <c r="A69" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B69" s="23" t="s">
-        <v>253</v>
-      </c>
-      <c r="C69" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-    </row>
-    <row r="70" spans="1:7" ht="42">
-      <c r="A70" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B70" s="23" t="s">
-        <v>254</v>
-      </c>
-      <c r="C70" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-    </row>
-    <row r="71" spans="1:7" ht="28">
-      <c r="A71" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B71" s="23" t="s">
-        <v>255</v>
-      </c>
-      <c r="C71" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="27" t="s">
-        <v>257</v>
-      </c>
-      <c r="B72" s="19"/>
-      <c r="C72" s="26"/>
-    </row>
-    <row r="73" spans="1:7" ht="42">
-      <c r="A73" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="23" t="s">
-        <v>258</v>
-      </c>
-      <c r="C73" s="16" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="42">
-      <c r="A74" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B74" s="23" t="s">
-        <v>259</v>
-      </c>
-      <c r="C74" s="16" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="42">
-      <c r="A75" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B75" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="C75" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-    </row>
-    <row r="76" spans="1:7" ht="42">
-      <c r="A76" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="B76" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="C76" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-    </row>
-    <row r="77" spans="1:7" ht="42">
-      <c r="A77" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B77" s="23" t="s">
-        <v>267</v>
-      </c>
-      <c r="C77" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-    </row>
-    <row r="78" spans="1:7" ht="42">
-      <c r="A78" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B78" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C78" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="D78" s="3"/>
+      <c r="D77" s="17"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="B78" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="C78" s="19"/>
+      <c r="D78" s="26"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
-    </row>
-    <row r="79" spans="1:7" ht="28">
-      <c r="A79" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B79" s="23" t="s">
-        <v>268</v>
-      </c>
-      <c r="C79" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="D79" s="3"/>
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="B79" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="D79" s="16" t="s">
+        <v>263</v>
+      </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="B80" s="19"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="3"/>
+      <c r="H79" s="3"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B80" s="48" t="s">
+        <v>285</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="D80" s="16"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="B81" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C81" s="16" t="s">
-        <v>274</v>
-      </c>
-      <c r="D81" s="3"/>
+      <c r="H80" s="3"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B81" s="48" t="s">
+        <v>295</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="D81" s="16"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="B82" s="19"/>
-      <c r="C82" s="26"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-    </row>
-    <row r="83" spans="1:7" ht="56">
-      <c r="A83" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="C83" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-    </row>
-    <row r="84" spans="1:7" ht="56">
-      <c r="A84" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="B84" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="C84" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-    </row>
-    <row r="85" spans="1:7" ht="56">
-      <c r="A85" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="B85" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="C85" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="D85" s="3"/>
+      <c r="H81" s="3"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="B82" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C82" s="19"/>
+      <c r="D82" s="26"/>
+    </row>
+    <row r="83" spans="1:8" ht="42">
+      <c r="B83" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C83" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="D83" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="42">
+      <c r="B84" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C84" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D84" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="42">
+      <c r="B85" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D85" s="16" t="s">
+        <v>196</v>
+      </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-    </row>
-    <row r="86" spans="1:7" ht="56">
-      <c r="A86" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="B86" s="18">
-        <v>21905</v>
-      </c>
-      <c r="C86" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="D86" s="3"/>
+      <c r="H85" s="3"/>
+    </row>
+    <row r="86" spans="1:8" ht="42">
+      <c r="B86" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="C86" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D86" s="16" t="s">
+        <v>198</v>
+      </c>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="B87" s="24"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="3"/>
+      <c r="H86" s="3"/>
+    </row>
+    <row r="87" spans="1:8" ht="56">
+      <c r="B87" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C87" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="D87" s="16" t="s">
+        <v>225</v>
+      </c>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="B88" s="24"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="3"/>
+      <c r="H87" s="3"/>
+    </row>
+    <row r="88" spans="1:8" ht="56">
+      <c r="B88" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C88" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>226</v>
+      </c>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="B89" s="24"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="3"/>
+      <c r="H88" s="3"/>
+    </row>
+    <row r="89" spans="1:8" ht="42">
+      <c r="B89" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C89" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>227</v>
+      </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="B90" s="24"/>
-      <c r="C90" s="10"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="B91" s="24"/>
-      <c r="C91" s="10"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="3"/>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="B92" s="24"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="B93" s="24"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="3"/>
+      <c r="H89" s="3"/>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="B90" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C90" s="19"/>
+      <c r="D90" s="26"/>
+    </row>
+    <row r="91" spans="1:8" ht="42">
+      <c r="B91" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C91" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="42">
+      <c r="B92" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C92" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="D92" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="42">
+      <c r="B93" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C93" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>238</v>
+      </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="B94" s="24"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="3"/>
+      <c r="H93" s="3"/>
+    </row>
+    <row r="94" spans="1:8" ht="42">
+      <c r="B94" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="C94" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>239</v>
+      </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
-    </row>
-    <row r="95" spans="1:7">
-      <c r="B95" s="24"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="3"/>
+      <c r="H94" s="3"/>
+    </row>
+    <row r="95" spans="1:8" ht="42">
+      <c r="B95" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C95" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="D95" s="16" t="s">
+        <v>240</v>
+      </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+    </row>
+    <row r="96" spans="1:8" ht="42">
+      <c r="B96" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C96" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+    </row>
+    <row r="97" spans="1:8" ht="28">
+      <c r="B97" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C97" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="B98" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="C98" s="19"/>
+      <c r="D98" s="26"/>
+    </row>
+    <row r="99" spans="1:8" ht="42">
+      <c r="B99" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C99" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="42">
+      <c r="B100" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C100" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="42">
+      <c r="B101" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C101" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+    </row>
+    <row r="102" spans="1:8" ht="42">
+      <c r="B102" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="C102" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="D102" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+    </row>
+    <row r="103" spans="1:8" ht="42">
+      <c r="B103" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C103" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="1:8" ht="42">
+      <c r="B104" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C104" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D104" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+    </row>
+    <row r="105" spans="1:8" ht="28">
+      <c r="B105" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C105" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="D105" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="B106" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="C106" s="19"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+    </row>
+    <row r="107" spans="1:8" ht="56">
+      <c r="B107" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C107" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B108" s="48" t="s">
+        <v>296</v>
+      </c>
+      <c r="C108" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="D108" s="16"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+    </row>
+    <row r="109" spans="1:8" ht="56">
+      <c r="B109" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+    </row>
+    <row r="110" spans="1:8" ht="56">
+      <c r="B110" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="C110" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="3"/>
+      <c r="H110" s="3"/>
+    </row>
+    <row r="111" spans="1:8" ht="56">
+      <c r="B111" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C111" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="D111" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="B112" s="48" t="s">
+        <v>297</v>
+      </c>
+      <c r="C112" s="38" t="s">
+        <v>362</v>
+      </c>
+      <c r="D112" s="39"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="B113" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="C113" s="19"/>
+      <c r="D113" s="26"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
+    </row>
+    <row r="114" spans="1:8" s="2" customFormat="1">
+      <c r="A114" s="41" t="s">
+        <v>291</v>
+      </c>
+      <c r="B114" s="46" t="s">
+        <v>291</v>
+      </c>
+      <c r="C114" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="D114" s="17"/>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="B115" s="48" t="s">
+        <v>298</v>
+      </c>
+      <c r="C115" s="24" t="s">
+        <v>356</v>
+      </c>
+      <c r="D115" s="10"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="3"/>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="B116" s="48" t="s">
+        <v>299</v>
+      </c>
+      <c r="C116" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="D116" s="10"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+      <c r="H116" s="3"/>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B117" s="48" t="s">
+        <v>300</v>
+      </c>
+      <c r="C117" s="24" t="s">
+        <v>358</v>
+      </c>
+      <c r="D117" s="10"/>
+      <c r="E117" s="3"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="3"/>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="B118" s="27" t="s">
+        <v>307</v>
+      </c>
+      <c r="C118" s="19"/>
+      <c r="D118" s="26"/>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="B119" s="47" t="s">
+        <v>308</v>
+      </c>
+      <c r="C119" s="24" t="s">
+        <v>366</v>
+      </c>
+      <c r="D119" s="10"/>
+      <c r="E119" s="3"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
+      <c r="H119" s="3"/>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B120" s="47" t="s">
+        <v>311</v>
+      </c>
+      <c r="C120" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="D120" s="10"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
+      <c r="H120" s="3"/>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" s="50"/>
+      <c r="C121" s="51"/>
+      <c r="D121" s="31"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="3"/>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" s="50" t="s">
+        <v>317</v>
+      </c>
+      <c r="B122" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="C122" s="51" t="s">
+        <v>376</v>
+      </c>
+      <c r="D122" s="31"/>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" s="50" t="s">
+        <v>318</v>
+      </c>
+      <c r="B123" s="40" t="s">
+        <v>330</v>
+      </c>
+      <c r="C123" s="51" t="s">
+        <v>376</v>
+      </c>
+      <c r="D123" s="31"/>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" s="50" t="s">
+        <v>319</v>
+      </c>
+      <c r="B124" s="40" t="s">
+        <v>373</v>
+      </c>
+      <c r="C124" s="51" t="s">
+        <v>376</v>
+      </c>
+      <c r="D124" s="31"/>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" s="50"/>
+      <c r="C125" s="51"/>
+      <c r="D125" s="31"/>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" s="50"/>
+      <c r="B126" s="31" t="s">
+        <v>377</v>
+      </c>
+      <c r="C126" s="51"/>
+      <c r="D126" s="31"/>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" s="50"/>
+      <c r="C127" s="51"/>
+      <c r="D127" s="31"/>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" s="50"/>
+      <c r="C128" s="51"/>
+      <c r="D128" s="31"/>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="50"/>
+      <c r="C129" s="51"/>
+      <c r="D129" s="31"/>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="50"/>
+      <c r="C130" s="51"/>
+      <c r="D130" s="31"/>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="50"/>
+      <c r="C131" s="51"/>
+      <c r="D131" s="31"/>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="50"/>
+      <c r="C132" s="51"/>
+      <c r="D132" s="31"/>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="50"/>
+      <c r="C133" s="51"/>
+      <c r="D133" s="31"/>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="50"/>
+      <c r="C134" s="51"/>
+      <c r="D134" s="31"/>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="50"/>
+      <c r="C135" s="51"/>
+      <c r="D135" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated SSP based on Hawaii requirements.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/ProsecutionCaseQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/ProsecutionCaseQueryResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="1780" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="-27020" yWindow="1840" windowWidth="27300" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="492">
   <si>
     <t>ATN [Arrest Tracking Number]</t>
   </si>
@@ -508,9 +508,6 @@
     <t>CD12951</t>
   </si>
   <si>
-    <t>Case Filing Date</t>
-  </si>
-  <si>
     <t>2016-10-13</t>
   </si>
   <si>
@@ -647,9 +644,6 @@
   </si>
   <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/nc:CaseFiling/nc:DocumentCategoryName</t>
-  </si>
-  <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/nc:CaseFiling/nc:DocumentFiledDate/nc:Date</t>
   </si>
   <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCourt/nc:OrganizationName</t>
@@ -879,12 +873,6 @@
     <t>Extended Case Title</t>
   </si>
   <si>
-    <t>Party ID</t>
-  </si>
-  <si>
-    <t>Name Suffix</t>
-  </si>
-  <si>
     <t>Juvenile Indicator</t>
   </si>
   <si>
@@ -930,21 +918,6 @@
     <t>Subject (PersonResidence or Organization Location)</t>
   </si>
   <si>
-    <t>Alias First Name</t>
-  </si>
-  <si>
-    <t>Alias Middle Name</t>
-  </si>
-  <si>
-    <t>Alias Last Name</t>
-  </si>
-  <si>
-    <t>Alternate Name</t>
-  </si>
-  <si>
-    <t>Arrest Date</t>
-  </si>
-  <si>
     <t>Booking</t>
   </si>
   <si>
@@ -954,9 +927,6 @@
     <t>Booking Agency</t>
   </si>
   <si>
-    <t>Booking Number</t>
-  </si>
-  <si>
     <t>Booking ID</t>
   </si>
   <si>
@@ -966,15 +936,9 @@
     <t xml:space="preserve">Count Number </t>
   </si>
   <si>
-    <t>Violation Category Text</t>
-  </si>
-  <si>
     <t>Change to Date/Time</t>
   </si>
   <si>
-    <t>Violation Description</t>
-  </si>
-  <si>
     <t>CDL</t>
   </si>
   <si>
@@ -984,12 +948,6 @@
     <t>CMV</t>
   </si>
   <si>
-    <t>Filing Party</t>
-  </si>
-  <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest/nc:ActivityDate/nc:Date</t>
-  </si>
-  <si>
     <t>DocumentType</t>
   </si>
   <si>
@@ -1071,21 +1029,12 @@
     <t>false</t>
   </si>
   <si>
-    <t>Defendant Party - Person</t>
-  </si>
-  <si>
     <t>Defendant Party - Organization</t>
   </si>
   <si>
-    <t>Defendant Org</t>
-  </si>
-  <si>
     <t>ACME Corporation</t>
   </si>
   <si>
-    <t>35765</t>
-  </si>
-  <si>
     <t>Contact Information</t>
   </si>
   <si>
@@ -1101,9 +1050,6 @@
     <t>(456) 121-2345</t>
   </si>
   <si>
-    <t>NEED TO CHECK FOR HI INFORMATION</t>
-  </si>
-  <si>
     <t>Apt #3</t>
   </si>
   <si>
@@ -1152,17 +1098,413 @@
     <t>Charge Description</t>
   </si>
   <si>
-    <t>Indicator ?</t>
-  </si>
-  <si>
-    <t>UPDATE MAPPING</t>
+    <t>Court Type</t>
+  </si>
+  <si>
+    <t>Domestic Violence</t>
+  </si>
+  <si>
+    <t>MOVE FROM PERSON</t>
+  </si>
+  <si>
+    <t>Confidential</t>
+  </si>
+  <si>
+    <t>Short Case Title</t>
+  </si>
+  <si>
+    <t>Case Description</t>
+  </si>
+  <si>
+    <t>Activity Description Text</t>
+  </si>
+  <si>
+    <t>2016-11-13:02:40:00</t>
+  </si>
+  <si>
+    <t>Filing Date/Time</t>
+  </si>
+  <si>
+    <t>Case Filing Date/Time</t>
+  </si>
+  <si>
+    <t>Party Role Text</t>
+  </si>
+  <si>
+    <t>Party Type</t>
+  </si>
+  <si>
+    <t>Party Type Text</t>
+  </si>
+  <si>
+    <t>Defendant Name Prefix</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>Defendant Given Name</t>
+  </si>
+  <si>
+    <t>Defendant Sur Name</t>
+  </si>
+  <si>
+    <t>Defendant Name Suffix</t>
+  </si>
+  <si>
+    <t>Party Confidential Indicator</t>
+  </si>
+  <si>
+    <t>Defendant Party - Person/Organization</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Sex Text</t>
+  </si>
+  <si>
+    <t>Eye Color Text</t>
+  </si>
+  <si>
+    <t>Address Type</t>
+  </si>
+  <si>
+    <t>Location Category Text</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Preferred</t>
+  </si>
+  <si>
+    <t>Default Location Indicator</t>
+  </si>
+  <si>
+    <t>Preferred Location Indicator</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Alias/Identity First Name</t>
+  </si>
+  <si>
+    <t>Alias/Identity Middle Name</t>
+  </si>
+  <si>
+    <t>Alias/Identity Last Name</t>
+  </si>
+  <si>
+    <t>Arrest for</t>
+  </si>
+  <si>
+    <t>Arrest Date/Time</t>
+  </si>
+  <si>
+    <t>LEO</t>
+  </si>
+  <si>
+    <t>Arrest Report #</t>
+  </si>
+  <si>
+    <t>Incident</t>
+  </si>
+  <si>
+    <t>Incident #</t>
+  </si>
+  <si>
+    <t>Incident Number</t>
+  </si>
+  <si>
+    <t>Violation Date/Time</t>
+  </si>
+  <si>
+    <t>Activity Date/Time</t>
+  </si>
+  <si>
+    <t>Charge Code</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Qualifier</t>
+  </si>
+  <si>
+    <t>Charge Qualifier</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>Booking #</t>
+  </si>
+  <si>
+    <t>CHECK WITH HAWAII ON INFO</t>
+  </si>
+  <si>
+    <t>Method of Case Initiation</t>
+  </si>
+  <si>
+    <t>Violation For</t>
+  </si>
+  <si>
+    <t>Arrest Detail</t>
+  </si>
+  <si>
+    <t>Date Range</t>
+  </si>
+  <si>
+    <t>Document Category</t>
+  </si>
+  <si>
+    <t>Filing Parties</t>
+  </si>
+  <si>
+    <t>In Response To</t>
+  </si>
+  <si>
+    <t>Supporting Doc For</t>
+  </si>
+  <si>
+    <t>Attached Lead Document</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>10/11</t>
+  </si>
+  <si>
+    <t>12-Ext</t>
+  </si>
+  <si>
+    <t>13-Ext</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20-Ext</t>
+  </si>
+  <si>
+    <t>21-Ext</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>Hair Color Text</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34-Ext</t>
+  </si>
+  <si>
+    <t>35-Ext</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>Identity</t>
+  </si>
+  <si>
+    <t>Alias First</t>
+  </si>
+  <si>
+    <t>Alias Middle</t>
+  </si>
+  <si>
+    <t>Alias Last</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51/52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>55/62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>59/64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66/67</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>DL #</t>
+  </si>
+  <si>
+    <t>DL State</t>
+  </si>
+  <si>
+    <t>Suffix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1337,8 +1679,14 @@
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1423,20 +1771,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1444,36 +1780,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="203">
+  <cellStyleXfs count="261">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1677,8 +1985,66 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1725,70 +2091,13 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1797,31 +2106,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1833,8 +2118,59 @@
     <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="203">
+  <cellStyles count="261">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -1950,6 +2286,35 @@
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2032,6 +2397,35 @@
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="90"/>
@@ -2336,1585 +2730,2112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:J158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138:B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" style="15" customWidth="1"/>
-    <col min="2" max="2" width="37.1640625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="23" style="25" customWidth="1"/>
-    <col min="4" max="4" width="77.5" style="13" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="7.83203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="37.1640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="23" style="17" customWidth="1"/>
+    <col min="5" max="5" width="77.5" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15">
+      <c r="C2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="C3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="C4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28">
+      <c r="C6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28">
+      <c r="C7" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>460</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>461</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>406</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>469</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>406</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>463</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>406</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:5" ht="28">
+      <c r="A12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>464</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>462</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:5" ht="28">
+      <c r="A14" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>470</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="42">
+      <c r="C15" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28">
+      <c r="C16" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="42">
+      <c r="C17" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="98">
+      <c r="C18" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A19" s="21"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="C20" s="28" t="s">
+        <v>395</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1">
+      <c r="A21" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>471</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="27"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="C22" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1">
+      <c r="A23" s="39" t="s">
+        <v>304</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A24" s="21"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A25" s="21"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="C26" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30"/>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1">
+      <c r="A27" s="21"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A28" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="B28" s="41">
+        <v>4</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A29" s="21"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A30" s="21"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="36" t="s">
+        <v>311</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1">
+      <c r="A31" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="B31" s="26"/>
+      <c r="C31" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="E31" s="27"/>
+    </row>
+    <row r="32" spans="1:5" s="2" customFormat="1">
+      <c r="A32" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="B32" s="41">
+        <v>5</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>406</v>
+      </c>
+      <c r="D32" s="38"/>
+      <c r="E32" s="27"/>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1">
+      <c r="A33" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>417</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="E33" s="27"/>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A34" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="B34" s="41">
+        <v>1</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A35" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="B35" s="41">
+        <v>2</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A36" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="B36" s="26">
+        <v>3</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A37" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="B37" s="26">
+        <v>6</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="B38" s="26">
+        <v>7</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="D38" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1">
+      <c r="A39" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="B39" s="41">
+        <v>9</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>363</v>
+      </c>
+      <c r="E39" s="39"/>
+    </row>
+    <row r="40" spans="1:5" s="2" customFormat="1">
+      <c r="A40" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="B40" s="41">
+        <v>8</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>320</v>
+      </c>
+      <c r="E40" s="27"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="C41" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="29"/>
+      <c r="E41" s="30"/>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A42" s="21"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="2" customFormat="1">
+      <c r="A43" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="B43" s="41" t="s">
+        <v>468</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="D43" s="26"/>
+      <c r="E43" s="27"/>
+    </row>
+    <row r="44" spans="1:5" s="2" customFormat="1">
+      <c r="A44" s="21" t="s">
+        <v>410</v>
+      </c>
+      <c r="B44" s="41" t="s">
+        <v>473</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="D44" s="26"/>
+      <c r="E44" s="27"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>472</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="15" t="s">
+        <v>398</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="D46" s="22"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="C47" s="15"/>
+      <c r="D47" s="22"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="C48" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="40" t="s">
+        <v>477</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A50" s="21"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="E50" s="27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A51" s="21"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E51" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A52" s="21"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A53" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="B53" s="41" t="s">
+        <v>476</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="2" customFormat="1">
+      <c r="A54" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>475</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="D54" s="37"/>
+      <c r="E54" s="27"/>
+    </row>
+    <row r="55" spans="1:10" s="2" customFormat="1">
+      <c r="A55" s="21"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E55" s="27"/>
+    </row>
+    <row r="56" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A56" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="B56" s="41" t="s">
+        <v>321</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="E56" s="27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A57" s="21"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A58" s="21"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="E58" s="27" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A59" s="21"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="2" customFormat="1" ht="56">
+      <c r="A60" s="21"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="E60" s="27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A61" s="21"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="E61" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="2" customFormat="1" ht="38" customHeight="1">
+      <c r="A62" s="21"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="E62" s="27" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="C63" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="29"/>
+      <c r="E63" s="30"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="B64" s="40" t="s">
+        <v>420</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="D64" s="22"/>
+      <c r="E64" s="20"/>
+    </row>
+    <row r="65" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A65" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B65" s="41" t="s">
+        <v>421</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="D65" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A66" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B66" s="41" t="s">
+        <v>422</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="E66" s="27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A67" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B67" s="41" t="s">
+        <v>423</v>
+      </c>
+      <c r="C67" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="D67" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="E67" s="27" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A68" s="21" t="s">
+        <v>491</v>
+      </c>
+      <c r="B68" s="41" t="s">
+        <v>424</v>
+      </c>
+      <c r="C68" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="D68" s="37" t="s">
+        <v>314</v>
+      </c>
+      <c r="E68" s="27" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="2" customFormat="1">
+      <c r="A69" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>428</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="D69" s="37"/>
+      <c r="E69" s="27"/>
+    </row>
+    <row r="70" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A70" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B70" s="41" t="s">
+        <v>429</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="E70" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A71" s="21"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D71" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="E71" s="27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A72" s="21"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D72" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="E72" s="27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="2" customFormat="1">
+      <c r="A73" s="21"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="D73" s="37" t="s">
+        <v>325</v>
+      </c>
+      <c r="E73" s="27"/>
+    </row>
+    <row r="74" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A74" s="21" t="s">
+        <v>488</v>
+      </c>
+      <c r="B74" s="41" t="s">
+        <v>438</v>
+      </c>
+      <c r="C74" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D74" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="E74" s="27" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="2" customFormat="1" ht="56">
+      <c r="A75" s="21"/>
+      <c r="B75" s="26"/>
+      <c r="C75" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D75" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="E75" s="27" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="2" customFormat="1" ht="56">
+      <c r="A76" s="21" t="s">
+        <v>489</v>
+      </c>
+      <c r="B76" s="41" t="s">
+        <v>435</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D76" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>273</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="B2" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28">
-      <c r="B6" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="E76" s="27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="2" customFormat="1" ht="56">
+      <c r="A77" s="21" t="s">
+        <v>490</v>
+      </c>
+      <c r="B77" s="41" t="s">
+        <v>436</v>
+      </c>
+      <c r="C77" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D77" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="E77" s="27" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="2" customFormat="1">
+      <c r="A78" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B78" s="41" t="s">
+        <v>427</v>
+      </c>
+      <c r="C78" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="D78" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="E78" s="27"/>
+    </row>
+    <row r="79" spans="1:5" s="2" customFormat="1">
+      <c r="A79" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="B79" s="41" t="s">
+        <v>430</v>
+      </c>
+      <c r="C79" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="D79" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="E79" s="27"/>
+    </row>
+    <row r="80" spans="1:5" s="2" customFormat="1">
+      <c r="A80" s="21"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="D80" s="37" t="s">
+        <v>322</v>
+      </c>
+      <c r="E80" s="27"/>
+    </row>
+    <row r="81" spans="1:9" s="2" customFormat="1">
+      <c r="A81" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="B81" s="41" t="s">
+        <v>431</v>
+      </c>
+      <c r="C81" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="D81" s="37" t="s">
+        <v>331</v>
+      </c>
+      <c r="E81" s="27"/>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="C82" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="2" customFormat="1">
+      <c r="A83" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="B83" s="41" t="s">
+        <v>432</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="D83" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="E83" s="27"/>
+    </row>
+    <row r="84" spans="1:9" s="2" customFormat="1">
+      <c r="A84" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="B84" s="41" t="s">
+        <v>433</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>434</v>
+      </c>
+      <c r="D84" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="E84" s="27"/>
+    </row>
+    <row r="85" spans="1:9" s="2" customFormat="1">
+      <c r="A85" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="B85" s="41" t="s">
+        <v>437</v>
+      </c>
+      <c r="C85" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D85" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="E85" s="27"/>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="B86" s="40" t="s">
+        <v>467</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="B87" s="40" t="s">
+        <v>456</v>
+      </c>
+      <c r="C87" s="28" t="s">
+        <v>452</v>
+      </c>
+      <c r="D87" s="29"/>
+      <c r="E87" s="30"/>
+    </row>
+    <row r="88" spans="1:9" s="2" customFormat="1">
+      <c r="A88" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="B88" s="41" t="s">
+        <v>457</v>
+      </c>
+      <c r="C88" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="D88" s="37"/>
+      <c r="E88" s="27"/>
+    </row>
+    <row r="89" spans="1:9" s="2" customFormat="1">
+      <c r="A89" s="21" t="s">
+        <v>454</v>
+      </c>
+      <c r="B89" s="41" t="s">
+        <v>458</v>
+      </c>
+      <c r="C89" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="D89" s="37"/>
+      <c r="E89" s="27"/>
+    </row>
+    <row r="90" spans="1:9" s="2" customFormat="1">
+      <c r="A90" s="21" t="s">
+        <v>455</v>
+      </c>
+      <c r="B90" s="41" t="s">
+        <v>459</v>
+      </c>
+      <c r="C90" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="D90" s="37"/>
+      <c r="E90" s="27"/>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="C91" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="D91" s="29"/>
+      <c r="E91" s="30"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="C92" s="15" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" s="2" customFormat="1">
+      <c r="A93" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="B93" s="26" t="s">
+        <v>419</v>
+      </c>
+      <c r="C93" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="D93" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="27"/>
+    </row>
+    <row r="94" spans="1:9" s="2" customFormat="1">
+      <c r="A94" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="B94" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="C94" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="D94" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28">
-      <c r="B7" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="26"/>
-    </row>
-    <row r="9" spans="1:4" ht="28">
-      <c r="B9" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="B10" s="43" t="s">
-        <v>306</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="28">
-      <c r="B11" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="42">
-      <c r="B12" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="28">
-      <c r="B13" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="42">
-      <c r="B14" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="98">
-      <c r="B15" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A16" s="41"/>
-      <c r="B16" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>268</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="B17" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="18" spans="1:4" s="2" customFormat="1">
-      <c r="A18" s="41" t="s">
-        <v>315</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>342</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A19" s="41"/>
-      <c r="B19" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="2" customFormat="1" ht="42">
-      <c r="A20" s="41"/>
-      <c r="B20" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="B21" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="26"/>
-    </row>
-    <row r="22" spans="1:4" s="2" customFormat="1">
-      <c r="A22" s="41"/>
-      <c r="B22" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A23" s="41" t="s">
-        <v>283</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="2" customFormat="1" ht="42">
-      <c r="A24" s="41"/>
-      <c r="B24" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A25" s="41"/>
-      <c r="B25" s="30" t="s">
-        <v>325</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="2" customFormat="1">
-      <c r="A26" s="41" t="s">
-        <v>322</v>
-      </c>
-      <c r="B26" s="44" t="s">
-        <v>326</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>323</v>
-      </c>
-      <c r="D26" s="17"/>
-    </row>
-    <row r="27" spans="1:4" s="2" customFormat="1">
-      <c r="A27" s="41" t="s">
-        <v>320</v>
-      </c>
-      <c r="B27" s="42" t="s">
-        <v>359</v>
-      </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="17"/>
-    </row>
-    <row r="28" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A28" s="41"/>
-      <c r="B28" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A29" s="41" t="s">
-        <v>281</v>
-      </c>
-      <c r="B29" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A30" s="41" t="s">
-        <v>282</v>
-      </c>
-      <c r="B30" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A31" s="41"/>
-      <c r="B31" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A32" s="41"/>
-      <c r="B32" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="2" customFormat="1">
-      <c r="A33" s="41" t="s">
-        <v>284</v>
-      </c>
-      <c r="B33" s="45" t="s">
-        <v>327</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="D33" s="17"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="B34" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="26"/>
-    </row>
-    <row r="35" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A35" s="41"/>
-      <c r="B35" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="B36" s="48" t="s">
-        <v>370</v>
-      </c>
-      <c r="C36" s="49" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="B37" s="47" t="s">
-        <v>372</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="B38" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="C38" s="49" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A39" s="41"/>
-      <c r="B39" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A40" s="41"/>
-      <c r="B40" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="2" customFormat="1" ht="42">
-      <c r="A41" s="41"/>
-      <c r="B41" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A42" s="41"/>
-      <c r="B42" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="2" customFormat="1">
-      <c r="A43" s="41"/>
-      <c r="B43" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="D43" s="17"/>
-    </row>
-    <row r="44" spans="1:4" s="2" customFormat="1" ht="42">
-      <c r="A44" s="41"/>
-      <c r="B44" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="2" customFormat="1" ht="42">
-      <c r="A45" s="41"/>
-      <c r="B45" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="2" customFormat="1" ht="42">
-      <c r="A46" s="41"/>
-      <c r="B46" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="2" customFormat="1" ht="28">
-      <c r="A47" s="41"/>
-      <c r="B47" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="2" customFormat="1" ht="56">
-      <c r="A48" s="41"/>
-      <c r="B48" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A49" s="41"/>
-      <c r="B49" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="2" customFormat="1" ht="38" customHeight="1">
-      <c r="A50" s="41"/>
-      <c r="B50" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>260</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="B51" s="27" t="s">
-        <v>349</v>
-      </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="26"/>
-    </row>
-    <row r="52" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A52" s="41"/>
-      <c r="B52" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="D52" s="17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A53" s="41"/>
-      <c r="B53" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C53" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A54" s="41"/>
-      <c r="B54" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A55" s="41" t="s">
-        <v>286</v>
-      </c>
-      <c r="B55" s="45"/>
-      <c r="C55" s="20" t="s">
-        <v>328</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" s="2" customFormat="1">
-      <c r="A56" s="41" t="s">
-        <v>305</v>
-      </c>
-      <c r="B56" s="45" t="s">
-        <v>302</v>
-      </c>
-      <c r="C56" s="20"/>
-      <c r="D56" s="17"/>
-    </row>
-    <row r="57" spans="1:9" s="2" customFormat="1">
-      <c r="A57" s="41"/>
-      <c r="B57" s="45" t="s">
-        <v>303</v>
-      </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="17"/>
-    </row>
-    <row r="58" spans="1:9" s="2" customFormat="1">
-      <c r="A58" s="41"/>
-      <c r="B58" s="45" t="s">
-        <v>304</v>
-      </c>
-      <c r="C58" s="20"/>
-      <c r="D58" s="17"/>
-    </row>
-    <row r="59" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A59" s="41"/>
-      <c r="B59" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A60" s="41"/>
-      <c r="B60" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A61" s="41"/>
-      <c r="B61" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C61" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" s="2" customFormat="1">
-      <c r="A62" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="B62" s="45" t="s">
-        <v>340</v>
-      </c>
-      <c r="C62" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="D62" s="17"/>
-    </row>
-    <row r="63" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A63" s="41"/>
-      <c r="B63" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="C63" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="2" customFormat="1" ht="56">
-      <c r="A64" s="41"/>
-      <c r="B64" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="C64" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="2" customFormat="1" ht="56">
-      <c r="A65" s="41"/>
-      <c r="B65" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C65" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="2" customFormat="1" ht="56">
-      <c r="A66" s="41"/>
-      <c r="B66" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C66" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" s="2" customFormat="1">
-      <c r="A67" s="41" t="s">
-        <v>287</v>
-      </c>
-      <c r="B67" s="45" t="s">
-        <v>287</v>
-      </c>
-      <c r="C67" s="20" t="s">
-        <v>348</v>
-      </c>
-      <c r="D67" s="17"/>
-    </row>
-    <row r="68" spans="1:8" s="2" customFormat="1">
-      <c r="A68" s="41" t="s">
-        <v>288</v>
-      </c>
-      <c r="B68" s="45" t="s">
-        <v>288</v>
-      </c>
-      <c r="C68" s="20" t="s">
-        <v>348</v>
-      </c>
-      <c r="D68" s="17"/>
-    </row>
-    <row r="69" spans="1:8" s="2" customFormat="1">
-      <c r="A69" s="41" t="s">
-        <v>289</v>
-      </c>
-      <c r="B69" s="45" t="s">
-        <v>289</v>
-      </c>
-      <c r="C69" s="20" t="s">
+      <c r="E94" s="27"/>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="C95" s="28" t="s">
         <v>335</v>
       </c>
-      <c r="D69" s="17"/>
-    </row>
-    <row r="70" spans="1:8" s="2" customFormat="1">
-      <c r="A70" s="41" t="s">
-        <v>343</v>
-      </c>
-      <c r="B70" s="45" t="s">
-        <v>343</v>
-      </c>
-      <c r="C70" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="D70" s="17"/>
-    </row>
-    <row r="71" spans="1:8" s="2" customFormat="1">
-      <c r="A71" s="41" t="s">
-        <v>290</v>
-      </c>
-      <c r="B71" s="45" t="s">
-        <v>290</v>
-      </c>
-      <c r="C71" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="D71" s="17"/>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="B72" s="47" t="s">
-        <v>344</v>
-      </c>
-      <c r="C72" s="25" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" s="2" customFormat="1">
-      <c r="A73" s="41" t="s">
-        <v>292</v>
-      </c>
-      <c r="B73" s="46" t="s">
-        <v>292</v>
-      </c>
-      <c r="C73" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="D73" s="17"/>
-    </row>
-    <row r="74" spans="1:8" s="2" customFormat="1">
-      <c r="A74" s="41" t="s">
-        <v>293</v>
-      </c>
-      <c r="B74" s="46" t="s">
-        <v>293</v>
-      </c>
-      <c r="C74" s="20" t="s">
-        <v>338</v>
-      </c>
-      <c r="D74" s="17"/>
-    </row>
-    <row r="75" spans="1:8" s="2" customFormat="1">
-      <c r="A75" s="41" t="s">
-        <v>294</v>
-      </c>
-      <c r="B75" s="45" t="s">
-        <v>294</v>
-      </c>
-      <c r="C75" s="20" t="s">
-        <v>347</v>
-      </c>
-      <c r="D75" s="17"/>
-    </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="B76" s="48" t="s">
-        <v>369</v>
-      </c>
-      <c r="C76" s="25" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" s="2" customFormat="1">
-      <c r="A77" s="41" t="s">
-        <v>295</v>
-      </c>
-      <c r="B77" s="45" t="s">
-        <v>295</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="17"/>
-    </row>
-    <row r="78" spans="1:8">
-      <c r="B78" s="27" t="s">
-        <v>350</v>
-      </c>
-      <c r="C78" s="19"/>
-      <c r="D78" s="26"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-    </row>
-    <row r="79" spans="1:8">
-      <c r="B79" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C79" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="D79" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-    </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="B80" s="48" t="s">
-        <v>285</v>
-      </c>
-      <c r="C80" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="D80" s="16"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-    </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="B81" s="48" t="s">
-        <v>295</v>
-      </c>
-      <c r="C81" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="D81" s="16"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
-      <c r="H81" s="3"/>
-    </row>
-    <row r="82" spans="1:8">
-      <c r="B82" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C82" s="19"/>
-      <c r="D82" s="26"/>
-    </row>
-    <row r="83" spans="1:8" ht="42">
-      <c r="B83" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C83" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="D83" s="16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="42">
-      <c r="B84" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C84" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="D84" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="42">
-      <c r="B85" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C85" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="D85" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-    </row>
-    <row r="86" spans="1:8" ht="42">
-      <c r="B86" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="C86" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="D86" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3"/>
-    </row>
-    <row r="87" spans="1:8" ht="56">
-      <c r="B87" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C87" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="D87" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
-    </row>
-    <row r="88" spans="1:8" ht="56">
-      <c r="B88" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C88" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="D88" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
-    </row>
-    <row r="89" spans="1:8" ht="42">
-      <c r="B89" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C89" s="23" t="s">
-        <v>262</v>
-      </c>
-      <c r="D89" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="B90" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="C90" s="19"/>
-      <c r="D90" s="26"/>
-    </row>
-    <row r="91" spans="1:8" ht="42">
-      <c r="B91" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C91" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="D91" s="16" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="42">
-      <c r="B92" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C92" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="D92" s="16" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="42">
-      <c r="B93" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C93" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="D93" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
-      <c r="H93" s="3"/>
-    </row>
-    <row r="94" spans="1:8" ht="42">
-      <c r="B94" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="C94" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="D94" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
-    </row>
-    <row r="95" spans="1:8" ht="42">
-      <c r="B95" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C95" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="D95" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="E95" s="3"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="30"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
-    </row>
-    <row r="96" spans="1:8" ht="42">
-      <c r="B96" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C96" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="D96" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="E96" s="3"/>
+      <c r="I95" s="3"/>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="C96" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D96" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="E96" s="20" t="s">
+        <v>261</v>
+      </c>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-    </row>
-    <row r="97" spans="1:8" ht="28">
-      <c r="B97" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C97" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="D97" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
-      <c r="H97" s="3"/>
-    </row>
-    <row r="98" spans="1:8">
-      <c r="B98" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="C98" s="19"/>
-      <c r="D98" s="26"/>
-    </row>
-    <row r="99" spans="1:8" ht="42">
-      <c r="B99" s="28" t="s">
+      <c r="I96" s="3"/>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="C97" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D97" s="29"/>
+      <c r="E97" s="30"/>
+    </row>
+    <row r="98" spans="1:9" s="2" customFormat="1">
+      <c r="A98" s="21" t="s">
+        <v>412</v>
+      </c>
+      <c r="B98" s="26" t="s">
+        <v>483</v>
+      </c>
+      <c r="C98" s="36" t="s">
+        <v>406</v>
+      </c>
+      <c r="D98" s="38"/>
+      <c r="E98" s="27"/>
+    </row>
+    <row r="99" spans="1:9" ht="42">
+      <c r="C99" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C99" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="D99" s="16" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="42">
-      <c r="B100" s="29" t="s">
+      <c r="D99" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="E99" s="20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="42">
+      <c r="C100" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C100" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="D100" s="16" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="42">
-      <c r="B101" s="29" t="s">
+      <c r="D100" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E100" s="20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="42">
+      <c r="C101" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C101" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="D101" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="E101" s="3"/>
+      <c r="D101" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="E101" s="20" t="s">
+        <v>195</v>
+      </c>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
-    </row>
-    <row r="102" spans="1:8" ht="42">
-      <c r="B102" s="29" t="s">
+      <c r="I101" s="3"/>
+    </row>
+    <row r="102" spans="1:9" ht="42">
+      <c r="C102" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="D102" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E102" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="C102" s="23" t="s">
-        <v>249</v>
-      </c>
-      <c r="D102" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
-    </row>
-    <row r="103" spans="1:8" ht="42">
-      <c r="B103" s="28" t="s">
+      <c r="I102" s="3"/>
+    </row>
+    <row r="103" spans="1:9" ht="56">
+      <c r="C103" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C103" s="23" t="s">
-        <v>256</v>
-      </c>
-      <c r="D103" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="E103" s="3"/>
+      <c r="D103" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="E103" s="20" t="s">
+        <v>223</v>
+      </c>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
-    </row>
-    <row r="104" spans="1:8" ht="42">
-      <c r="B104" s="28" t="s">
+      <c r="I103" s="3"/>
+    </row>
+    <row r="104" spans="1:9" ht="56">
+      <c r="C104" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C104" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="D104" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="E104" s="3"/>
+      <c r="D104" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="E104" s="20" t="s">
+        <v>224</v>
+      </c>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
-    </row>
-    <row r="105" spans="1:8" ht="28">
-      <c r="B105" s="28" t="s">
+      <c r="I104" s="3"/>
+    </row>
+    <row r="105" spans="1:9" ht="42">
+      <c r="C105" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C105" s="23" t="s">
-        <v>257</v>
-      </c>
-      <c r="D105" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="E105" s="3"/>
+      <c r="D105" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="E105" s="20" t="s">
+        <v>225</v>
+      </c>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
-    </row>
-    <row r="106" spans="1:8">
-      <c r="B106" s="27" t="s">
-        <v>301</v>
-      </c>
-      <c r="C106" s="19"/>
-      <c r="D106" s="26"/>
-      <c r="E106" s="3"/>
-      <c r="F106" s="3"/>
-      <c r="G106" s="3"/>
-      <c r="H106" s="3"/>
-    </row>
-    <row r="107" spans="1:8" ht="56">
-      <c r="B107" s="28" t="s">
-        <v>138</v>
-      </c>
+      <c r="I105" s="3"/>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="C106" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="D106" s="29"/>
+      <c r="E106" s="30"/>
+    </row>
+    <row r="107" spans="1:9" ht="42">
       <c r="C107" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="D107" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="E107" s="3"/>
-      <c r="F107" s="3"/>
-      <c r="G107" s="3"/>
-      <c r="H107" s="3"/>
-    </row>
-    <row r="108" spans="1:8">
-      <c r="A108" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="B108" s="48" t="s">
-        <v>296</v>
-      </c>
-      <c r="C108" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="D108" s="16"/>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3"/>
-      <c r="G108" s="3"/>
-      <c r="H108" s="3"/>
-    </row>
-    <row r="109" spans="1:8" ht="56">
-      <c r="B109" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="C109" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="D109" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="E109" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="D107" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="E107" s="20" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="42">
+      <c r="C108" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D108" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E108" s="20" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="42">
+      <c r="C109" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D109" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="E109" s="20" t="s">
+        <v>236</v>
+      </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
-    </row>
-    <row r="110" spans="1:8" ht="56">
-      <c r="B110" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C110" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="D110" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E110" s="3"/>
+      <c r="I109" s="3"/>
+    </row>
+    <row r="110" spans="1:9" ht="42">
+      <c r="C110" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="D110" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="E110" s="20" t="s">
+        <v>237</v>
+      </c>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
-    </row>
-    <row r="111" spans="1:8" ht="56">
-      <c r="B111" s="28" t="s">
-        <v>141</v>
-      </c>
+      <c r="I110" s="3"/>
+    </row>
+    <row r="111" spans="1:9" ht="42">
       <c r="C111" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="D111" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="E111" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="D111" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="E111" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
-    </row>
-    <row r="112" spans="1:8">
-      <c r="A112" s="15" t="s">
-        <v>297</v>
-      </c>
-      <c r="B112" s="48" t="s">
-        <v>297</v>
-      </c>
-      <c r="C112" s="38" t="s">
-        <v>362</v>
-      </c>
-      <c r="D112" s="39"/>
-      <c r="E112" s="3"/>
+      <c r="I111" s="3"/>
+    </row>
+    <row r="112" spans="1:9" ht="42">
+      <c r="C112" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D112" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E112" s="20" t="s">
+        <v>239</v>
+      </c>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
-    </row>
-    <row r="113" spans="1:8">
-      <c r="B113" s="27" t="s">
-        <v>354</v>
-      </c>
-      <c r="C113" s="19"/>
-      <c r="D113" s="26"/>
-      <c r="E113" s="3"/>
+      <c r="I112" s="3"/>
+    </row>
+    <row r="113" spans="1:9" ht="28">
+      <c r="C113" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D113" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="E113" s="20" t="s">
+        <v>243</v>
+      </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
-    </row>
-    <row r="114" spans="1:8" s="2" customFormat="1">
-      <c r="A114" s="41" t="s">
-        <v>291</v>
-      </c>
-      <c r="B114" s="46" t="s">
-        <v>291</v>
-      </c>
-      <c r="C114" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="D114" s="17"/>
-    </row>
-    <row r="115" spans="1:8">
-      <c r="A115" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="B115" s="48" t="s">
-        <v>298</v>
-      </c>
-      <c r="C115" s="24" t="s">
-        <v>356</v>
-      </c>
-      <c r="D115" s="10"/>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
-      <c r="G115" s="3"/>
-      <c r="H115" s="3"/>
-    </row>
-    <row r="116" spans="1:8">
-      <c r="A116" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="B116" s="48" t="s">
-        <v>299</v>
-      </c>
-      <c r="C116" s="24" t="s">
-        <v>357</v>
-      </c>
-      <c r="D116" s="10"/>
-      <c r="E116" s="3"/>
-      <c r="F116" s="3"/>
-      <c r="G116" s="3"/>
-      <c r="H116" s="3"/>
-    </row>
-    <row r="117" spans="1:8">
-      <c r="A117" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="B117" s="48" t="s">
-        <v>300</v>
-      </c>
-      <c r="C117" s="24" t="s">
-        <v>358</v>
-      </c>
-      <c r="D117" s="10"/>
-      <c r="E117" s="3"/>
+      <c r="I113" s="3"/>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="C114" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="D114" s="29"/>
+      <c r="E114" s="30"/>
+    </row>
+    <row r="115" spans="1:9" ht="42">
+      <c r="C115" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D115" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="E115" s="20" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="42">
+      <c r="C116" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D116" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="E116" s="20" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="42">
+      <c r="C117" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D117" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="E117" s="20" t="s">
+        <v>250</v>
+      </c>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
-    </row>
-    <row r="118" spans="1:8">
-      <c r="B118" s="27" t="s">
-        <v>307</v>
-      </c>
-      <c r="C118" s="19"/>
-      <c r="D118" s="26"/>
-    </row>
-    <row r="119" spans="1:8">
-      <c r="A119" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="B119" s="47" t="s">
-        <v>308</v>
-      </c>
-      <c r="C119" s="24" t="s">
-        <v>366</v>
-      </c>
-      <c r="D119" s="10"/>
-      <c r="E119" s="3"/>
+      <c r="I117" s="3"/>
+    </row>
+    <row r="118" spans="1:9" ht="42">
+      <c r="C118" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="D118" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E118" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="3"/>
+      <c r="I118" s="3"/>
+    </row>
+    <row r="119" spans="1:9" ht="42">
+      <c r="C119" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D119" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="E119" s="20" t="s">
+        <v>252</v>
+      </c>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
-    </row>
-    <row r="120" spans="1:8">
-      <c r="A120" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="B120" s="47" t="s">
-        <v>311</v>
-      </c>
-      <c r="C120" s="24" t="s">
-        <v>365</v>
-      </c>
-      <c r="D120" s="10"/>
-      <c r="E120" s="3"/>
+      <c r="I119" s="3"/>
+    </row>
+    <row r="120" spans="1:9" ht="42">
+      <c r="C120" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D120" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="E120" s="20" t="s">
+        <v>253</v>
+      </c>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
-    </row>
-    <row r="121" spans="1:8">
-      <c r="A121" s="50"/>
-      <c r="C121" s="51"/>
-      <c r="D121" s="31"/>
-      <c r="E121" s="3"/>
+      <c r="I120" s="3"/>
+    </row>
+    <row r="121" spans="1:9" ht="28">
+      <c r="C121" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D121" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="E121" s="20" t="s">
+        <v>256</v>
+      </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
-    </row>
-    <row r="122" spans="1:8">
-      <c r="A122" s="50" t="s">
+      <c r="I121" s="3"/>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="B122" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="C122" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="D122" s="29"/>
+      <c r="E122" s="30"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+      <c r="H122" s="3"/>
+      <c r="I122" s="3"/>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="B123" s="22" t="s">
+        <v>440</v>
+      </c>
+      <c r="C123" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="D123" s="22"/>
+      <c r="E123" s="20"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="3"/>
+      <c r="I123" s="3"/>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="B124" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="C124" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="D124" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E124" s="20"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
+      <c r="H124" s="3"/>
+      <c r="I124" s="3"/>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B125" s="22" t="s">
+        <v>442</v>
+      </c>
+      <c r="C125" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="D125" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E125" s="20"/>
+      <c r="F125" s="3"/>
+      <c r="G125" s="3"/>
+      <c r="H125" s="3"/>
+      <c r="I125" s="3"/>
+    </row>
+    <row r="126" spans="1:9" ht="56">
+      <c r="B126" s="40" t="s">
+        <v>443</v>
+      </c>
+      <c r="C126" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D126" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E126" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
+      <c r="H126" s="3"/>
+      <c r="I126" s="3"/>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B127" s="40" t="s">
+        <v>444</v>
+      </c>
+      <c r="C127" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="D127" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="E127" s="20"/>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="3"/>
+      <c r="I127" s="3"/>
+    </row>
+    <row r="128" spans="1:9" ht="56">
+      <c r="A128" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B128" s="40" t="s">
+        <v>445</v>
+      </c>
+      <c r="C128" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D128" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="E128" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="F128" s="3"/>
+      <c r="G128" s="3"/>
+      <c r="H128" s="3"/>
+      <c r="I128" s="3"/>
+    </row>
+    <row r="129" spans="1:9" ht="56">
+      <c r="A129" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B129" s="40" t="s">
+        <v>446</v>
+      </c>
+      <c r="C129" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D129" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="E129" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="3"/>
+      <c r="I129" s="3"/>
+    </row>
+    <row r="130" spans="1:9" ht="56">
+      <c r="A130" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="B130" s="40" t="s">
+        <v>447</v>
+      </c>
+      <c r="C130" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D130" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="E130" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="F130" s="3"/>
+      <c r="G130" s="3"/>
+      <c r="H130" s="3"/>
+      <c r="I130" s="3"/>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B131" s="40" t="s">
+        <v>448</v>
+      </c>
+      <c r="C131" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="D131" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="E131" s="20"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
+      <c r="H131" s="3"/>
+      <c r="I131" s="3"/>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="C132" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="D132" s="29"/>
+      <c r="E132" s="30"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
+      <c r="H132" s="3"/>
+      <c r="I132" s="3"/>
+    </row>
+    <row r="133" spans="1:9" s="2" customFormat="1">
+      <c r="A133" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="B133" s="41" t="s">
+        <v>425</v>
+      </c>
+      <c r="C133" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="D133" s="37" t="s">
+        <v>338</v>
+      </c>
+      <c r="E133" s="27"/>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B134" s="40" t="s">
+        <v>449</v>
+      </c>
+      <c r="C134" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="D134" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="E134" s="10"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
+      <c r="H134" s="3"/>
+      <c r="I134" s="3"/>
+    </row>
+    <row r="135" spans="1:9">
+      <c r="A135" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B135" s="40" t="s">
+        <v>450</v>
+      </c>
+      <c r="C135" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="D135" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="E135" s="10"/>
+      <c r="F135" s="3"/>
+      <c r="G135" s="3"/>
+      <c r="H135" s="3"/>
+      <c r="I135" s="3"/>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="A136" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B136" s="40" t="s">
+        <v>451</v>
+      </c>
+      <c r="C136" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="D136" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="E136" s="10"/>
+      <c r="F136" s="3"/>
+      <c r="G136" s="3"/>
+      <c r="H136" s="3"/>
+      <c r="I136" s="3"/>
+    </row>
+    <row r="137" spans="1:9">
+      <c r="C137" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="D137" s="29"/>
+      <c r="E137" s="30"/>
+    </row>
+    <row r="138" spans="1:9">
+      <c r="A138" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B138" s="40" t="s">
+        <v>465</v>
+      </c>
+      <c r="C138" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="D138" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="E138" s="10"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
+      <c r="H138" s="3"/>
+      <c r="I138" s="3"/>
+    </row>
+    <row r="139" spans="1:9">
+      <c r="A139" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="B139" s="40" t="s">
+        <v>466</v>
+      </c>
+      <c r="C139" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="D139" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="E139" s="10"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3"/>
+      <c r="H139" s="3"/>
+      <c r="I139" s="3"/>
+    </row>
+    <row r="140" spans="1:9">
+      <c r="C140" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="D140" s="29"/>
+      <c r="E140" s="30"/>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="A141" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="B141" s="24" t="s">
+        <v>478</v>
+      </c>
+      <c r="C141" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="B122" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="C122" s="51" t="s">
-        <v>376</v>
-      </c>
-      <c r="D122" s="31"/>
-    </row>
-    <row r="123" spans="1:8">
-      <c r="A123" s="50" t="s">
-        <v>318</v>
-      </c>
-      <c r="B123" s="40" t="s">
-        <v>330</v>
-      </c>
-      <c r="C123" s="51" t="s">
-        <v>376</v>
-      </c>
-      <c r="D123" s="31"/>
-    </row>
-    <row r="124" spans="1:8">
-      <c r="A124" s="50" t="s">
-        <v>319</v>
-      </c>
-      <c r="B124" s="40" t="s">
-        <v>373</v>
-      </c>
-      <c r="C124" s="51" t="s">
-        <v>376</v>
-      </c>
-      <c r="D124" s="31"/>
-    </row>
-    <row r="125" spans="1:8">
-      <c r="A125" s="50"/>
-      <c r="C125" s="51"/>
-      <c r="D125" s="31"/>
-    </row>
-    <row r="126" spans="1:8">
-      <c r="A126" s="50"/>
-      <c r="B126" s="31" t="s">
-        <v>377</v>
-      </c>
-      <c r="C126" s="51"/>
-      <c r="D126" s="31"/>
-    </row>
-    <row r="127" spans="1:8">
-      <c r="A127" s="50"/>
-      <c r="C127" s="51"/>
-      <c r="D127" s="31"/>
-    </row>
-    <row r="128" spans="1:8">
-      <c r="A128" s="50"/>
-      <c r="C128" s="51"/>
-      <c r="D128" s="31"/>
-    </row>
-    <row r="129" spans="1:4">
-      <c r="A129" s="50"/>
-      <c r="C129" s="51"/>
-      <c r="D129" s="31"/>
-    </row>
-    <row r="130" spans="1:4">
-      <c r="A130" s="50"/>
-      <c r="C130" s="51"/>
-      <c r="D130" s="31"/>
-    </row>
-    <row r="131" spans="1:4">
-      <c r="A131" s="50"/>
-      <c r="C131" s="51"/>
-      <c r="D131" s="31"/>
-    </row>
-    <row r="132" spans="1:4">
-      <c r="A132" s="50"/>
-      <c r="C132" s="51"/>
-      <c r="D132" s="31"/>
-    </row>
-    <row r="133" spans="1:4">
-      <c r="A133" s="50"/>
-      <c r="C133" s="51"/>
-      <c r="D133" s="31"/>
-    </row>
-    <row r="134" spans="1:4">
-      <c r="A134" s="50"/>
-      <c r="C134" s="51"/>
-      <c r="D134" s="31"/>
-    </row>
-    <row r="135" spans="1:4">
-      <c r="A135" s="50"/>
-      <c r="C135" s="51"/>
-      <c r="D135" s="31"/>
+      <c r="D141" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="E141" s="18"/>
+    </row>
+    <row r="142" spans="1:9">
+      <c r="A142" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="B142" s="24" t="s">
+        <v>479</v>
+      </c>
+      <c r="C142" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="D142" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="E142" s="18"/>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="A143" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="B143" s="24" t="s">
+        <v>480</v>
+      </c>
+      <c r="C143" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="D143" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="E143" s="18"/>
+    </row>
+    <row r="144" spans="1:9">
+      <c r="B144" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="C144" s="28" t="s">
+        <v>415</v>
+      </c>
+      <c r="D144" s="29"/>
+      <c r="E144" s="30"/>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="B145" s="22" t="s">
+        <v>481</v>
+      </c>
+      <c r="C145" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="D145" s="19"/>
+      <c r="E145" s="20"/>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B146" s="22" t="s">
+        <v>482</v>
+      </c>
+      <c r="C146" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="D146" s="19"/>
+      <c r="E146" s="20"/>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B147" s="22" t="s">
+        <v>484</v>
+      </c>
+      <c r="C147" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="D147" s="19"/>
+      <c r="E147" s="20"/>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="B148" s="22" t="s">
+        <v>485</v>
+      </c>
+      <c r="C148" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="D148" s="19"/>
+      <c r="E148" s="20"/>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="B149" s="22" t="s">
+        <v>487</v>
+      </c>
+      <c r="C149" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="D149" s="19"/>
+      <c r="E149" s="20"/>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" s="23"/>
+      <c r="B150" s="24"/>
+      <c r="D150" s="24"/>
+      <c r="E150" s="18"/>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" s="23"/>
+      <c r="B151" s="24"/>
+      <c r="D151" s="24"/>
+      <c r="E151" s="18"/>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" s="23"/>
+      <c r="B152" s="24"/>
+      <c r="D152" s="24"/>
+      <c r="E152" s="18"/>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="23"/>
+      <c r="B153" s="24"/>
+      <c r="D153" s="24"/>
+      <c r="E153" s="18"/>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="23"/>
+      <c r="B154" s="24"/>
+      <c r="D154" s="24"/>
+      <c r="E154" s="18"/>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="23"/>
+      <c r="B155" s="24"/>
+      <c r="D155" s="24"/>
+      <c r="E155" s="18"/>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="23"/>
+      <c r="B156" s="24"/>
+      <c r="D156" s="24"/>
+      <c r="E156" s="18"/>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" s="23"/>
+      <c r="B157" s="24"/>
+      <c r="D157" s="24"/>
+      <c r="E157" s="18"/>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" s="23"/>
+      <c r="B158" s="24"/>
+      <c r="D158" s="24"/>
+      <c r="E158" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated SSPs for Hawaii.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/ProsecutionCaseQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/ProsecutionCaseQueryResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27020" yWindow="1840" windowWidth="27300" windowHeight="13740"/>
+    <workbookView xWindow="6000" yWindow="2900" windowWidth="27300" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="531">
   <si>
     <t>ATN [Arrest Tracking Number]</t>
   </si>
@@ -655,9 +655,6 @@
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCourt/j:CourtCategoryCode</t>
   </si>
   <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge/pcq-res-ext:ChargeDomesticViolenceIndicator</t>
-  </si>
-  <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeApplicabilityText</t>
   </si>
   <si>
@@ -670,12 +667,6 @@
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeSeverityLevel/j:SeverityLevelDescriptionText</t>
   </si>
   <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeSeverityText</t>
-  </si>
-  <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationJurisdiction/nc:JurisdictionText</t>
   </si>
   <si>
@@ -700,18 +691,6 @@
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:JudicialOfficial[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseInitiatingParty/nc:EntityPerson/@structures:ref]/j:JudicialOfficialCategoryText</t>
   </si>
   <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation[nc:Person/@structures:ref=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:Location/@structures:ref]/nc:Address/nc:LocationStreet/nc:StreetFullText</t>
-  </si>
-  <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation[nc:Person/@structures:ref=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:Location/@structures:ref]/nc:Address/nc:LocationCityName</t>
-  </si>
-  <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation[nc:Person/@structures:ref=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:Location/@structures:ref]/nc:Address/nc:LocationStateUSPostalServiceCode</t>
-  </si>
-  <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation[nc:Person/@structures:ref=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:Location/@structures:ref]/nc:Address/nc:LocationPostalCode</t>
-  </si>
-  <si>
     <t>Case  Judge</t>
   </si>
   <si>
@@ -803,9 +782,6 @@
   </si>
   <si>
     <t>Position</t>
-  </si>
-  <si>
-    <t>ADD TO MODEL</t>
   </si>
   <si>
     <t>Honolulu Police Department</t>
@@ -840,12 +816,6 @@
     <t>Prosecution Case Query Result Element</t>
   </si>
   <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest/j:ArrestAgency/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest/j:ArrestAgencyRecordIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest/j:ArrestAgencyRecordIdentification/nc:IdentificationJurisdiction/nc:JurisdictionText</t>
   </si>
   <si>
@@ -972,12 +942,6 @@
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonName/nc:PersonNameSuffixText</t>
   </si>
   <si>
-    <t>Use nc:VehicleAugmentation</t>
-  </si>
-  <si>
-    <t>Use j:driverLicenseAugmentation</t>
-  </si>
-  <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/j:PersonAugmentation/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -1089,9 +1053,6 @@
     <t>Charge Category Description Text</t>
   </si>
   <si>
-    <t>Vehicle CMV Indicator</t>
-  </si>
-  <si>
     <t>Charge Category</t>
   </si>
   <si>
@@ -1104,9 +1065,6 @@
     <t>Domestic Violence</t>
   </si>
   <si>
-    <t>MOVE FROM PERSON</t>
-  </si>
-  <si>
     <t>Confidential</t>
   </si>
   <si>
@@ -1458,12 +1416,6 @@
     <t>71</t>
   </si>
   <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
     <t>74</t>
   </si>
   <si>
@@ -1498,13 +1450,179 @@
   </si>
   <si>
     <t>Suffix</t>
+  </si>
+  <si>
+    <t>RED - In XML Instance
+Black - Waiting for more info</t>
+  </si>
+  <si>
+    <t>72-Ext</t>
+  </si>
+  <si>
+    <t>73-Ext</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest[@structures:id=..//j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:ArrestAgencyRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest[@structures:id=../j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:ArrestAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest[@structures:id=../j:ActivityCaseAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Incident[@structures:id=../j:ActivityCaseAssociation/nc:Activity/@structures:ref]/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/nc:CaseFiling/nc:DocumentFiledDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseDomesticViolenceIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/pcq-res-ext:CaseConfidentialIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/nc:ActivityDescriptionText</t>
+  </si>
+  <si>
+    <t>pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/nc:CaseTitleText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge[@structures:id=../../../j:OffenseChargeAssociation/j:Charge/@structures:ref]/j:ChargeCountQuantity</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge[@structures:id=../../../j:OffenseChargeAssociation/j:Charge/@structures:ref]/j:ChargeDescriptionText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge[@structures:id=../../../j:OffenseChargeAssociation/j:Charge/@structures:ref]/j:ChargeSeverityText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge[@structures:id=../../../j:OffenseChargeAssociation/j:Charge/@structures:ref]/j:ChargeQualifierText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge[@structures:id=../../../j:OffenseChargeAssociation/j:Charge/@structures:ref]/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Person (Defendant)</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonName/nc:PersonNamePrefixText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/pcq-res-ext:PersonJuvenileIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonHeightMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonHeightMeasure/nc:LengthUnitCode</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonWeightMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonHeightMeasure/nc:WeightUnitCode</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonEyeColorText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonHairColorText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/nc:PersonSSNIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/pcq-res-ext:IdentifiedPersonTrackingIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Identity[@structures:id=../nc:PersonIdentityAssociation/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Identity[@structures:id=../nc:PersonIdentityAssociation/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Identity[@structures:id=../nc:PersonIdentityAssociation/nc:Identity/@structures:ref]/nc:IdentityPersonRepresentation/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseDefendantParty/pcq-res-ext:PartyRoleText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseDefendantParty/pcq-res-ext:PartyCategoryText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseDefendantParty/pcq-res-ext:PartyConfidentialIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityOrganization/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:LocationCategoryText</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/pcq-res-ext:DefaultLocationIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/pcq-res-ext:PreferredLocationIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:AddressSecondaryUnitText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:LocationStateUSPostalServiceCode</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Location[@structures:id=../nc:PersonResidenceAssociation/nc:Location/@structures:ref]/nc:Address/nc:LocationCountryName</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:ContactInformation[@structures:id=../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:ContactEmailID</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:ContactInformation[@structures:id=../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:ContactTelephoneNumber[nc:TelephoneNumberCategoryText='Home']/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:ContactInformation[@structures:id=../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:ContactTelephoneNumber[nc:TelephoneNumberCategoryText='Business']/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:ContactInformation[@structures:id=../nc:ContactInformationAssociation/nc:ContactInformation/@structures:ref]/nc:ContactTelephoneNumber[nc:TelephoneNumberCategoryText='Cell']/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Booking[@structures:id=../j:ActivityCaseAssociation/nc:Activity/@structures:ref]/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Booking[@structures:id=../j:ActivityCaseAssociation/nc:Activity/@structures:ref]/j:BookingAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Person[@structures:id=../nc:Case/j:CaseAugmentation/j:CaseDefendantParty/nc:EntityPerson/@structures:ref]/j:PersonAugmentation/j:DriverLicense/pcq-res-ext:DriverLicenseCDLIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Vehicle[@structures:id=../nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/nc:VehicleCMVIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Vehicle[@structures:id=../nc:PersonConveyanceAssociation/nc:Conveyance/@structures:ref]/pcq-res-ext:VehicleHazmatIndicator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1685,6 +1803,26 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1781,7 +1919,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="261">
+  <cellStyleXfs count="337">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -2043,8 +2181,84 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2103,9 +2317,6 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2124,16 +2335,10 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2169,8 +2374,26 @@
     <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="261">
+  <cellStyles count="337">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2315,6 +2538,44 @@
     <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2426,6 +2687,44 @@
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="90"/>
@@ -2732,43 +3031,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138:B139"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D142" sqref="D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" style="15" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="22" customWidth="1"/>
+    <col min="2" max="2" width="21" style="21" customWidth="1"/>
     <col min="3" max="3" width="37.1640625" style="18" customWidth="1"/>
     <col min="4" max="4" width="23" style="17" customWidth="1"/>
-    <col min="5" max="5" width="77.5" style="13" customWidth="1"/>
+    <col min="5" max="5" width="83.83203125" style="43" customWidth="1"/>
     <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" ht="49" customHeight="1">
+      <c r="A1" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>346</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>271</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="B1" s="40" t="s">
+        <v>476</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="28" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15">
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="35"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:5">
       <c r="C3" s="18" t="s">
@@ -2777,7 +3076,7 @@
       <c r="D3" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="18" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2788,7 +3087,7 @@
       <c r="D4" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>200</v>
       </c>
     </row>
@@ -2799,7 +3098,7 @@
       <c r="D5" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>201</v>
       </c>
     </row>
@@ -2810,18 +3109,18 @@
       <c r="D6" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="18" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28">
+    <row r="7" spans="1:5">
       <c r="C7" s="18" t="s">
         <v>135</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="18" t="s">
         <v>203</v>
       </c>
     </row>
@@ -2829,112 +3128,114 @@
       <c r="A8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>460</v>
-      </c>
-      <c r="C8" s="28" t="s">
+      <c r="B8" s="37" t="s">
+        <v>446</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="15" t="s">
-        <v>391</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>461</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>406</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="20"/>
+        <v>377</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>447</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="15" t="s">
-        <v>409</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>469</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>406</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="20"/>
+        <v>395</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>455</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="15" t="s">
-        <v>393</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>463</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>406</v>
-      </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="20"/>
-    </row>
-    <row r="12" spans="1:5" ht="28">
+        <v>379</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>449</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="18"/>
+    </row>
+    <row r="12" spans="1:5" ht="42">
       <c r="A12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="40" t="s">
-        <v>464</v>
+      <c r="B12" s="37" t="s">
+        <v>450</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>254</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="42">
       <c r="A13" s="15" t="s">
-        <v>392</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>462</v>
+        <v>378</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>448</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>268</v>
-      </c>
-      <c r="E13" s="20"/>
-    </row>
-    <row r="14" spans="1:5" ht="28">
+        <v>260</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="42">
       <c r="A14" s="15" t="s">
-        <v>394</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>470</v>
+        <v>380</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>456</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>263</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="42">
+        <v>255</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="28">
       <c r="C15" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>274</v>
+        <v>254</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="28">
@@ -2942,10 +3243,10 @@
         <v>35</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>264</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>275</v>
+        <v>256</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="42">
@@ -2953,10 +3254,10 @@
         <v>36</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>276</v>
+        <v>254</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="98">
@@ -2964,1051 +3265,1107 @@
         <v>37</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>265</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>277</v>
+        <v>257</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A19" s="21"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="25" t="s">
+      <c r="A19" s="20"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="37" t="s">
-        <v>266</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>278</v>
+      <c r="D19" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="C20" s="28" t="s">
-        <v>395</v>
-      </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1">
-      <c r="A21" s="21" t="s">
-        <v>396</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>471</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>397</v>
+      <c r="C20" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="42"/>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A21" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>457</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>383</v>
       </c>
       <c r="D21" s="19"/>
-      <c r="E21" s="27"/>
+      <c r="E21" s="18" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D22" s="29"/>
-      <c r="E22" s="30"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="42"/>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1">
-      <c r="A23" s="39" t="s">
-        <v>304</v>
-      </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="25" t="s">
-        <v>328</v>
+      <c r="A23" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="24" t="s">
+        <v>316</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>267</v>
+        <v>315</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A24" s="21"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="36" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="D24" s="37" t="s">
-        <v>258</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>257</v>
+      <c r="D24" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A25" s="21"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="25" t="s">
+      <c r="A25" s="20"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="37" t="s">
-        <v>270</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>269</v>
+      <c r="D25" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="42"/>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1">
-      <c r="A27" s="21"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="25" t="s">
+      <c r="A27" s="20"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="24" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A28" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="B28" s="41">
+      <c r="A28" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B28" s="38">
         <v>4</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="24" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A29" s="21"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="25" t="s">
+      <c r="A29" s="20"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="24" t="s">
         <v>134</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="24" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A30" s="21"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="36" t="s">
-        <v>311</v>
-      </c>
-      <c r="D30" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="E30" s="27" t="s">
+      <c r="A30" s="20"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="E30" s="24" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="E31" s="24"/>
+    </row>
+    <row r="32" spans="1:5" s="2" customFormat="1">
+      <c r="A32" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="B32" s="38">
+        <v>5</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="24"/>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A33" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>403</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A34" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B34" s="38">
+        <v>1</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A35" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="B35" s="38">
+        <v>2</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A36" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="B36" s="38">
+        <v>3</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A37" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="B37" s="38">
+        <v>6</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="B38" s="38">
+        <v>7</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="E38" s="24" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1">
+      <c r="A39" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="B39" s="38">
+        <v>9</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="2" customFormat="1">
+      <c r="A40" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="B40" s="38">
+        <v>8</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="D40" s="34" t="s">
         <v>308</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="36" t="s">
-        <v>312</v>
-      </c>
-      <c r="D31" s="38" t="s">
-        <v>309</v>
-      </c>
-      <c r="E31" s="27"/>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1">
-      <c r="A32" s="21" t="s">
-        <v>407</v>
-      </c>
-      <c r="B32" s="41">
+      <c r="E40" s="24" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="C41" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="36" t="s">
-        <v>406</v>
-      </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="27"/>
-    </row>
-    <row r="33" spans="1:5" s="2" customFormat="1">
-      <c r="A33" s="21" t="s">
-        <v>366</v>
-      </c>
-      <c r="B33" s="41" t="s">
-        <v>417</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>365</v>
-      </c>
-      <c r="E33" s="27"/>
-    </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A34" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="B34" s="41">
-        <v>1</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="E34" s="27" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A35" s="21" t="s">
-        <v>280</v>
-      </c>
-      <c r="B35" s="41">
-        <v>2</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="E35" s="27" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A36" s="21" t="s">
-        <v>358</v>
-      </c>
-      <c r="B36" s="26">
-        <v>3</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A37" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="B37" s="26">
-        <v>6</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="E37" s="27" t="s">
+      <c r="D41" s="27"/>
+      <c r="E41" s="42"/>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="A42" s="20"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="24" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="2" customFormat="1">
-      <c r="A38" s="21" t="s">
-        <v>361</v>
-      </c>
-      <c r="B38" s="26">
-        <v>7</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="D38" s="37" t="s">
-        <v>334</v>
-      </c>
-      <c r="E38" s="39" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1">
-      <c r="A39" s="21" t="s">
-        <v>282</v>
-      </c>
-      <c r="B39" s="41">
-        <v>9</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>364</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>363</v>
-      </c>
-      <c r="E39" s="39"/>
-    </row>
-    <row r="40" spans="1:5" s="2" customFormat="1">
-      <c r="A40" s="21" t="s">
-        <v>362</v>
-      </c>
-      <c r="B40" s="41">
-        <v>8</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>313</v>
-      </c>
-      <c r="D40" s="37" t="s">
-        <v>320</v>
-      </c>
-      <c r="E40" s="27"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="C41" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="30"/>
-    </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A42" s="21"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>212</v>
-      </c>
-    </row>
     <row r="43" spans="1:5" s="2" customFormat="1">
-      <c r="A43" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="B43" s="41" t="s">
-        <v>468</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>406</v>
-      </c>
-      <c r="D43" s="26"/>
-      <c r="E43" s="27"/>
+      <c r="A43" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>454</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="D43" s="25"/>
+      <c r="E43" s="24"/>
     </row>
     <row r="44" spans="1:5" s="2" customFormat="1">
-      <c r="A44" s="21" t="s">
-        <v>410</v>
-      </c>
-      <c r="B44" s="41" t="s">
-        <v>473</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>406</v>
-      </c>
-      <c r="D44" s="26"/>
-      <c r="E44" s="27"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="A44" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="D44" s="25"/>
+      <c r="E44" s="24"/>
+    </row>
+    <row r="45" spans="1:5" ht="42">
       <c r="A45" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>472</v>
+        <v>293</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>458</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>352</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>350</v>
+        <v>340</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="E45" s="43" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="15" t="s">
-        <v>398</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>474</v>
+        <v>384</v>
+      </c>
+      <c r="B46" s="37" t="s">
+        <v>460</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>399</v>
-      </c>
-      <c r="D46" s="22"/>
+        <v>385</v>
+      </c>
+      <c r="D46" s="21"/>
+      <c r="E46" s="43" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="47" spans="1:5">
       <c r="C47" s="15"/>
-      <c r="D47" s="22"/>
+      <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:5">
       <c r="C48" s="18" t="s">
-        <v>354</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+        <v>342</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="42">
       <c r="A49" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B49" s="40" t="s">
-        <v>477</v>
+      <c r="B49" s="37" t="s">
+        <v>463</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>357</v>
+        <v>341</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="E49" s="43" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="2" customFormat="1" ht="28">
-      <c r="A50" s="21"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="25" t="s">
+      <c r="A50" s="20"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="E50" s="27" t="s">
+      <c r="E50" s="24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A51" s="20"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="E51" s="24" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="2" customFormat="1" ht="28">
-      <c r="A51" s="21"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="E51" s="27" t="s">
+    <row r="52" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A52" s="20"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="E52" s="24" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="2" customFormat="1" ht="42">
-      <c r="A52" s="21"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="E52" s="27" t="s">
+    <row r="53" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A53" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="B53" s="38" t="s">
+        <v>462</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="E53" s="43" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A54" s="20" t="s">
+        <v>388</v>
+      </c>
+      <c r="B54" s="38" t="s">
+        <v>461</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>389</v>
+      </c>
+      <c r="D54" s="34"/>
+      <c r="E54" s="43" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="2" customFormat="1">
+      <c r="A55" s="20"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="E55" s="24"/>
+    </row>
+    <row r="56" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A56" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="B56" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="C56" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E56" s="43" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A57" s="20"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="E57" s="24" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="2" customFormat="1" ht="28">
-      <c r="A53" s="21" t="s">
-        <v>401</v>
-      </c>
-      <c r="B53" s="41" t="s">
-        <v>476</v>
-      </c>
-      <c r="C53" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="E53" s="27" t="s">
+    <row r="58" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A58" s="20"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="E58" s="24" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="2" customFormat="1">
-      <c r="A54" s="21" t="s">
-        <v>402</v>
-      </c>
-      <c r="B54" s="26" t="s">
-        <v>475</v>
-      </c>
-      <c r="C54" s="25" t="s">
-        <v>403</v>
-      </c>
-      <c r="D54" s="37"/>
-      <c r="E54" s="27"/>
-    </row>
-    <row r="55" spans="1:10" s="2" customFormat="1">
-      <c r="A55" s="21"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="E55" s="27"/>
-    </row>
-    <row r="56" spans="1:10" s="2" customFormat="1" ht="42">
-      <c r="A56" s="21" t="s">
-        <v>400</v>
-      </c>
-      <c r="B56" s="41" t="s">
-        <v>321</v>
-      </c>
-      <c r="C56" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="37" t="s">
-        <v>155</v>
-      </c>
-      <c r="E56" s="27" t="s">
+    <row r="59" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A59" s="20"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E59" s="24" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="2" customFormat="1" ht="42">
-      <c r="A57" s="21"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="D57" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="E57" s="27" t="s">
+    <row r="60" spans="1:10" s="2" customFormat="1" ht="56">
+      <c r="A60" s="20"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="E60" s="24" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="2" customFormat="1" ht="42">
-      <c r="A58" s="21"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D58" s="37" t="s">
-        <v>167</v>
-      </c>
-      <c r="E58" s="27" t="s">
+    <row r="61" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A61" s="20"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="E61" s="24" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" s="2" customFormat="1" ht="28">
-      <c r="A59" s="21"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D59" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="E59" s="27" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" s="2" customFormat="1" ht="56">
-      <c r="A60" s="21"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D60" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="E60" s="27" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" ht="42">
-      <c r="A61" s="21"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D61" s="37" t="s">
-        <v>171</v>
-      </c>
-      <c r="E61" s="27" t="s">
-        <v>222</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="2" customFormat="1" ht="38" customHeight="1">
-      <c r="A62" s="21"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="25" t="s">
+      <c r="A62" s="20"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="D62" s="26" t="s">
-        <v>258</v>
-      </c>
-      <c r="E62" s="27" t="s">
-        <v>257</v>
+      <c r="D62" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="63" spans="1:10">
-      <c r="C63" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="29"/>
-      <c r="E63" s="30"/>
-    </row>
-    <row r="64" spans="1:10">
+      <c r="C63" s="26" t="s">
+        <v>493</v>
+      </c>
+      <c r="D63" s="27"/>
+      <c r="E63" s="42"/>
+    </row>
+    <row r="64" spans="1:10" ht="42">
       <c r="A64" s="15" t="s">
-        <v>372</v>
-      </c>
-      <c r="B64" s="40" t="s">
+        <v>358</v>
+      </c>
+      <c r="B64" s="37" t="s">
+        <v>406</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="D64" s="21"/>
+      <c r="E64" s="24" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A65" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B65" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>359</v>
+      </c>
+      <c r="D65" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A66" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B66" s="38" t="s">
+        <v>408</v>
+      </c>
+      <c r="C66" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="E66" s="24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A67" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="B67" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="D67" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="E67" s="24" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A68" s="20" t="s">
+        <v>475</v>
+      </c>
+      <c r="B68" s="38" t="s">
+        <v>410</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>361</v>
+      </c>
+      <c r="D68" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="E68" s="24" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A69" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="B69" s="38" t="s">
+        <v>414</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>365</v>
+      </c>
+      <c r="D69" s="34"/>
+      <c r="E69" s="24" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A70" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B70" s="38" t="s">
+        <v>415</v>
+      </c>
+      <c r="C70" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E70" s="24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A71" s="20"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D71" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="E71" s="24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A72" s="20"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D72" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="E72" s="24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="2" customFormat="1">
+      <c r="A73" s="20"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="D73" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="E73" s="24"/>
+    </row>
+    <row r="74" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A74" s="20" t="s">
+        <v>472</v>
+      </c>
+      <c r="B74" s="38" t="s">
+        <v>424</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D74" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="E74" s="24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="2" customFormat="1" ht="56">
+      <c r="A75" s="20"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D75" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="E75" s="24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A76" s="20" t="s">
+        <v>473</v>
+      </c>
+      <c r="B76" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D76" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="E76" s="24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="2" customFormat="1" ht="56">
+      <c r="A77" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="B77" s="38" t="s">
+        <v>422</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D77" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="E77" s="24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A78" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B78" s="38" t="s">
+        <v>413</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="D78" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A79" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B79" s="38" t="s">
+        <v>416</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="D79" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="E79" s="24" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="A80" s="20"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="D80" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A81" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="B81" s="38" t="s">
+        <v>417</v>
+      </c>
+      <c r="C81" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="D81" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="E81" s="24" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="42">
+      <c r="C82" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="E82" s="24" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A83" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="B83" s="38" t="s">
+        <v>418</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="D83" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="E83" s="24" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A84" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B84" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="C84" s="20" t="s">
         <v>420</v>
       </c>
-      <c r="C64" s="18" t="s">
-        <v>371</v>
-      </c>
-      <c r="D64" s="22"/>
-      <c r="E64" s="20"/>
-    </row>
-    <row r="65" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A65" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B65" s="41" t="s">
-        <v>421</v>
-      </c>
-      <c r="C65" s="25" t="s">
-        <v>373</v>
-      </c>
-      <c r="D65" s="37" t="s">
-        <v>177</v>
-      </c>
-      <c r="E65" s="27" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A66" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" s="41" t="s">
-        <v>422</v>
-      </c>
-      <c r="C66" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D66" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="E66" s="27" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A67" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="B67" s="41" t="s">
+      <c r="D84" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="E84" s="24" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A85" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="B85" s="38" t="s">
         <v>423</v>
       </c>
-      <c r="C67" s="25" t="s">
+      <c r="C85" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="D85" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="E85" s="24" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="42">
+      <c r="A86" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B86" s="37" t="s">
+        <v>453</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="E86" s="24" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="B87" s="37" t="s">
+        <v>442</v>
+      </c>
+      <c r="C87" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="D87" s="27"/>
+      <c r="E87" s="42"/>
+    </row>
+    <row r="88" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A88" s="20" t="s">
+        <v>439</v>
+      </c>
+      <c r="B88" s="38" t="s">
+        <v>443</v>
+      </c>
+      <c r="C88" s="24" t="s">
         <v>374</v>
       </c>
-      <c r="D67" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="E67" s="27" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A68" s="21" t="s">
-        <v>491</v>
-      </c>
-      <c r="B68" s="41" t="s">
-        <v>424</v>
-      </c>
-      <c r="C68" s="25" t="s">
+      <c r="D88" s="34"/>
+      <c r="E88" s="24" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A89" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B89" s="38" t="s">
+        <v>444</v>
+      </c>
+      <c r="C89" s="24" t="s">
         <v>375</v>
       </c>
-      <c r="D68" s="37" t="s">
-        <v>314</v>
-      </c>
-      <c r="E68" s="27" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="2" customFormat="1">
-      <c r="A69" s="21" t="s">
-        <v>378</v>
-      </c>
-      <c r="B69" s="26" t="s">
-        <v>428</v>
-      </c>
-      <c r="C69" s="25" t="s">
-        <v>379</v>
-      </c>
-      <c r="D69" s="37"/>
-      <c r="E69" s="27"/>
-    </row>
-    <row r="70" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A70" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B70" s="41" t="s">
-        <v>429</v>
-      </c>
-      <c r="C70" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D70" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="E70" s="27" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A71" s="21"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D71" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="E71" s="27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A72" s="21"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D72" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="E72" s="27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="2" customFormat="1">
-      <c r="A73" s="21"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="25" t="s">
-        <v>326</v>
-      </c>
-      <c r="D73" s="37" t="s">
-        <v>325</v>
-      </c>
-      <c r="E73" s="27"/>
-    </row>
-    <row r="74" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A74" s="21" t="s">
-        <v>488</v>
-      </c>
-      <c r="B74" s="41" t="s">
-        <v>438</v>
-      </c>
-      <c r="C74" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D74" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="E74" s="27" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="2" customFormat="1" ht="56">
-      <c r="A75" s="21"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D75" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="E75" s="27" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="2" customFormat="1" ht="56">
-      <c r="A76" s="21" t="s">
-        <v>489</v>
-      </c>
-      <c r="B76" s="41" t="s">
-        <v>435</v>
-      </c>
-      <c r="C76" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D76" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="E76" s="27" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="2" customFormat="1" ht="56">
-      <c r="A77" s="21" t="s">
-        <v>490</v>
-      </c>
-      <c r="B77" s="41" t="s">
-        <v>436</v>
-      </c>
-      <c r="C77" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D77" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="E77" s="27" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="2" customFormat="1">
-      <c r="A78" s="21" t="s">
-        <v>283</v>
-      </c>
-      <c r="B78" s="41" t="s">
-        <v>427</v>
-      </c>
-      <c r="C78" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="D78" s="37" t="s">
-        <v>334</v>
-      </c>
-      <c r="E78" s="27"/>
-    </row>
-    <row r="79" spans="1:5" s="2" customFormat="1">
-      <c r="A79" s="21" t="s">
-        <v>285</v>
-      </c>
-      <c r="B79" s="41" t="s">
-        <v>430</v>
-      </c>
-      <c r="C79" s="25" t="s">
-        <v>285</v>
-      </c>
-      <c r="D79" s="37" t="s">
-        <v>321</v>
-      </c>
-      <c r="E79" s="27"/>
-    </row>
-    <row r="80" spans="1:5" s="2" customFormat="1">
-      <c r="A80" s="21"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="25" t="s">
-        <v>329</v>
-      </c>
-      <c r="D80" s="37" t="s">
-        <v>322</v>
-      </c>
-      <c r="E80" s="27"/>
-    </row>
-    <row r="81" spans="1:9" s="2" customFormat="1">
-      <c r="A81" s="21" t="s">
-        <v>286</v>
-      </c>
-      <c r="B81" s="41" t="s">
-        <v>431</v>
-      </c>
-      <c r="C81" s="25" t="s">
-        <v>286</v>
-      </c>
-      <c r="D81" s="37" t="s">
-        <v>331</v>
-      </c>
-      <c r="E81" s="27"/>
-    </row>
-    <row r="82" spans="1:9">
-      <c r="C82" s="18" t="s">
-        <v>330</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" s="2" customFormat="1">
-      <c r="A83" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="B83" s="41" t="s">
-        <v>432</v>
-      </c>
-      <c r="C83" s="21" t="s">
-        <v>380</v>
-      </c>
-      <c r="D83" s="37" t="s">
-        <v>323</v>
-      </c>
-      <c r="E83" s="27"/>
-    </row>
-    <row r="84" spans="1:9" s="2" customFormat="1">
-      <c r="A84" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="B84" s="41" t="s">
-        <v>433</v>
-      </c>
-      <c r="C84" s="21" t="s">
-        <v>434</v>
-      </c>
-      <c r="D84" s="37" t="s">
-        <v>324</v>
-      </c>
-      <c r="E84" s="27"/>
-    </row>
-    <row r="85" spans="1:9" s="2" customFormat="1">
-      <c r="A85" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="B85" s="41" t="s">
-        <v>437</v>
-      </c>
-      <c r="C85" s="25" t="s">
-        <v>290</v>
-      </c>
-      <c r="D85" s="37" t="s">
-        <v>333</v>
-      </c>
-      <c r="E85" s="27"/>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="B86" s="40" t="s">
-        <v>467</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="D86" s="17" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="B87" s="40" t="s">
-        <v>456</v>
-      </c>
-      <c r="C87" s="28" t="s">
-        <v>452</v>
-      </c>
-      <c r="D87" s="29"/>
-      <c r="E87" s="30"/>
-    </row>
-    <row r="88" spans="1:9" s="2" customFormat="1">
-      <c r="A88" s="21" t="s">
-        <v>453</v>
-      </c>
-      <c r="B88" s="41" t="s">
-        <v>457</v>
-      </c>
-      <c r="C88" s="25" t="s">
-        <v>388</v>
-      </c>
-      <c r="D88" s="37"/>
-      <c r="E88" s="27"/>
-    </row>
-    <row r="89" spans="1:9" s="2" customFormat="1">
-      <c r="A89" s="21" t="s">
-        <v>454</v>
-      </c>
-      <c r="B89" s="41" t="s">
-        <v>458</v>
-      </c>
-      <c r="C89" s="25" t="s">
-        <v>389</v>
-      </c>
-      <c r="D89" s="37"/>
-      <c r="E89" s="27"/>
-    </row>
-    <row r="90" spans="1:9" s="2" customFormat="1">
-      <c r="A90" s="21" t="s">
-        <v>455</v>
-      </c>
-      <c r="B90" s="41" t="s">
-        <v>459</v>
-      </c>
-      <c r="C90" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="D90" s="37"/>
-      <c r="E90" s="27"/>
+      <c r="D89" s="34"/>
+      <c r="E89" s="24" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A90" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="B90" s="38" t="s">
+        <v>445</v>
+      </c>
+      <c r="C90" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="D90" s="34"/>
+      <c r="E90" s="24" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="91" spans="1:9">
-      <c r="C91" s="28" t="s">
-        <v>377</v>
-      </c>
-      <c r="D91" s="29"/>
-      <c r="E91" s="30"/>
+      <c r="C91" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="D91" s="27"/>
+      <c r="E91" s="42"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" ht="28">
       <c r="A92" s="15" t="s">
-        <v>369</v>
-      </c>
-      <c r="B92" s="22" t="s">
-        <v>418</v>
+        <v>355</v>
+      </c>
+      <c r="B92" s="37" t="s">
+        <v>404</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" s="2" customFormat="1">
-      <c r="A93" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="B93" s="26" t="s">
-        <v>419</v>
-      </c>
-      <c r="C93" s="25" t="s">
-        <v>368</v>
-      </c>
-      <c r="D93" s="37" t="s">
+        <v>356</v>
+      </c>
+      <c r="E92" s="24" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" s="2" customFormat="1" ht="28">
+      <c r="A93" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B93" s="38" t="s">
+        <v>405</v>
+      </c>
+      <c r="C93" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="D93" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="27"/>
-    </row>
-    <row r="94" spans="1:9" s="2" customFormat="1">
-      <c r="A94" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="B94" s="26" t="s">
-        <v>426</v>
-      </c>
-      <c r="C94" s="25" t="s">
-        <v>376</v>
-      </c>
-      <c r="D94" s="37" t="s">
+      <c r="E93" s="24" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" s="2" customFormat="1" ht="28">
+      <c r="A94" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="B94" s="38" t="s">
+        <v>412</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>362</v>
+      </c>
+      <c r="D94" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="E94" s="27"/>
+      <c r="E94" s="24" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="95" spans="1:9">
-      <c r="C95" s="28" t="s">
-        <v>335</v>
-      </c>
-      <c r="D95" s="29"/>
-      <c r="E95" s="30"/>
+      <c r="C95" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D95" s="27"/>
+      <c r="E95" s="42"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" ht="28">
       <c r="C96" s="18" t="s">
         <v>137</v>
       </c>
       <c r="D96" s="19" t="s">
-        <v>336</v>
-      </c>
-      <c r="E96" s="20" t="s">
-        <v>261</v>
+        <v>324</v>
+      </c>
+      <c r="E96" s="18" t="s">
+        <v>511</v>
       </c>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
@@ -4016,55 +4373,55 @@
       <c r="I96" s="3"/>
     </row>
     <row r="97" spans="1:9">
-      <c r="C97" s="28" t="s">
+      <c r="C97" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D97" s="29"/>
-      <c r="E97" s="30"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="42"/>
     </row>
     <row r="98" spans="1:9" s="2" customFormat="1">
-      <c r="A98" s="21" t="s">
-        <v>412</v>
-      </c>
-      <c r="B98" s="26" t="s">
-        <v>483</v>
-      </c>
-      <c r="C98" s="36" t="s">
-        <v>406</v>
-      </c>
-      <c r="D98" s="38"/>
-      <c r="E98" s="27"/>
+      <c r="A98" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="B98" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="C98" s="33" t="s">
+        <v>392</v>
+      </c>
+      <c r="D98" s="35"/>
+      <c r="E98" s="24"/>
     </row>
     <row r="99" spans="1:9" ht="42">
       <c r="C99" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D99" s="22" t="s">
+      <c r="D99" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="E99" s="20" t="s">
+      <c r="E99" s="18" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="42">
-      <c r="C100" s="25" t="s">
+      <c r="C100" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D100" s="22" t="s">
+      <c r="D100" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="E100" s="20" t="s">
+      <c r="E100" s="18" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="42">
-      <c r="C101" s="25" t="s">
+      <c r="C101" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D101" s="22" t="s">
+      <c r="D101" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E101" s="20" t="s">
+      <c r="E101" s="18" t="s">
         <v>195</v>
       </c>
       <c r="F101" s="3"/>
@@ -4073,13 +4430,13 @@
       <c r="I101" s="3"/>
     </row>
     <row r="102" spans="1:9" ht="42">
-      <c r="C102" s="25" t="s">
+      <c r="C102" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="D102" s="22" t="s">
+      <c r="D102" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="E102" s="20" t="s">
+      <c r="E102" s="18" t="s">
         <v>197</v>
       </c>
       <c r="F102" s="3"/>
@@ -4087,15 +4444,15 @@
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
     </row>
-    <row r="103" spans="1:9" ht="56">
+    <row r="103" spans="1:9" ht="42">
       <c r="C103" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D103" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="E103" s="20" t="s">
-        <v>223</v>
+      <c r="D103" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="E103" s="18" t="s">
+        <v>220</v>
       </c>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
@@ -4106,11 +4463,11 @@
       <c r="C104" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D104" s="22" t="s">
+      <c r="D104" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="E104" s="20" t="s">
-        <v>224</v>
+      <c r="E104" s="18" t="s">
+        <v>221</v>
       </c>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
@@ -4121,11 +4478,11 @@
       <c r="C105" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D105" s="22" t="s">
-        <v>260</v>
-      </c>
-      <c r="E105" s="20" t="s">
-        <v>225</v>
+      <c r="D105" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="E105" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
@@ -4133,43 +4490,43 @@
       <c r="I105" s="3"/>
     </row>
     <row r="106" spans="1:9">
-      <c r="C106" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="D106" s="29"/>
-      <c r="E106" s="30"/>
+      <c r="C106" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="D106" s="27"/>
+      <c r="E106" s="42"/>
     </row>
     <row r="107" spans="1:9" ht="42">
       <c r="C107" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D107" s="22" t="s">
+      <c r="D107" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="E107" s="20" t="s">
-        <v>234</v>
+      <c r="E107" s="18" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="42">
-      <c r="C108" s="25" t="s">
+      <c r="C108" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D108" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="E108" s="20" t="s">
-        <v>235</v>
+      <c r="D108" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="E108" s="18" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="42">
-      <c r="C109" s="25" t="s">
+      <c r="C109" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D109" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="E109" s="20" t="s">
-        <v>236</v>
+      <c r="D109" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="E109" s="18" t="s">
+        <v>229</v>
       </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
@@ -4177,14 +4534,14 @@
       <c r="I109" s="3"/>
     </row>
     <row r="110" spans="1:9" ht="42">
-      <c r="C110" s="25" t="s">
+      <c r="C110" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="D110" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="E110" s="20" t="s">
-        <v>237</v>
+      <c r="D110" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="E110" s="18" t="s">
+        <v>230</v>
       </c>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
@@ -4195,11 +4552,11 @@
       <c r="C111" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D111" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="E111" s="20" t="s">
-        <v>238</v>
+      <c r="D111" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="E111" s="18" t="s">
+        <v>231</v>
       </c>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
@@ -4210,11 +4567,11 @@
       <c r="C112" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D112" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="E112" s="20" t="s">
-        <v>239</v>
+      <c r="D112" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E112" s="18" t="s">
+        <v>232</v>
       </c>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
@@ -4225,11 +4582,11 @@
       <c r="C113" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D113" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="E113" s="20" t="s">
-        <v>243</v>
+      <c r="D113" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="E113" s="18" t="s">
+        <v>236</v>
       </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -4237,43 +4594,43 @@
       <c r="I113" s="3"/>
     </row>
     <row r="114" spans="1:9">
-      <c r="C114" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="D114" s="29"/>
-      <c r="E114" s="30"/>
+      <c r="C114" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="D114" s="27"/>
+      <c r="E114" s="42"/>
     </row>
     <row r="115" spans="1:9" ht="42">
       <c r="C115" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D115" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="E115" s="20" t="s">
-        <v>248</v>
+      <c r="D115" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="E115" s="18" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="42">
-      <c r="C116" s="25" t="s">
+      <c r="C116" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D116" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="E116" s="20" t="s">
-        <v>249</v>
+      <c r="D116" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="E116" s="18" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="42">
-      <c r="C117" s="25" t="s">
+      <c r="C117" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D117" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="E117" s="20" t="s">
-        <v>250</v>
+      <c r="D117" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="E117" s="18" t="s">
+        <v>243</v>
       </c>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
@@ -4281,14 +4638,14 @@
       <c r="I117" s="3"/>
     </row>
     <row r="118" spans="1:9" ht="42">
-      <c r="C118" s="25" t="s">
+      <c r="C118" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="D118" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="E118" s="20" t="s">
-        <v>251</v>
+      <c r="D118" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="E118" s="18" t="s">
+        <v>244</v>
       </c>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
@@ -4299,11 +4656,11 @@
       <c r="C119" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D119" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="E119" s="20" t="s">
-        <v>252</v>
+      <c r="D119" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="E119" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
@@ -4314,11 +4671,11 @@
       <c r="C120" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D120" s="22" t="s">
+      <c r="D120" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="E120" s="20" t="s">
-        <v>253</v>
+      <c r="E120" s="18" t="s">
+        <v>246</v>
       </c>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
@@ -4329,11 +4686,11 @@
       <c r="C121" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D121" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="E121" s="20" t="s">
-        <v>256</v>
+      <c r="D121" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="E121" s="18" t="s">
+        <v>249</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
@@ -4341,77 +4698,85 @@
       <c r="I121" s="3"/>
     </row>
     <row r="122" spans="1:9">
-      <c r="B122" s="22" t="s">
-        <v>439</v>
-      </c>
-      <c r="C122" s="28" t="s">
-        <v>297</v>
-      </c>
-      <c r="D122" s="29"/>
-      <c r="E122" s="30"/>
+      <c r="B122" s="37" t="s">
+        <v>425</v>
+      </c>
+      <c r="C122" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="D122" s="27"/>
+      <c r="E122" s="42"/>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" ht="42">
       <c r="A123" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="B123" s="22" t="s">
-        <v>440</v>
+        <v>367</v>
+      </c>
+      <c r="B123" s="37" t="s">
+        <v>426</v>
       </c>
       <c r="C123" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="D123" s="22"/>
-      <c r="E123" s="20"/>
+        <v>368</v>
+      </c>
+      <c r="D123" s="21" t="s">
+        <v>513</v>
+      </c>
+      <c r="E123" s="18" t="s">
+        <v>512</v>
+      </c>
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" ht="42">
       <c r="A124" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="B124" s="22" t="s">
-        <v>441</v>
+        <v>369</v>
+      </c>
+      <c r="B124" s="37" t="s">
+        <v>427</v>
       </c>
       <c r="C124" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="D124" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="D124" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="E124" s="20"/>
+      <c r="E124" s="18" t="s">
+        <v>514</v>
+      </c>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" ht="42">
       <c r="A125" s="15" t="s">
-        <v>384</v>
-      </c>
-      <c r="B125" s="22" t="s">
-        <v>442</v>
+        <v>370</v>
+      </c>
+      <c r="B125" s="37" t="s">
+        <v>428</v>
       </c>
       <c r="C125" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="D125" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="D125" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="E125" s="20"/>
+      <c r="E125" s="18" t="s">
+        <v>515</v>
+      </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
     </row>
-    <row r="126" spans="1:9" ht="56">
-      <c r="B126" s="40" t="s">
-        <v>443</v>
+    <row r="126" spans="1:9" ht="42">
+      <c r="B126" s="37" t="s">
+        <v>429</v>
       </c>
       <c r="C126" s="18" t="s">
         <v>138</v>
@@ -4419,422 +4784,435 @@
       <c r="D126" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="E126" s="20" t="s">
-        <v>226</v>
+      <c r="E126" s="18" t="s">
+        <v>516</v>
       </c>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" ht="42">
       <c r="A127" s="15" t="s">
-        <v>292</v>
-      </c>
-      <c r="B127" s="40" t="s">
-        <v>444</v>
+        <v>282</v>
+      </c>
+      <c r="B127" s="37" t="s">
+        <v>430</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="D127" s="19" t="s">
-        <v>342</v>
-      </c>
-      <c r="E127" s="20"/>
+        <v>330</v>
+      </c>
+      <c r="E127" s="18" t="s">
+        <v>517</v>
+      </c>
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
     </row>
-    <row r="128" spans="1:9" ht="56">
+    <row r="128" spans="1:9" ht="42">
       <c r="A128" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B128" s="40" t="s">
-        <v>445</v>
+      <c r="B128" s="37" t="s">
+        <v>431</v>
       </c>
       <c r="C128" s="18" t="s">
         <v>139</v>
       </c>
       <c r="D128" s="19" t="s">
-        <v>345</v>
-      </c>
-      <c r="E128" s="20" t="s">
-        <v>227</v>
+        <v>333</v>
+      </c>
+      <c r="E128" s="18" t="s">
+        <v>518</v>
       </c>
       <c r="F128" s="3"/>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
     </row>
-    <row r="129" spans="1:9" ht="56">
+    <row r="129" spans="1:9" ht="42">
       <c r="A129" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B129" s="40" t="s">
-        <v>446</v>
+      <c r="B129" s="37" t="s">
+        <v>432</v>
       </c>
       <c r="C129" s="18" t="s">
         <v>140</v>
       </c>
       <c r="D129" s="19" t="s">
-        <v>346</v>
-      </c>
-      <c r="E129" s="20" t="s">
-        <v>228</v>
+        <v>334</v>
+      </c>
+      <c r="E129" s="18" t="s">
+        <v>519</v>
       </c>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
     </row>
-    <row r="130" spans="1:9" ht="56">
+    <row r="130" spans="1:9" ht="42">
       <c r="A130" s="15" t="s">
-        <v>387</v>
-      </c>
-      <c r="B130" s="40" t="s">
-        <v>447</v>
+        <v>373</v>
+      </c>
+      <c r="B130" s="37" t="s">
+        <v>433</v>
       </c>
       <c r="C130" s="18" t="s">
         <v>141</v>
       </c>
       <c r="D130" s="19" t="s">
-        <v>343</v>
-      </c>
-      <c r="E130" s="20" t="s">
-        <v>229</v>
+        <v>331</v>
+      </c>
+      <c r="E130" s="18" t="s">
+        <v>520</v>
       </c>
       <c r="F130" s="3"/>
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" ht="42">
       <c r="A131" s="15" t="s">
-        <v>293</v>
-      </c>
-      <c r="B131" s="40" t="s">
-        <v>448</v>
+        <v>283</v>
+      </c>
+      <c r="B131" s="37" t="s">
+        <v>434</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D131" s="19" t="s">
-        <v>344</v>
-      </c>
-      <c r="E131" s="20"/>
+        <v>332</v>
+      </c>
+      <c r="E131" s="18" t="s">
+        <v>521</v>
+      </c>
       <c r="F131" s="3"/>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
     </row>
     <row r="132" spans="1:9">
-      <c r="C132" s="28" t="s">
-        <v>337</v>
-      </c>
-      <c r="D132" s="29"/>
-      <c r="E132" s="30"/>
+      <c r="C132" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="D132" s="27"/>
+      <c r="E132" s="42"/>
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
     </row>
-    <row r="133" spans="1:9" s="2" customFormat="1">
-      <c r="A133" s="21" t="s">
-        <v>287</v>
-      </c>
-      <c r="B133" s="41" t="s">
-        <v>425</v>
-      </c>
-      <c r="C133" s="21" t="s">
-        <v>287</v>
-      </c>
-      <c r="D133" s="37" t="s">
-        <v>338</v>
-      </c>
-      <c r="E133" s="27"/>
-    </row>
-    <row r="134" spans="1:9">
+    <row r="133" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="A133" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="B133" s="38" t="s">
+        <v>411</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="D133" s="34" t="s">
+        <v>326</v>
+      </c>
+      <c r="E133" s="24" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="56">
       <c r="A134" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="B134" s="40" t="s">
-        <v>449</v>
+        <v>284</v>
+      </c>
+      <c r="B134" s="37" t="s">
+        <v>435</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D134" s="16" t="s">
-        <v>339</v>
-      </c>
-      <c r="E134" s="10"/>
+        <v>327</v>
+      </c>
+      <c r="E134" s="24" t="s">
+        <v>523</v>
+      </c>
       <c r="F134" s="3"/>
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" ht="56">
       <c r="A135" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="B135" s="40" t="s">
-        <v>450</v>
+        <v>285</v>
+      </c>
+      <c r="B135" s="37" t="s">
+        <v>436</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="D135" s="16" t="s">
-        <v>340</v>
-      </c>
-      <c r="E135" s="10"/>
+        <v>328</v>
+      </c>
+      <c r="E135" s="24" t="s">
+        <v>524</v>
+      </c>
       <c r="F135" s="3"/>
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" ht="56">
       <c r="A136" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="B136" s="40" t="s">
-        <v>451</v>
+        <v>286</v>
+      </c>
+      <c r="B136" s="37" t="s">
+        <v>437</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="D136" s="16" t="s">
-        <v>341</v>
-      </c>
-      <c r="E136" s="10"/>
+        <v>329</v>
+      </c>
+      <c r="E136" s="24" t="s">
+        <v>525</v>
+      </c>
       <c r="F136" s="3"/>
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
     </row>
     <row r="137" spans="1:9">
-      <c r="C137" s="28" t="s">
-        <v>298</v>
-      </c>
-      <c r="D137" s="29"/>
-      <c r="E137" s="30"/>
-    </row>
-    <row r="138" spans="1:9">
+      <c r="C137" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="D137" s="27"/>
+      <c r="E137" s="42"/>
+    </row>
+    <row r="138" spans="1:9" ht="36">
       <c r="A138" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="B138" s="40" t="s">
-        <v>465</v>
+        <v>290</v>
+      </c>
+      <c r="B138" s="37" t="s">
+        <v>451</v>
       </c>
       <c r="C138" s="18" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="D138" s="16" t="s">
-        <v>348</v>
-      </c>
-      <c r="E138" s="10"/>
+        <v>336</v>
+      </c>
+      <c r="E138" s="44" t="s">
+        <v>527</v>
+      </c>
       <c r="F138" s="3"/>
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" ht="36">
       <c r="A139" s="15" t="s">
-        <v>405</v>
-      </c>
-      <c r="B139" s="40" t="s">
-        <v>466</v>
+        <v>391</v>
+      </c>
+      <c r="B139" s="37" t="s">
+        <v>452</v>
       </c>
       <c r="C139" s="18" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D139" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="E139" s="10"/>
+        <v>335</v>
+      </c>
+      <c r="E139" s="44" t="s">
+        <v>526</v>
+      </c>
       <c r="F139" s="3"/>
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
     </row>
     <row r="140" spans="1:9">
-      <c r="C140" s="28" t="s">
-        <v>404</v>
-      </c>
-      <c r="D140" s="29"/>
-      <c r="E140" s="30"/>
-    </row>
-    <row r="141" spans="1:9">
-      <c r="A141" s="23" t="s">
-        <v>305</v>
-      </c>
-      <c r="B141" s="24" t="s">
+      <c r="C140" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="D140" s="27"/>
+      <c r="E140" s="42"/>
+    </row>
+    <row r="141" spans="1:9" ht="42">
+      <c r="A141" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="B141" s="41" t="s">
+        <v>477</v>
+      </c>
+      <c r="D141" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="E141" s="18" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="42">
+      <c r="A142" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="B142" s="41" t="s">
         <v>478</v>
       </c>
-      <c r="C141" s="18" t="s">
-        <v>317</v>
-      </c>
-      <c r="D141" s="24" t="s">
-        <v>334</v>
-      </c>
-      <c r="E141" s="18"/>
-    </row>
-    <row r="142" spans="1:9">
-      <c r="A142" s="23" t="s">
-        <v>306</v>
-      </c>
-      <c r="B142" s="24" t="s">
-        <v>479</v>
-      </c>
-      <c r="C142" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="D142" s="24" t="s">
-        <v>334</v>
-      </c>
-      <c r="E142" s="18"/>
-    </row>
-    <row r="143" spans="1:9">
-      <c r="A143" s="23" t="s">
-        <v>307</v>
-      </c>
-      <c r="B143" s="24" t="s">
-        <v>480</v>
-      </c>
-      <c r="C143" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="D143" s="24" t="s">
-        <v>334</v>
-      </c>
-      <c r="E143" s="18"/>
+      <c r="D142" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="E142" s="18" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="42">
+      <c r="A143" s="22" t="s">
+        <v>297</v>
+      </c>
+      <c r="B143" s="41" t="s">
+        <v>464</v>
+      </c>
+      <c r="D143" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="E143" s="18" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="144" spans="1:9">
-      <c r="B144" s="22" t="s">
-        <v>486</v>
-      </c>
-      <c r="C144" s="28" t="s">
-        <v>415</v>
-      </c>
-      <c r="D144" s="29"/>
-      <c r="E144" s="30"/>
+      <c r="B144" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="C144" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="D144" s="27"/>
+      <c r="E144" s="42"/>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="15" t="s">
-        <v>411</v>
-      </c>
-      <c r="B145" s="22" t="s">
-        <v>481</v>
+        <v>397</v>
+      </c>
+      <c r="B145" s="21" t="s">
+        <v>465</v>
       </c>
       <c r="C145" s="18" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="D145" s="19"/>
-      <c r="E145" s="20"/>
+      <c r="E145" s="18"/>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B146" s="22" t="s">
-        <v>482</v>
+      <c r="B146" s="21" t="s">
+        <v>466</v>
       </c>
       <c r="C146" s="18" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="D146" s="19"/>
-      <c r="E146" s="20"/>
+      <c r="E146" s="18"/>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="15" t="s">
-        <v>413</v>
-      </c>
-      <c r="B147" s="22" t="s">
-        <v>484</v>
+        <v>399</v>
+      </c>
+      <c r="B147" s="21" t="s">
+        <v>468</v>
       </c>
       <c r="C147" s="18" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="D147" s="19"/>
-      <c r="E147" s="20"/>
+      <c r="E147" s="18"/>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="15" t="s">
-        <v>414</v>
-      </c>
-      <c r="B148" s="22" t="s">
-        <v>485</v>
+        <v>400</v>
+      </c>
+      <c r="B148" s="21" t="s">
+        <v>469</v>
       </c>
       <c r="C148" s="18" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="D148" s="19"/>
-      <c r="E148" s="20"/>
+      <c r="E148" s="18"/>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="B149" s="22" t="s">
-        <v>487</v>
+        <v>402</v>
+      </c>
+      <c r="B149" s="21" t="s">
+        <v>471</v>
       </c>
       <c r="C149" s="18" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="D149" s="19"/>
-      <c r="E149" s="20"/>
+      <c r="E149" s="18"/>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="23"/>
-      <c r="B150" s="24"/>
-      <c r="D150" s="24"/>
+      <c r="A150" s="22"/>
+      <c r="B150" s="23"/>
+      <c r="D150" s="23"/>
       <c r="E150" s="18"/>
     </row>
     <row r="151" spans="1:5">
-      <c r="A151" s="23"/>
-      <c r="B151" s="24"/>
-      <c r="D151" s="24"/>
+      <c r="A151" s="22"/>
+      <c r="B151" s="23"/>
+      <c r="D151" s="23"/>
       <c r="E151" s="18"/>
     </row>
     <row r="152" spans="1:5">
-      <c r="A152" s="23"/>
-      <c r="B152" s="24"/>
-      <c r="D152" s="24"/>
+      <c r="A152" s="22"/>
+      <c r="B152" s="23"/>
+      <c r="D152" s="23"/>
       <c r="E152" s="18"/>
     </row>
     <row r="153" spans="1:5">
-      <c r="A153" s="23"/>
-      <c r="B153" s="24"/>
-      <c r="D153" s="24"/>
+      <c r="A153" s="22"/>
+      <c r="B153" s="23"/>
+      <c r="D153" s="23"/>
       <c r="E153" s="18"/>
     </row>
     <row r="154" spans="1:5">
-      <c r="A154" s="23"/>
-      <c r="B154" s="24"/>
-      <c r="D154" s="24"/>
+      <c r="A154" s="22"/>
+      <c r="B154" s="23"/>
+      <c r="D154" s="23"/>
       <c r="E154" s="18"/>
     </row>
     <row r="155" spans="1:5">
-      <c r="A155" s="23"/>
-      <c r="B155" s="24"/>
-      <c r="D155" s="24"/>
+      <c r="A155" s="22"/>
+      <c r="B155" s="23"/>
+      <c r="D155" s="23"/>
       <c r="E155" s="18"/>
     </row>
     <row r="156" spans="1:5">
-      <c r="A156" s="23"/>
-      <c r="B156" s="24"/>
-      <c r="D156" s="24"/>
+      <c r="A156" s="22"/>
+      <c r="B156" s="23"/>
+      <c r="D156" s="23"/>
       <c r="E156" s="18"/>
     </row>
     <row r="157" spans="1:5">
-      <c r="A157" s="23"/>
-      <c r="B157" s="24"/>
-      <c r="D157" s="24"/>
+      <c r="A157" s="22"/>
+      <c r="B157" s="23"/>
+      <c r="D157" s="23"/>
       <c r="E157" s="18"/>
     </row>
     <row r="158" spans="1:5">
-      <c r="A158" s="23"/>
-      <c r="B158" s="24"/>
-      <c r="D158" s="24"/>
+      <c r="A158" s="22"/>
+      <c r="B158" s="23"/>
+      <c r="D158" s="23"/>
       <c r="E158" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated SSP with additional Hawaii requirements.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/ProsecutionCaseQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/ProsecutionCaseQueryResults.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="1680" windowWidth="27300" windowHeight="13740"/>
+    <workbookView xWindow="4780" yWindow="2540" windowWidth="28560" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="576">
   <si>
     <t>ATN [Arrest Tracking Number]</t>
   </si>
@@ -795,9 +795,6 @@
     <t>1143299</t>
   </si>
   <si>
-    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Offense/nc:ActivityDate/nc:Date</t>
-  </si>
-  <si>
     <t>2016-09-12</t>
   </si>
   <si>
@@ -807,9 +804,6 @@
     <t>Smithville</t>
   </si>
   <si>
-    <t>Prosecution Case Query Result Element</t>
-  </si>
-  <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest/j:ArrestAgencyRecordIdentification/nc:IdentificationJurisdiction/nc:JurisdictionText</t>
   </si>
   <si>
@@ -900,9 +894,6 @@
     <t xml:space="preserve">Count Number </t>
   </si>
   <si>
-    <t>Change to Date/Time</t>
-  </si>
-  <si>
     <t>CDL</t>
   </si>
   <si>
@@ -1170,12 +1161,6 @@
     <t>Incident Number</t>
   </si>
   <si>
-    <t>Violation Date/Time</t>
-  </si>
-  <si>
-    <t>Activity Date/Time</t>
-  </si>
-  <si>
     <t>Charge Code</t>
   </si>
   <si>
@@ -1194,36 +1179,21 @@
     <t>Booking #</t>
   </si>
   <si>
-    <t>CHECK WITH HAWAII ON INFO</t>
-  </si>
-  <si>
     <t>Method of Case Initiation</t>
   </si>
   <si>
     <t>Violation For</t>
   </si>
   <si>
-    <t>Arrest Detail</t>
-  </si>
-  <si>
-    <t>Date Range</t>
-  </si>
-  <si>
     <t>Document Category</t>
   </si>
   <si>
-    <t>Filing Parties</t>
-  </si>
-  <si>
     <t>In Response To</t>
   </si>
   <si>
     <t>Supporting Doc For</t>
   </si>
   <si>
-    <t>Attached Lead Document</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -1380,12 +1350,6 @@
     <t>58</t>
   </si>
   <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
     <t>55/62</t>
   </si>
   <si>
@@ -1398,9 +1362,6 @@
     <t>65</t>
   </si>
   <si>
-    <t>66/67</t>
-  </si>
-  <si>
     <t>69</t>
   </si>
   <si>
@@ -1419,21 +1380,12 @@
     <t>76</t>
   </si>
   <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>78</t>
-  </si>
-  <si>
     <t>79</t>
   </si>
   <si>
     <t>80</t>
   </si>
   <si>
-    <t>81</t>
-  </si>
-  <si>
     <t>SID</t>
   </si>
   <si>
@@ -1446,10 +1398,6 @@
     <t>Suffix</t>
   </si>
   <si>
-    <t>RED - In XML Instance
-Black - Waiting for more info</t>
-  </si>
-  <si>
     <t>72-Ext</t>
   </si>
   <si>
@@ -1622,13 +1570,193 @@
   </si>
   <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCourt/nc:OrganizationLocation/nc:LocationName</t>
+  </si>
+  <si>
+    <t>Person Arrested (First, Middle, Last)</t>
+  </si>
+  <si>
+    <t>Person Charged (First, Middle, Last)</t>
+  </si>
+  <si>
+    <t>Plantiff and Defendant (Part Type and Party Name)</t>
+  </si>
+  <si>
+    <t>Supporting documents for a lead document</t>
+  </si>
+  <si>
+    <t>Note for each document filed</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>Lead Document</t>
+  </si>
+  <si>
+    <t>In Camera</t>
+  </si>
+  <si>
+    <t>Seal</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Element/Description</t>
+  </si>
+  <si>
+    <t>Arrest Subject</t>
+  </si>
+  <si>
+    <t>Arrest Official</t>
+  </si>
+  <si>
+    <t>60, 61</t>
+  </si>
+  <si>
+    <t>Document Category Name</t>
+  </si>
+  <si>
+    <t>Document Related Resource Text</t>
+  </si>
+  <si>
+    <t>Document Description Text</t>
+  </si>
+  <si>
+    <t>Previously filed docket entries</t>
+  </si>
+  <si>
+    <t>Previously Filed Docket Text</t>
+  </si>
+  <si>
+    <t>78-Ext</t>
+  </si>
+  <si>
+    <t>Document viewing by public and other parties is restricted</t>
+  </si>
+  <si>
+    <t>Document viewing by public is restricted</t>
+  </si>
+  <si>
+    <t>Document Public Viewing Restricted Indicator</t>
+  </si>
+  <si>
+    <t>Document Public Party Viewing Restricted Indicator</t>
+  </si>
+  <si>
+    <t>81-Ext</t>
+  </si>
+  <si>
+    <t>83-Ext</t>
+  </si>
+  <si>
+    <t>Case Initiation Method Text</t>
+  </si>
+  <si>
+    <t>5-Ext</t>
+  </si>
+  <si>
+    <t>Element Reference</t>
+  </si>
+  <si>
+    <t>Element Description</t>
+  </si>
+  <si>
+    <t>Charge Subject</t>
+  </si>
+  <si>
+    <t>66, 67</t>
+  </si>
+  <si>
+    <t>Offense Date/Time Range</t>
+  </si>
+  <si>
+    <t>77-Ext</t>
+  </si>
+  <si>
+    <t>Case Initiating Party (Person/Official)</t>
+  </si>
+  <si>
+    <t>84-Ext</t>
+  </si>
+  <si>
+    <t>Document is Lead Document</t>
+  </si>
+  <si>
+    <t>Lead Document Indicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest/j:ArrestSubject/structures:ref</t>
+  </si>
+  <si>
+    <t>pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Arrest/j:ArrestOfficial/structures:ref</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Offense/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/j:Offense/nc:ActivityDateRange</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/pcq-res-ext:CaseInitiationMethodText</t>
+  </si>
+  <si>
+    <t>pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeSubject/structures:ref</t>
+  </si>
+  <si>
+    <t>Secondary Document</t>
+  </si>
+  <si>
+    <t>Primary Document (Lead)</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:SecondaryDocument/nc:DocumentCategoryText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:SecondaryDocument/nc:DocumentCategoryName</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:SecondaryDocument/nc:DocumentDescriptionText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:SecondaryDocument/pcq-res-ext:PreviouslyFiledDocketText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:SecondaryDocument/pcq-res-ext:DocumentPublicPartyViewingRestrictedIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:SecondaryDocument/pcq-res-ext:DocumentPublicViewingRestrictedIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:PrimaryDocument/nc:DocumentCategoryText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:PrimaryDocument/nc:DocumentCategoryName</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:PrimaryDocument/pcq-res-ext:PreviouslyFiledDocketText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:PrimaryDocument/nc:DocumentRelatedResourceText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:PrimaryDocument/nc:DocumentDescriptionText</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:PrimaryDocument/pcq-res-ext:DocumentPublicPartyViewingRestrictedIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:PrimaryDocument/pcq-res-ext:DocumentPublicViewingRestrictedIndicator</t>
+  </si>
+  <si>
+    <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:PrimaryDocument/pcq-res-ext:LeadDocumentIndicator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1829,6 +1957,21 @@
       <sz val="9"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1925,7 +2068,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="341">
+  <cellStyleXfs count="393">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -2267,8 +2410,60 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2402,8 +2597,17 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="341">
+  <cellStyles count="393">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -2588,6 +2792,32 @@
     <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -2739,6 +2969,32 @@
     <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="90"/>
@@ -3043,2191 +3299,2502 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J158"/>
+  <dimension ref="A1:K166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E159" sqref="E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21" style="21" customWidth="1"/>
-    <col min="3" max="3" width="37.1640625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="23" style="17" customWidth="1"/>
-    <col min="5" max="5" width="83.83203125" style="43" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="1"/>
+    <col min="2" max="3" width="21" style="21" customWidth="1"/>
+    <col min="4" max="4" width="37.1640625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="23" style="17" customWidth="1"/>
+    <col min="6" max="6" width="83.83203125" style="43" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="49" customHeight="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:6" ht="15">
+      <c r="A1" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>474</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>261</v>
-      </c>
-      <c r="D1" s="29" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+    </row>
+    <row r="2" spans="1:6" ht="49" customHeight="1">
+      <c r="A2" s="39" t="s">
+        <v>525</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>544</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>545</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F2" s="28" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="C2" s="30" t="s">
+    <row r="3" spans="1:6" ht="15">
+      <c r="D3" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="C3" s="18" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="D4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E4" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F4" s="18" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="C4" s="18" t="s">
+    <row r="5" spans="1:6">
+      <c r="D5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="E5" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F5" s="18" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="C5" s="18" t="s">
+    <row r="6" spans="1:6">
+      <c r="D6" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="E6" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="F6" s="18" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28">
-      <c r="C6" s="18" t="s">
+    <row r="7" spans="1:6" ht="28">
+      <c r="D7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="E7" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="C7" s="18" t="s">
+    <row r="8" spans="1:6">
+      <c r="D8" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="E8" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="F8" s="18" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="15" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>444</v>
-      </c>
-      <c r="C8" s="26" t="s">
+      <c r="B9" s="37" t="s">
+        <v>434</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="42"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="15" t="s">
-        <v>375</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>445</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>390</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="18"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="27"/>
+      <c r="F9" s="42"/>
+    </row>
+    <row r="10" spans="1:6" ht="28">
       <c r="A10" s="15" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>390</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="18"/>
-    </row>
-    <row r="11" spans="1:5">
+        <v>516</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>527</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="18" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28">
       <c r="A11" s="15" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>447</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>390</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="18"/>
-    </row>
-    <row r="12" spans="1:5" ht="42">
+        <v>437</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>528</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="18" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="42">
       <c r="A12" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>448</v>
-      </c>
-      <c r="C12" s="18" t="s">
+        <v>438</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="E12" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="42">
+      <c r="F12" s="18" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="42">
       <c r="A13" s="15" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>446</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="42">
+        <v>436</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="42">
       <c r="A14" s="15" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>454</v>
-      </c>
-      <c r="C14" s="18" t="s">
+        <v>442</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="28">
-      <c r="C15" s="18" t="s">
+      <c r="F14" s="18" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28">
+      <c r="D15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="E15" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="F15" s="18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28">
+      <c r="D16" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="42">
+      <c r="D17" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28">
-      <c r="C16" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="E16" s="18" t="s">
+    <row r="18" spans="1:6" ht="98">
+      <c r="D18" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="F18" s="43" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="42">
-      <c r="C17" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>252</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="98">
-      <c r="C18" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="E18" s="43" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="28">
       <c r="A19" s="20"/>
       <c r="B19" s="25"/>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="25"/>
+      <c r="D19" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="E19" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="C20" s="26" t="s">
-        <v>379</v>
-      </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="42"/>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="F19" s="18" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="D20" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="42"/>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="42">
       <c r="A21" s="20" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>455</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>381</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="18" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="C22" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="18" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="D22" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="42"/>
-    </row>
-    <row r="23" spans="1:5" s="2" customFormat="1">
-      <c r="A23" s="36" t="s">
-        <v>292</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="24" t="s">
-        <v>314</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>313</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A24" s="20"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="E22" s="27"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1">
+      <c r="A23" s="36"/>
+      <c r="B23" s="38" t="s">
+        <v>547</v>
+      </c>
+      <c r="C23" s="38"/>
+      <c r="D23" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1">
+      <c r="A24" s="36"/>
+      <c r="B24" s="38" t="s">
+        <v>445</v>
+      </c>
+      <c r="C24" s="38"/>
+      <c r="D24" s="24" t="s">
+        <v>548</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="24" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="28">
       <c r="A25" s="20"/>
       <c r="B25" s="25"/>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="25"/>
+      <c r="D25" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A26" s="20"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="34" t="s">
-        <v>260</v>
-      </c>
-      <c r="E25" s="24" t="s">
+      <c r="E26" s="34" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="C26" s="26" t="s">
+      <c r="F26" s="24" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="D27" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="42"/>
-    </row>
-    <row r="27" spans="1:5" s="2" customFormat="1">
-      <c r="A27" s="20"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="24" t="s">
+      <c r="E27" s="27"/>
+      <c r="F27" s="42"/>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1">
+      <c r="A28" s="20"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="E28" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="F28" s="24" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A28" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="B28" s="38">
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A29" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="B29" s="38">
         <v>4</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C29" s="38"/>
+      <c r="D29" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="E29" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="E28" s="24" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A29" s="20"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" ht="28">
+      <c r="F29" s="24" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="42">
       <c r="A30" s="20"/>
       <c r="B30" s="25"/>
-      <c r="C30" s="33" t="s">
-        <v>299</v>
-      </c>
-      <c r="D30" s="35" t="s">
+      <c r="C30" s="25"/>
+      <c r="D30" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A31" s="20"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="2" customFormat="1">
+      <c r="A32" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="F32" s="24"/>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1">
+      <c r="A33" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>543</v>
+      </c>
+      <c r="C33" s="38"/>
+      <c r="D33" s="33" t="s">
+        <v>542</v>
+      </c>
+      <c r="E33" s="35"/>
+      <c r="F33" s="24" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A34" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>391</v>
+      </c>
+      <c r="C34" s="38"/>
+      <c r="D34" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A35" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>513</v>
+      </c>
+      <c r="C35" s="38"/>
+      <c r="D35" s="24" t="s">
+        <v>514</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A36" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="B36" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="C36" s="38"/>
+      <c r="D36" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A37" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="B37" s="38">
+        <v>3</v>
+      </c>
+      <c r="C37" s="38"/>
+      <c r="D37" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A38" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="B38" s="38">
+        <v>6</v>
+      </c>
+      <c r="C38" s="38"/>
+      <c r="D38" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="2" customFormat="1">
+      <c r="A39" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="B39" s="38">
+        <v>7</v>
+      </c>
+      <c r="C39" s="38"/>
+      <c r="D39" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="2" customFormat="1">
+      <c r="A40" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="B40" s="38">
+        <v>9</v>
+      </c>
+      <c r="C40" s="38"/>
+      <c r="D40" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="F40" s="24" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="2" customFormat="1">
+      <c r="A41" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="B41" s="38">
+        <v>8</v>
+      </c>
+      <c r="C41" s="38"/>
+      <c r="D41" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="E30" s="24" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="2" customFormat="1">
-      <c r="A31" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="D31" s="35" t="s">
-        <v>297</v>
-      </c>
-      <c r="E31" s="24"/>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1">
-      <c r="A32" s="20" t="s">
-        <v>391</v>
-      </c>
-      <c r="B32" s="38">
+      <c r="E41" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="D42" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="33" t="s">
-        <v>390</v>
-      </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="24"/>
-    </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A33" s="20" t="s">
-        <v>350</v>
-      </c>
-      <c r="B33" s="38" t="s">
-        <v>401</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>351</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>349</v>
-      </c>
-      <c r="E33" s="24" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A34" s="20" t="s">
-        <v>268</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>530</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>531</v>
-      </c>
-      <c r="D34" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A35" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="B35" s="38" t="s">
+      <c r="E42" s="27"/>
+      <c r="F42" s="42"/>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A43" s="20"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A44" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="B44" s="38" t="s">
+        <v>529</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>517</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>546</v>
+      </c>
+      <c r="E44" s="25"/>
+      <c r="F44" s="24" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="42">
+      <c r="A45" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>444</v>
+      </c>
+      <c r="C45" s="37"/>
+      <c r="D45" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="F45" s="43" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="D46" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="42">
+      <c r="A47" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="37" t="s">
+        <v>448</v>
+      </c>
+      <c r="C47" s="37"/>
+      <c r="D47" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="C35" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A36" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="B36" s="38">
-        <v>3</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A37" s="20" t="s">
-        <v>344</v>
-      </c>
-      <c r="B37" s="38">
-        <v>6</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>320</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="2" customFormat="1">
-      <c r="A38" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="B38" s="38">
-        <v>7</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="D38" s="34" t="s">
-        <v>320</v>
-      </c>
-      <c r="E38" s="24" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1">
-      <c r="A39" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="B39" s="38">
-        <v>9</v>
-      </c>
-      <c r="C39" s="24" t="s">
-        <v>348</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>347</v>
-      </c>
-      <c r="E39" s="24" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="2" customFormat="1">
-      <c r="A40" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="B40" s="38">
-        <v>8</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>301</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>306</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="C41" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="42"/>
-    </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="28">
-      <c r="A42" s="20"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="2" customFormat="1">
-      <c r="A43" s="20" t="s">
-        <v>392</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>452</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>390</v>
-      </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="24"/>
-    </row>
-    <row r="44" spans="1:5" s="2" customFormat="1">
-      <c r="A44" s="20" t="s">
-        <v>394</v>
-      </c>
-      <c r="B44" s="34" t="s">
-        <v>457</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>390</v>
-      </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="24"/>
-    </row>
-    <row r="45" spans="1:5" ht="42">
-      <c r="A45" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="B45" s="37" t="s">
-        <v>456</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>336</v>
-      </c>
-      <c r="E45" s="43" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="15" t="s">
+      <c r="E47" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="F47" s="43" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="2" customFormat="1" ht="28">
+      <c r="A48" s="20"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="2" customFormat="1" ht="28">
+      <c r="A49" s="20"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" s="2" customFormat="1" ht="28">
+      <c r="A50" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="B50" s="38" t="s">
+        <v>447</v>
+      </c>
+      <c r="C50" s="38"/>
+      <c r="D50" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="F50" s="24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="2" customFormat="1" ht="42">
+      <c r="D51" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="F51" s="43" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="2" customFormat="1" ht="42">
+      <c r="A52" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="B52" s="38" t="s">
+        <v>446</v>
+      </c>
+      <c r="C52" s="38"/>
+      <c r="D52" s="24" t="s">
         <v>382</v>
       </c>
-      <c r="B46" s="37" t="s">
-        <v>458</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="D46" s="21"/>
-      <c r="E46" s="43" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="C47" s="15"/>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="C48" s="18" t="s">
-        <v>340</v>
-      </c>
-      <c r="D48" s="21" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="42">
-      <c r="A49" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B49" s="37" t="s">
-        <v>461</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>339</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>342</v>
-      </c>
-      <c r="E49" s="43" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" s="2" customFormat="1" ht="28">
-      <c r="A50" s="20"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" s="2" customFormat="1" ht="28">
-      <c r="A51" s="20"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="E51" s="24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" s="2" customFormat="1" ht="28">
-      <c r="A52" s="20" t="s">
-        <v>385</v>
-      </c>
-      <c r="B52" s="38" t="s">
-        <v>460</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="E52" s="24" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" s="2" customFormat="1" ht="42">
-      <c r="C53" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="E53" s="43" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="E52" s="34"/>
+      <c r="F52" s="43" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="2" customFormat="1">
+      <c r="A53" s="20"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="E53" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="F53" s="24"/>
+    </row>
+    <row r="54" spans="1:11" s="2" customFormat="1" ht="42">
       <c r="A54" s="20" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>459</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>387</v>
-      </c>
-      <c r="D54" s="34"/>
-      <c r="E54" s="43" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" s="2" customFormat="1">
+        <v>304</v>
+      </c>
+      <c r="C54" s="38"/>
+      <c r="D54" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="F54" s="43" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="2" customFormat="1" ht="42">
       <c r="A55" s="20"/>
       <c r="B55" s="25"/>
-      <c r="C55" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="E55" s="24"/>
-    </row>
-    <row r="56" spans="1:10" s="2" customFormat="1" ht="42">
-      <c r="A56" s="20" t="s">
-        <v>384</v>
-      </c>
-      <c r="B56" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="E56" s="43" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="C55" s="25"/>
+      <c r="D55" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="E55" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="F55" s="24" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="2" customFormat="1" ht="42">
+      <c r="A56" s="20"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="25"/>
+      <c r="D56" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="F56" s="24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" s="2" customFormat="1" ht="28">
       <c r="A57" s="20"/>
       <c r="B57" s="25"/>
-      <c r="C57" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="D57" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="E57" s="24" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="C57" s="25"/>
+      <c r="D57" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="F57" s="24" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="2" customFormat="1" ht="56">
       <c r="A58" s="20"/>
       <c r="B58" s="25"/>
-      <c r="C58" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D58" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="E58" s="24" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="C58" s="25"/>
+      <c r="D58" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="F58" s="24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="2" customFormat="1" ht="28">
       <c r="A59" s="20"/>
       <c r="B59" s="25"/>
-      <c r="C59" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D59" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="E59" s="24" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" s="2" customFormat="1" ht="56">
+      <c r="C59" s="25"/>
+      <c r="D59" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="F59" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" s="2" customFormat="1" ht="38" customHeight="1">
       <c r="A60" s="20"/>
       <c r="B60" s="25"/>
-      <c r="C60" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D60" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="E60" s="24" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" ht="28">
-      <c r="A61" s="20"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="D61" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="E61" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" s="2" customFormat="1" ht="38" customHeight="1">
-      <c r="A62" s="20"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="24" t="s">
+      <c r="C60" s="25"/>
+      <c r="D60" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="D62" s="25" t="s">
+      <c r="E60" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="E62" s="24" t="s">
+      <c r="F60" s="24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
-      <c r="C63" s="26" t="s">
-        <v>491</v>
-      </c>
-      <c r="D63" s="27"/>
-      <c r="E63" s="42"/>
-    </row>
-    <row r="64" spans="1:10" ht="42">
-      <c r="A64" s="15" t="s">
+    <row r="61" spans="1:11">
+      <c r="D61" s="26" t="s">
+        <v>474</v>
+      </c>
+      <c r="E61" s="27"/>
+      <c r="F61" s="42"/>
+    </row>
+    <row r="62" spans="1:11" ht="42">
+      <c r="A62" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="B62" s="37" t="s">
+        <v>394</v>
+      </c>
+      <c r="C62" s="37"/>
+      <c r="D62" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="E62" s="21"/>
+      <c r="F62" s="24" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="2" customFormat="1" ht="42">
+      <c r="A63" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="38" t="s">
+        <v>395</v>
+      </c>
+      <c r="C63" s="38"/>
+      <c r="D63" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="E63" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="2" customFormat="1" ht="42">
+      <c r="A64" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" s="38" t="s">
+        <v>396</v>
+      </c>
+      <c r="C64" s="38"/>
+      <c r="D64" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E64" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A65" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="B65" s="38" t="s">
+        <v>397</v>
+      </c>
+      <c r="C65" s="38"/>
+      <c r="D65" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="E65" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A66" s="20" t="s">
+        <v>457</v>
+      </c>
+      <c r="B66" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="C66" s="38"/>
+      <c r="D66" s="24" t="s">
         <v>356</v>
       </c>
-      <c r="B64" s="37" t="s">
-        <v>404</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="D64" s="21"/>
-      <c r="E64" s="24" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A65" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B65" s="38" t="s">
-        <v>405</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>357</v>
-      </c>
-      <c r="D65" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="E65" s="24" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A66" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" s="38" t="s">
-        <v>406</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D66" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="E66" s="24" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="E66" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="F66" s="24" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="2" customFormat="1" ht="42">
       <c r="A67" s="20" t="s">
-        <v>196</v>
+        <v>359</v>
       </c>
       <c r="B67" s="38" t="s">
-        <v>407</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>358</v>
-      </c>
-      <c r="D67" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="E67" s="24" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="2" customFormat="1" ht="42">
+        <v>402</v>
+      </c>
+      <c r="C67" s="38"/>
+      <c r="D67" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E67" s="34"/>
+      <c r="F67" s="24" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="2" customFormat="1" ht="42">
       <c r="A68" s="20" t="s">
-        <v>473</v>
+        <v>43</v>
       </c>
       <c r="B68" s="38" t="s">
-        <v>408</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>359</v>
-      </c>
-      <c r="D68" s="34" t="s">
-        <v>302</v>
-      </c>
-      <c r="E68" s="24" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A69" s="20" t="s">
-        <v>362</v>
-      </c>
-      <c r="B69" s="38" t="s">
-        <v>412</v>
-      </c>
-      <c r="C69" s="24" t="s">
-        <v>363</v>
-      </c>
-      <c r="D69" s="34"/>
-      <c r="E69" s="24" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A70" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="C68" s="38"/>
+      <c r="D68" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B70" s="38" t="s">
-        <v>413</v>
-      </c>
-      <c r="C70" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D70" s="34" t="s">
+      <c r="E68" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="E70" s="24" t="s">
+      <c r="F68" s="24" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="69" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A69" s="20"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E69" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A70" s="20"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E70" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="2" customFormat="1">
       <c r="A71" s="20"/>
       <c r="B71" s="25"/>
-      <c r="C71" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D71" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="E71" s="24" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A72" s="20"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D72" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="E72" s="24" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="2" customFormat="1">
+      <c r="C71" s="25"/>
+      <c r="D71" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="E71" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="F71" s="24"/>
+    </row>
+    <row r="72" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A72" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="B72" s="38" t="s">
+        <v>412</v>
+      </c>
+      <c r="C72" s="38"/>
+      <c r="D72" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E72" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="F72" s="24" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="2" customFormat="1" ht="56">
       <c r="A73" s="20"/>
       <c r="B73" s="25"/>
-      <c r="C73" s="24" t="s">
+      <c r="C73" s="25"/>
+      <c r="D73" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E73" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A74" s="20" t="s">
+        <v>455</v>
+      </c>
+      <c r="B74" s="38" t="s">
+        <v>409</v>
+      </c>
+      <c r="C74" s="38"/>
+      <c r="D74" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E74" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="2" customFormat="1" ht="56">
+      <c r="A75" s="20" t="s">
+        <v>456</v>
+      </c>
+      <c r="B75" s="38" t="s">
+        <v>410</v>
+      </c>
+      <c r="C75" s="38"/>
+      <c r="D75" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A76" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B76" s="38" t="s">
+        <v>401</v>
+      </c>
+      <c r="C76" s="38"/>
+      <c r="D76" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="E76" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A77" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B77" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="C77" s="38"/>
+      <c r="D77" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="E77" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="2" customFormat="1" ht="42">
+      <c r="A78" s="20"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="D73" s="34" t="s">
-        <v>311</v>
-      </c>
-      <c r="E73" s="24"/>
-    </row>
-    <row r="74" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A74" s="20" t="s">
-        <v>470</v>
-      </c>
-      <c r="B74" s="38" t="s">
-        <v>422</v>
-      </c>
-      <c r="C74" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D74" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="E74" s="24" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="2" customFormat="1" ht="56">
-      <c r="A75" s="20"/>
-      <c r="B75" s="25"/>
-      <c r="C75" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D75" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="E75" s="24" t="s">
+      <c r="E78" s="34" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A76" s="20" t="s">
-        <v>471</v>
-      </c>
-      <c r="B76" s="38" t="s">
-        <v>419</v>
-      </c>
-      <c r="C76" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D76" s="34" t="s">
-        <v>185</v>
-      </c>
-      <c r="E76" s="24" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="2" customFormat="1" ht="56">
-      <c r="A77" s="20" t="s">
-        <v>472</v>
-      </c>
-      <c r="B77" s="38" t="s">
-        <v>420</v>
-      </c>
-      <c r="C77" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D77" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="E77" s="24" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A78" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="B78" s="38" t="s">
-        <v>411</v>
-      </c>
-      <c r="C78" s="24" t="s">
-        <v>271</v>
-      </c>
-      <c r="D78" s="34" t="s">
-        <v>320</v>
-      </c>
-      <c r="E78" s="24" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="2" customFormat="1" ht="42">
+      <c r="F78" s="24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="2" customFormat="1" ht="42">
       <c r="A79" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B79" s="38" t="s">
-        <v>414</v>
-      </c>
-      <c r="C79" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="D79" s="34" t="s">
-        <v>307</v>
-      </c>
-      <c r="E79" s="24" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="2" customFormat="1" ht="42">
-      <c r="A80" s="20"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="C79" s="38"/>
+      <c r="D79" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="E79" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="42">
+      <c r="D80" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="E80" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="D80" s="34" t="s">
-        <v>308</v>
-      </c>
-      <c r="E80" s="24" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" s="2" customFormat="1" ht="42">
+      <c r="F80" s="24" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" s="2" customFormat="1" ht="42">
       <c r="A81" s="20" t="s">
         <v>274</v>
       </c>
       <c r="B81" s="38" t="s">
-        <v>415</v>
-      </c>
-      <c r="C81" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="D81" s="34" t="s">
-        <v>317</v>
-      </c>
-      <c r="E81" s="24" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="42">
-      <c r="C82" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>318</v>
-      </c>
-      <c r="E82" s="24" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" s="2" customFormat="1" ht="42">
+        <v>406</v>
+      </c>
+      <c r="C81" s="38"/>
+      <c r="D81" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="E81" s="34" t="s">
+        <v>306</v>
+      </c>
+      <c r="F81" s="24" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A82" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B82" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="C82" s="38"/>
+      <c r="D82" s="20" t="s">
+        <v>408</v>
+      </c>
+      <c r="E82" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="F82" s="24" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" s="2" customFormat="1" ht="42">
       <c r="A83" s="20" t="s">
         <v>276</v>
       </c>
       <c r="B83" s="38" t="s">
-        <v>416</v>
-      </c>
-      <c r="C83" s="20" t="s">
-        <v>364</v>
-      </c>
-      <c r="D83" s="34" t="s">
-        <v>309</v>
-      </c>
-      <c r="E83" s="24" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A84" s="20" t="s">
+        <v>411</v>
+      </c>
+      <c r="C83" s="38"/>
+      <c r="D83" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="E83" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="42">
+      <c r="A84" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B84" s="37" t="s">
+        <v>441</v>
+      </c>
+      <c r="C84" s="37"/>
+      <c r="D84" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="E84" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="F84" s="24" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="B85" s="37" t="s">
+        <v>430</v>
+      </c>
+      <c r="C85" s="37"/>
+      <c r="D85" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="E85" s="27"/>
+      <c r="F85" s="42"/>
+    </row>
+    <row r="86" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A86" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="B86" s="38" t="s">
+        <v>431</v>
+      </c>
+      <c r="C86" s="38"/>
+      <c r="D86" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="E86" s="34"/>
+      <c r="F86" s="24" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A87" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="B87" s="38" t="s">
+        <v>432</v>
+      </c>
+      <c r="C87" s="38"/>
+      <c r="D87" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="E87" s="34"/>
+      <c r="F87" s="24" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A88" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="B88" s="38" t="s">
+        <v>433</v>
+      </c>
+      <c r="C88" s="38"/>
+      <c r="D88" s="24" t="s">
+        <v>371</v>
+      </c>
+      <c r="E88" s="34"/>
+      <c r="F88" s="24" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="D89" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="E89" s="27"/>
+      <c r="F89" s="42"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10" ht="28">
+      <c r="A90" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="B90" s="37" t="s">
+        <v>392</v>
+      </c>
+      <c r="C90" s="37"/>
+      <c r="D90" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="F90" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A91" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="B84" s="38" t="s">
-        <v>417</v>
-      </c>
-      <c r="C84" s="20" t="s">
-        <v>418</v>
-      </c>
-      <c r="D84" s="34" t="s">
-        <v>310</v>
-      </c>
-      <c r="E84" s="24" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A85" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="B85" s="38" t="s">
-        <v>421</v>
-      </c>
-      <c r="C85" s="24" t="s">
-        <v>278</v>
-      </c>
-      <c r="D85" s="34" t="s">
+      <c r="B91" s="38" t="s">
+        <v>393</v>
+      </c>
+      <c r="C91" s="38"/>
+      <c r="D91" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="E91" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A92" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="B92" s="38" t="s">
+        <v>400</v>
+      </c>
+      <c r="C92" s="38"/>
+      <c r="D92" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="E92" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="D93" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E93" s="27"/>
+      <c r="F93" s="42"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="1:10" ht="28">
+      <c r="A94" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="B94" s="37" t="s">
+        <v>549</v>
+      </c>
+      <c r="C94" s="33" t="s">
+        <v>518</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="F94" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A95" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="E95" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F95" s="24" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="2" customFormat="1" ht="28">
+      <c r="A96" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="B96" s="38"/>
+      <c r="C96" s="38"/>
+      <c r="D96" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="E96" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="F96" s="24" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="97" spans="4:10">
+      <c r="D97" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="E97" s="27"/>
+      <c r="F97" s="42"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="4:10" ht="28">
+      <c r="D98" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="E98" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="E85" s="24" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="42">
-      <c r="A86" s="15" t="s">
-        <v>290</v>
-      </c>
-      <c r="B86" s="37" t="s">
-        <v>451</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="D86" s="17" t="s">
-        <v>335</v>
-      </c>
-      <c r="E86" s="24" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="B87" s="37" t="s">
-        <v>440</v>
-      </c>
-      <c r="C87" s="26" t="s">
-        <v>436</v>
-      </c>
-      <c r="D87" s="27"/>
-      <c r="E87" s="42"/>
-    </row>
-    <row r="88" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A88" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="B88" s="38" t="s">
-        <v>441</v>
-      </c>
-      <c r="C88" s="24" t="s">
-        <v>372</v>
-      </c>
-      <c r="D88" s="34"/>
-      <c r="E88" s="24" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A89" s="20" t="s">
-        <v>438</v>
-      </c>
-      <c r="B89" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="C89" s="24" t="s">
-        <v>373</v>
-      </c>
-      <c r="D89" s="34"/>
-      <c r="E89" s="24" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A90" s="20" t="s">
-        <v>439</v>
-      </c>
-      <c r="B90" s="38" t="s">
-        <v>443</v>
-      </c>
-      <c r="C90" s="24" t="s">
-        <v>374</v>
-      </c>
-      <c r="D90" s="34"/>
-      <c r="E90" s="24" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="C91" s="26" t="s">
-        <v>361</v>
-      </c>
-      <c r="D91" s="27"/>
-      <c r="E91" s="42"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="3"/>
-      <c r="H91" s="3"/>
-      <c r="I91" s="3"/>
-    </row>
-    <row r="92" spans="1:9" ht="28">
-      <c r="A92" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="B92" s="37" t="s">
-        <v>402</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>354</v>
-      </c>
-      <c r="E92" s="24" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" s="2" customFormat="1" ht="28">
-      <c r="A93" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="B93" s="38" t="s">
-        <v>403</v>
-      </c>
-      <c r="C93" s="24" t="s">
-        <v>352</v>
-      </c>
-      <c r="D93" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93" s="24" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" s="2" customFormat="1" ht="28">
-      <c r="A94" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="B94" s="38" t="s">
-        <v>410</v>
-      </c>
-      <c r="C94" s="24" t="s">
-        <v>360</v>
-      </c>
-      <c r="D94" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="E94" s="24" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
-      <c r="C95" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="D95" s="27"/>
-      <c r="E95" s="42"/>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
-    </row>
-    <row r="96" spans="1:9" ht="28">
-      <c r="C96" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D96" s="19" t="s">
-        <v>322</v>
-      </c>
-      <c r="E96" s="18" t="s">
-        <v>509</v>
-      </c>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="C97" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D97" s="27"/>
-      <c r="E97" s="42"/>
-    </row>
-    <row r="98" spans="1:9" s="2" customFormat="1">
-      <c r="A98" s="20" t="s">
-        <v>396</v>
-      </c>
-      <c r="B98" s="25" t="s">
-        <v>465</v>
-      </c>
-      <c r="C98" s="33" t="s">
-        <v>390</v>
-      </c>
-      <c r="D98" s="35"/>
-      <c r="E98" s="24"/>
-    </row>
-    <row r="99" spans="1:9" ht="42">
-      <c r="C99" s="18" t="s">
+      <c r="F98" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+    </row>
+    <row r="99" spans="4:10">
+      <c r="D99" s="26" t="s">
+        <v>550</v>
+      </c>
+      <c r="E99" s="27"/>
+      <c r="F99" s="42"/>
+    </row>
+    <row r="100" spans="4:10" ht="42">
+      <c r="D100" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D99" s="21" t="s">
+      <c r="E100" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="E99" s="18" t="s">
+      <c r="F100" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="42">
-      <c r="C100" s="24" t="s">
+    <row r="101" spans="4:10" ht="42">
+      <c r="D101" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D100" s="21" t="s">
+      <c r="E101" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="E100" s="18" t="s">
+      <c r="F101" s="18" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="42">
-      <c r="C101" s="24" t="s">
+    <row r="102" spans="4:10" ht="42">
+      <c r="D102" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D101" s="21" t="s">
+      <c r="E102" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E101" s="18" t="s">
+      <c r="F102" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-    </row>
-    <row r="102" spans="1:9" ht="42">
-      <c r="C102" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="D102" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="E102" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="F102" s="3"/>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
-    </row>
-    <row r="103" spans="1:9" ht="42">
-      <c r="C103" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D103" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="E103" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="F103" s="3"/>
+      <c r="J102" s="3"/>
+    </row>
+    <row r="103" spans="4:10" ht="42">
+      <c r="D103" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="E103" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="F103" s="18" t="s">
+        <v>197</v>
+      </c>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
-    </row>
-    <row r="104" spans="1:9" ht="56">
-      <c r="C104" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D104" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="E104" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="F104" s="3"/>
+      <c r="J103" s="3"/>
+    </row>
+    <row r="104" spans="4:10" ht="42">
+      <c r="D104" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E104" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="F104" s="18" t="s">
+        <v>218</v>
+      </c>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
-    </row>
-    <row r="105" spans="1:9" ht="42">
-      <c r="C105" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D105" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="E105" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="F105" s="3"/>
+      <c r="J104" s="3"/>
+    </row>
+    <row r="105" spans="4:10" ht="56">
+      <c r="D105" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E105" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="F105" s="18" t="s">
+        <v>219</v>
+      </c>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
-    </row>
-    <row r="106" spans="1:9">
-      <c r="C106" s="26" t="s">
+      <c r="J105" s="3"/>
+    </row>
+    <row r="106" spans="4:10" ht="42">
+      <c r="D106" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E106" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="F106" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+    </row>
+    <row r="107" spans="4:10">
+      <c r="D107" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="D106" s="27"/>
-      <c r="E106" s="42"/>
-    </row>
-    <row r="107" spans="1:9" ht="42">
-      <c r="C107" s="18" t="s">
+      <c r="E107" s="27"/>
+      <c r="F107" s="42"/>
+    </row>
+    <row r="108" spans="4:10" ht="42">
+      <c r="D108" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D107" s="21" t="s">
+      <c r="E108" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="E107" s="18" t="s">
+      <c r="F108" s="18" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="42">
-      <c r="C108" s="24" t="s">
+    <row r="109" spans="4:10" ht="42">
+      <c r="D109" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D108" s="21" t="s">
+      <c r="E109" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="E108" s="18" t="s">
+      <c r="F109" s="18" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="42">
-      <c r="C109" s="24" t="s">
+    <row r="110" spans="4:10" ht="42">
+      <c r="D110" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D109" s="21" t="s">
+      <c r="E110" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="E109" s="18" t="s">
+      <c r="F110" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="F109" s="3"/>
-      <c r="G109" s="3"/>
-      <c r="H109" s="3"/>
-      <c r="I109" s="3"/>
-    </row>
-    <row r="110" spans="1:9" ht="42">
-      <c r="C110" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="D110" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="E110" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="F110" s="3"/>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
-    </row>
-    <row r="111" spans="1:9" ht="42">
-      <c r="C111" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D111" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="E111" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="F111" s="3"/>
+      <c r="J110" s="3"/>
+    </row>
+    <row r="111" spans="4:10" ht="42">
+      <c r="D111" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="E111" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="F111" s="18" t="s">
+        <v>228</v>
+      </c>
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
-    </row>
-    <row r="112" spans="1:9" ht="42">
-      <c r="C112" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D112" s="21" t="s">
-        <v>232</v>
-      </c>
-      <c r="E112" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="F112" s="3"/>
+      <c r="J111" s="3"/>
+    </row>
+    <row r="112" spans="4:10" ht="42">
+      <c r="D112" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E112" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="F112" s="18" t="s">
+        <v>229</v>
+      </c>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
-    </row>
-    <row r="113" spans="1:9" ht="28">
-      <c r="C113" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D113" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="E113" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="F113" s="3"/>
+      <c r="J112" s="3"/>
+    </row>
+    <row r="113" spans="1:10" ht="42">
+      <c r="D113" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E113" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="F113" s="18" t="s">
+        <v>230</v>
+      </c>
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
-    </row>
-    <row r="114" spans="1:9">
-      <c r="C114" s="26" t="s">
+      <c r="J113" s="3"/>
+    </row>
+    <row r="114" spans="1:10" ht="28">
+      <c r="D114" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E114" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="F114" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="G114" s="3"/>
+      <c r="H114" s="3"/>
+      <c r="I114" s="3"/>
+      <c r="J114" s="3"/>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="D115" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="D114" s="27"/>
-      <c r="E114" s="42"/>
-    </row>
-    <row r="115" spans="1:9" ht="42">
-      <c r="C115" s="18" t="s">
+      <c r="E115" s="27"/>
+      <c r="F115" s="42"/>
+    </row>
+    <row r="116" spans="1:10" ht="42">
+      <c r="D116" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D115" s="21" t="s">
+      <c r="E116" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="E115" s="18" t="s">
+      <c r="F116" s="18" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="42">
-      <c r="C116" s="24" t="s">
+    <row r="117" spans="1:10" ht="42">
+      <c r="D117" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D116" s="21" t="s">
+      <c r="E117" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="E116" s="18" t="s">
+      <c r="F117" s="18" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="42">
-      <c r="C117" s="24" t="s">
+    <row r="118" spans="1:10" ht="42">
+      <c r="D118" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D117" s="21" t="s">
+      <c r="E118" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="E117" s="18" t="s">
+      <c r="F118" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="F117" s="3"/>
-      <c r="G117" s="3"/>
-      <c r="H117" s="3"/>
-      <c r="I117" s="3"/>
-    </row>
-    <row r="118" spans="1:9" ht="42">
-      <c r="C118" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="D118" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="E118" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="F118" s="3"/>
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
-    </row>
-    <row r="119" spans="1:9" ht="42">
-      <c r="C119" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D119" s="21" t="s">
-        <v>245</v>
-      </c>
-      <c r="E119" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="F119" s="3"/>
+      <c r="J118" s="3"/>
+    </row>
+    <row r="119" spans="1:10" ht="42">
+      <c r="D119" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="E119" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="F119" s="18" t="s">
+        <v>242</v>
+      </c>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
-    </row>
-    <row r="120" spans="1:9" ht="42">
-      <c r="C120" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D120" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="E120" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="F120" s="3"/>
+      <c r="J119" s="3"/>
+    </row>
+    <row r="120" spans="1:10" ht="42">
+      <c r="D120" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E120" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="F120" s="18" t="s">
+        <v>243</v>
+      </c>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
-    </row>
-    <row r="121" spans="1:9" ht="28">
-      <c r="C121" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D121" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="E121" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="F121" s="3"/>
+      <c r="J120" s="3"/>
+    </row>
+    <row r="121" spans="1:10" ht="42">
+      <c r="D121" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E121" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="F121" s="18" t="s">
+        <v>244</v>
+      </c>
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
-    </row>
-    <row r="122" spans="1:9">
-      <c r="B122" s="37" t="s">
-        <v>423</v>
-      </c>
-      <c r="C122" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="D122" s="27"/>
-      <c r="E122" s="42"/>
-      <c r="F122" s="3"/>
+      <c r="J121" s="3"/>
+    </row>
+    <row r="122" spans="1:10" ht="28">
+      <c r="D122" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E122" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="F122" s="18" t="s">
+        <v>247</v>
+      </c>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
-    </row>
-    <row r="123" spans="1:9" ht="42">
-      <c r="A123" s="15" t="s">
-        <v>365</v>
-      </c>
+      <c r="J122" s="3"/>
+    </row>
+    <row r="123" spans="1:10">
       <c r="B123" s="37" t="s">
-        <v>424</v>
-      </c>
-      <c r="C123" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="D123" s="21" t="s">
-        <v>511</v>
-      </c>
-      <c r="E123" s="18" t="s">
-        <v>510</v>
-      </c>
-      <c r="F123" s="3"/>
+        <v>413</v>
+      </c>
+      <c r="C123" s="37"/>
+      <c r="D123" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="E123" s="27"/>
+      <c r="F123" s="42"/>
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
-    </row>
-    <row r="124" spans="1:9" ht="42">
+      <c r="J123" s="3"/>
+    </row>
+    <row r="124" spans="1:10" ht="42">
       <c r="A124" s="15" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B124" s="37" t="s">
-        <v>425</v>
-      </c>
-      <c r="C124" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="D124" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="E124" s="18" t="s">
-        <v>512</v>
-      </c>
-      <c r="F124" s="3"/>
+        <v>414</v>
+      </c>
+      <c r="C124" s="37"/>
+      <c r="D124" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="E124" s="21" t="s">
+        <v>494</v>
+      </c>
+      <c r="F124" s="18" t="s">
+        <v>493</v>
+      </c>
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
-    </row>
-    <row r="125" spans="1:9" ht="42">
+      <c r="J124" s="3"/>
+    </row>
+    <row r="125" spans="1:10" ht="42">
       <c r="A125" s="15" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B125" s="37" t="s">
-        <v>426</v>
-      </c>
-      <c r="C125" s="18" t="s">
-        <v>370</v>
-      </c>
-      <c r="D125" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="C125" s="37"/>
+      <c r="D125" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="E125" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="E125" s="18" t="s">
-        <v>513</v>
-      </c>
-      <c r="F125" s="3"/>
+      <c r="F125" s="18" t="s">
+        <v>495</v>
+      </c>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
-    </row>
-    <row r="126" spans="1:9" ht="42">
+      <c r="J125" s="3"/>
+    </row>
+    <row r="126" spans="1:10" ht="42">
+      <c r="A126" s="15" t="s">
+        <v>365</v>
+      </c>
       <c r="B126" s="37" t="s">
-        <v>427</v>
-      </c>
-      <c r="C126" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D126" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="E126" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="F126" s="3"/>
+        <v>416</v>
+      </c>
+      <c r="C126" s="37"/>
+      <c r="D126" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="E126" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="F126" s="18" t="s">
+        <v>496</v>
+      </c>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
-    </row>
-    <row r="127" spans="1:9" ht="42">
-      <c r="A127" s="15" t="s">
-        <v>280</v>
-      </c>
+      <c r="J126" s="3"/>
+    </row>
+    <row r="127" spans="1:10" ht="42">
       <c r="B127" s="37" t="s">
-        <v>428</v>
-      </c>
-      <c r="C127" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="D127" s="19" t="s">
-        <v>328</v>
-      </c>
-      <c r="E127" s="18" t="s">
-        <v>515</v>
-      </c>
-      <c r="F127" s="3"/>
+        <v>417</v>
+      </c>
+      <c r="C127" s="37"/>
+      <c r="D127" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E127" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="F127" s="18" t="s">
+        <v>497</v>
+      </c>
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
-    </row>
-    <row r="128" spans="1:9" ht="42">
+      <c r="J127" s="3"/>
+    </row>
+    <row r="128" spans="1:10" ht="42">
       <c r="A128" s="15" t="s">
-        <v>139</v>
+        <v>278</v>
       </c>
       <c r="B128" s="37" t="s">
-        <v>429</v>
-      </c>
-      <c r="C128" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D128" s="19" t="s">
-        <v>331</v>
-      </c>
-      <c r="E128" s="18" t="s">
-        <v>516</v>
-      </c>
-      <c r="F128" s="3"/>
+        <v>418</v>
+      </c>
+      <c r="C128" s="37"/>
+      <c r="D128" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="E128" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="F128" s="18" t="s">
+        <v>498</v>
+      </c>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
-    </row>
-    <row r="129" spans="1:9" ht="42">
+      <c r="J128" s="3"/>
+    </row>
+    <row r="129" spans="1:10" ht="42">
       <c r="A129" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B129" s="37" t="s">
-        <v>430</v>
-      </c>
-      <c r="C129" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D129" s="19" t="s">
-        <v>332</v>
-      </c>
-      <c r="E129" s="18" t="s">
-        <v>517</v>
-      </c>
-      <c r="F129" s="3"/>
+        <v>419</v>
+      </c>
+      <c r="C129" s="37"/>
+      <c r="D129" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E129" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="F129" s="18" t="s">
+        <v>499</v>
+      </c>
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
-    </row>
-    <row r="130" spans="1:9" ht="42">
+      <c r="J129" s="3"/>
+    </row>
+    <row r="130" spans="1:10" ht="42">
       <c r="A130" s="15" t="s">
-        <v>371</v>
+        <v>140</v>
       </c>
       <c r="B130" s="37" t="s">
-        <v>431</v>
-      </c>
-      <c r="C130" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="D130" s="19" t="s">
+        <v>420</v>
+      </c>
+      <c r="C130" s="37"/>
+      <c r="D130" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="E130" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="E130" s="18" t="s">
-        <v>518</v>
-      </c>
-      <c r="F130" s="3"/>
+      <c r="F130" s="18" t="s">
+        <v>500</v>
+      </c>
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
-    </row>
-    <row r="131" spans="1:9" ht="42">
+      <c r="J130" s="3"/>
+    </row>
+    <row r="131" spans="1:10" ht="42">
       <c r="A131" s="15" t="s">
-        <v>281</v>
+        <v>368</v>
       </c>
       <c r="B131" s="37" t="s">
-        <v>432</v>
-      </c>
-      <c r="C131" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="D131" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="E131" s="18" t="s">
-        <v>519</v>
-      </c>
-      <c r="F131" s="3"/>
+        <v>421</v>
+      </c>
+      <c r="C131" s="37"/>
+      <c r="D131" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="E131" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="F131" s="18" t="s">
+        <v>501</v>
+      </c>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
-    </row>
-    <row r="132" spans="1:9">
-      <c r="C132" s="26" t="s">
-        <v>323</v>
-      </c>
-      <c r="D132" s="27"/>
-      <c r="E132" s="42"/>
-      <c r="F132" s="3"/>
+      <c r="J131" s="3"/>
+    </row>
+    <row r="132" spans="1:10" ht="42">
+      <c r="A132" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="B132" s="37" t="s">
+        <v>422</v>
+      </c>
+      <c r="C132" s="37"/>
+      <c r="D132" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="E132" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="F132" s="18" t="s">
+        <v>502</v>
+      </c>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
-    </row>
-    <row r="133" spans="1:9" s="2" customFormat="1" ht="42">
-      <c r="A133" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="B133" s="38" t="s">
-        <v>409</v>
-      </c>
-      <c r="C133" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="D133" s="34" t="s">
-        <v>324</v>
-      </c>
-      <c r="E133" s="24" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="56">
-      <c r="A134" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="B134" s="37" t="s">
-        <v>433</v>
-      </c>
-      <c r="C134" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="D134" s="16" t="s">
-        <v>325</v>
-      </c>
-      <c r="E134" s="24" t="s">
-        <v>521</v>
-      </c>
-      <c r="F134" s="3"/>
-      <c r="G134" s="3"/>
-      <c r="H134" s="3"/>
-      <c r="I134" s="3"/>
-    </row>
-    <row r="135" spans="1:9" ht="56">
+      <c r="J132" s="3"/>
+    </row>
+    <row r="133" spans="1:10">
+      <c r="D133" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="E133" s="27"/>
+      <c r="F133" s="42"/>
+      <c r="G133" s="3"/>
+      <c r="H133" s="3"/>
+      <c r="I133" s="3"/>
+      <c r="J133" s="3"/>
+    </row>
+    <row r="134" spans="1:10" s="2" customFormat="1" ht="42">
+      <c r="A134" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B134" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="C134" s="38"/>
+      <c r="D134" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="E134" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="F134" s="24" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="56">
       <c r="A135" s="15" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B135" s="37" t="s">
-        <v>434</v>
-      </c>
-      <c r="C135" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="D135" s="16" t="s">
-        <v>326</v>
-      </c>
-      <c r="E135" s="24" t="s">
-        <v>522</v>
-      </c>
-      <c r="F135" s="3"/>
+        <v>423</v>
+      </c>
+      <c r="C135" s="37"/>
+      <c r="D135" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="E135" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="F135" s="24" t="s">
+        <v>504</v>
+      </c>
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
-    </row>
-    <row r="136" spans="1:9" ht="56">
+      <c r="J135" s="3"/>
+    </row>
+    <row r="136" spans="1:10" ht="56">
       <c r="A136" s="15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B136" s="37" t="s">
-        <v>435</v>
-      </c>
-      <c r="C136" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="D136" s="16" t="s">
-        <v>327</v>
-      </c>
-      <c r="E136" s="24" t="s">
-        <v>523</v>
-      </c>
-      <c r="F136" s="3"/>
+        <v>424</v>
+      </c>
+      <c r="C136" s="37"/>
+      <c r="D136" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="E136" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="F136" s="24" t="s">
+        <v>505</v>
+      </c>
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
-    </row>
-    <row r="137" spans="1:9">
-      <c r="C137" s="26" t="s">
+      <c r="J136" s="3"/>
+    </row>
+    <row r="137" spans="1:10" ht="56">
+      <c r="A137" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="B137" s="37" t="s">
+        <v>425</v>
+      </c>
+      <c r="C137" s="37"/>
+      <c r="D137" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="E137" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="F137" s="24" t="s">
+        <v>506</v>
+      </c>
+      <c r="G137" s="3"/>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="3"/>
+    </row>
+    <row r="138" spans="1:10">
+      <c r="D138" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="E138" s="27"/>
+      <c r="F138" s="42"/>
+    </row>
+    <row r="139" spans="1:10" ht="36">
+      <c r="A139" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="D137" s="27"/>
-      <c r="E137" s="42"/>
-    </row>
-    <row r="138" spans="1:9" ht="36">
-      <c r="A138" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="B138" s="37" t="s">
-        <v>449</v>
-      </c>
-      <c r="C138" s="18" t="s">
-        <v>287</v>
-      </c>
-      <c r="D138" s="16" t="s">
-        <v>334</v>
-      </c>
-      <c r="E138" s="44" t="s">
-        <v>525</v>
-      </c>
-      <c r="F138" s="3"/>
-      <c r="G138" s="3"/>
-      <c r="H138" s="3"/>
-      <c r="I138" s="3"/>
-    </row>
-    <row r="139" spans="1:9" ht="36">
-      <c r="A139" s="15" t="s">
-        <v>389</v>
-      </c>
       <c r="B139" s="37" t="s">
-        <v>450</v>
-      </c>
-      <c r="C139" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="D139" s="16" t="s">
-        <v>333</v>
-      </c>
-      <c r="E139" s="44" t="s">
-        <v>524</v>
-      </c>
-      <c r="F139" s="3"/>
+        <v>439</v>
+      </c>
+      <c r="C139" s="37"/>
+      <c r="D139" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="E139" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="F139" s="44" t="s">
+        <v>508</v>
+      </c>
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
-    </row>
-    <row r="140" spans="1:9">
-      <c r="C140" s="26" t="s">
+      <c r="J139" s="3"/>
+    </row>
+    <row r="140" spans="1:10" ht="36">
+      <c r="A140" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B140" s="37" t="s">
+        <v>440</v>
+      </c>
+      <c r="C140" s="37"/>
+      <c r="D140" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="E140" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="F140" s="44" t="s">
+        <v>507</v>
+      </c>
+      <c r="G140" s="3"/>
+      <c r="H140" s="3"/>
+      <c r="I140" s="3"/>
+      <c r="J140" s="3"/>
+    </row>
+    <row r="141" spans="1:10">
+      <c r="D141" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="E141" s="27"/>
+      <c r="F141" s="42"/>
+    </row>
+    <row r="142" spans="1:10" ht="42">
+      <c r="A142" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="B142" s="41" t="s">
+        <v>458</v>
+      </c>
+      <c r="C142" s="41"/>
+      <c r="E142" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="F142" s="18" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="42">
+      <c r="A143" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="B143" s="41" t="s">
+        <v>459</v>
+      </c>
+      <c r="C143" s="41"/>
+      <c r="E143" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="F143" s="18" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="42">
+      <c r="A144" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="B144" s="41" t="s">
+        <v>449</v>
+      </c>
+      <c r="C144" s="41"/>
+      <c r="E144" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="F144" s="18" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="B145" s="37" t="s">
+        <v>453</v>
+      </c>
+      <c r="C145" s="37"/>
+      <c r="D145" s="26" t="s">
+        <v>560</v>
+      </c>
+      <c r="E145" s="27"/>
+      <c r="F145" s="42"/>
+    </row>
+    <row r="146" spans="1:6" ht="28">
+      <c r="A146" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="B146" s="37" t="s">
+        <v>450</v>
+      </c>
+      <c r="C146" s="37"/>
+      <c r="D146" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="E146" s="19"/>
+      <c r="F146" s="18" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="28">
+      <c r="A147" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B147" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="C147" s="37"/>
+      <c r="D147" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="E147" s="19"/>
+      <c r="F147" s="18" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="28">
+      <c r="A148" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="D140" s="27"/>
-      <c r="E140" s="42"/>
-    </row>
-    <row r="141" spans="1:9" ht="42">
-      <c r="A141" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="B141" s="41" t="s">
-        <v>475</v>
-      </c>
-      <c r="D141" s="23" t="s">
-        <v>320</v>
-      </c>
-      <c r="E141" s="18" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" ht="42">
-      <c r="A142" s="22" t="s">
-        <v>294</v>
-      </c>
-      <c r="B142" s="41" t="s">
-        <v>476</v>
-      </c>
-      <c r="D142" s="23" t="s">
-        <v>320</v>
-      </c>
-      <c r="E142" s="18" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" ht="42">
-      <c r="A143" s="22" t="s">
-        <v>295</v>
-      </c>
-      <c r="B143" s="41" t="s">
-        <v>462</v>
-      </c>
-      <c r="D143" s="23" t="s">
-        <v>320</v>
-      </c>
-      <c r="E143" s="18" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9">
-      <c r="B144" s="21" t="s">
-        <v>468</v>
-      </c>
-      <c r="C144" s="26" t="s">
-        <v>399</v>
-      </c>
-      <c r="D144" s="27"/>
-      <c r="E144" s="42"/>
-    </row>
-    <row r="145" spans="1:5">
-      <c r="A145" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="B145" s="21" t="s">
-        <v>463</v>
-      </c>
-      <c r="C145" s="18" t="s">
+      <c r="B148" s="37" t="s">
+        <v>535</v>
+      </c>
+      <c r="C148" s="18" t="s">
+        <v>533</v>
+      </c>
+      <c r="D148" s="18" t="s">
+        <v>534</v>
+      </c>
+      <c r="E148" s="19"/>
+      <c r="F148" s="18" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="28">
+      <c r="A149" s="15" t="s">
         <v>390</v>
       </c>
-      <c r="D145" s="19"/>
-      <c r="E145" s="18"/>
-    </row>
-    <row r="146" spans="1:5">
-      <c r="A146" s="15" t="s">
+      <c r="B149" s="37" t="s">
+        <v>540</v>
+      </c>
+      <c r="C149" s="18" t="s">
+        <v>520</v>
+      </c>
+      <c r="D149" s="18" t="s">
+        <v>532</v>
+      </c>
+      <c r="E149" s="19"/>
+      <c r="F149" s="18" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="42">
+      <c r="A150" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B150" s="37" t="s">
+        <v>541</v>
+      </c>
+      <c r="C150" s="18" t="s">
+        <v>536</v>
+      </c>
+      <c r="D150" s="18" t="s">
+        <v>539</v>
+      </c>
+      <c r="E150" s="19"/>
+      <c r="F150" s="18" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="28">
+      <c r="A151" s="22" t="s">
+        <v>524</v>
+      </c>
+      <c r="B151" s="41" t="s">
+        <v>551</v>
+      </c>
+      <c r="C151" s="18" t="s">
+        <v>537</v>
+      </c>
+      <c r="D151" s="18" t="s">
+        <v>538</v>
+      </c>
+      <c r="E151" s="23"/>
+      <c r="F151" s="18" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="B152" s="37" t="s">
+        <v>453</v>
+      </c>
+      <c r="C152" s="37"/>
+      <c r="D152" s="26" t="s">
+        <v>561</v>
+      </c>
+      <c r="E152" s="27"/>
+      <c r="F152" s="42"/>
+    </row>
+    <row r="153" spans="1:6" ht="28">
+      <c r="A153" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="B153" s="37" t="s">
+        <v>450</v>
+      </c>
+      <c r="C153" s="37"/>
+      <c r="D153" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="E153" s="19"/>
+      <c r="F153" s="18" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="28">
+      <c r="A154" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B146" s="21" t="s">
-        <v>464</v>
-      </c>
-      <c r="C146" s="18" t="s">
+      <c r="B154" s="37" t="s">
+        <v>451</v>
+      </c>
+      <c r="C154" s="37"/>
+      <c r="D154" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="E154" s="19"/>
+      <c r="F154" s="18" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="28">
+      <c r="A155" s="15" t="s">
+        <v>388</v>
+      </c>
+      <c r="B155" s="37" t="s">
+        <v>535</v>
+      </c>
+      <c r="C155" s="18" t="s">
+        <v>533</v>
+      </c>
+      <c r="D155" s="18" t="s">
+        <v>534</v>
+      </c>
+      <c r="E155" s="19"/>
+      <c r="F155" s="18" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="28">
+      <c r="A156" s="15" t="s">
         <v>390</v>
       </c>
-      <c r="D146" s="19"/>
-      <c r="E146" s="18"/>
-    </row>
-    <row r="147" spans="1:5">
-      <c r="A147" s="15" t="s">
-        <v>397</v>
-      </c>
-      <c r="B147" s="21" t="s">
-        <v>466</v>
-      </c>
-      <c r="C147" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="D147" s="19"/>
-      <c r="E147" s="18"/>
-    </row>
-    <row r="148" spans="1:5">
-      <c r="A148" s="15" t="s">
-        <v>398</v>
-      </c>
-      <c r="B148" s="21" t="s">
-        <v>467</v>
-      </c>
-      <c r="C148" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="D148" s="19"/>
-      <c r="E148" s="18"/>
-    </row>
-    <row r="149" spans="1:5">
-      <c r="A149" s="15" t="s">
-        <v>400</v>
-      </c>
-      <c r="B149" s="21" t="s">
-        <v>469</v>
-      </c>
-      <c r="C149" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="D149" s="19"/>
-      <c r="E149" s="18"/>
-    </row>
-    <row r="150" spans="1:5">
-      <c r="A150" s="22"/>
-      <c r="B150" s="23"/>
-      <c r="D150" s="23"/>
-      <c r="E150" s="18"/>
-    </row>
-    <row r="151" spans="1:5">
-      <c r="A151" s="22"/>
-      <c r="B151" s="23"/>
-      <c r="D151" s="23"/>
-      <c r="E151" s="18"/>
-    </row>
-    <row r="152" spans="1:5">
-      <c r="A152" s="22"/>
-      <c r="B152" s="23"/>
-      <c r="D152" s="23"/>
-      <c r="E152" s="18"/>
-    </row>
-    <row r="153" spans="1:5">
-      <c r="A153" s="22"/>
-      <c r="B153" s="23"/>
-      <c r="D153" s="23"/>
-      <c r="E153" s="18"/>
-    </row>
-    <row r="154" spans="1:5">
-      <c r="A154" s="22"/>
-      <c r="B154" s="23"/>
-      <c r="D154" s="23"/>
-      <c r="E154" s="18"/>
-    </row>
-    <row r="155" spans="1:5">
-      <c r="A155" s="22"/>
-      <c r="B155" s="23"/>
-      <c r="D155" s="23"/>
-      <c r="E155" s="18"/>
-    </row>
-    <row r="156" spans="1:5">
-      <c r="A156" s="22"/>
-      <c r="B156" s="23"/>
-      <c r="D156" s="23"/>
-      <c r="E156" s="18"/>
-    </row>
-    <row r="157" spans="1:5">
-      <c r="A157" s="22"/>
-      <c r="B157" s="23"/>
-      <c r="D157" s="23"/>
-      <c r="E157" s="18"/>
-    </row>
-    <row r="158" spans="1:5">
-      <c r="A158" s="22"/>
-      <c r="B158" s="23"/>
-      <c r="D158" s="23"/>
-      <c r="E158" s="18"/>
+      <c r="B156" s="37" t="s">
+        <v>540</v>
+      </c>
+      <c r="C156" s="18" t="s">
+        <v>520</v>
+      </c>
+      <c r="D156" s="18" t="s">
+        <v>532</v>
+      </c>
+      <c r="E156" s="19"/>
+      <c r="F156" s="18" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="42">
+      <c r="A157" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B157" s="37" t="s">
+        <v>541</v>
+      </c>
+      <c r="C157" s="18" t="s">
+        <v>536</v>
+      </c>
+      <c r="D157" s="18" t="s">
+        <v>539</v>
+      </c>
+      <c r="E157" s="19"/>
+      <c r="F157" s="18" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="28">
+      <c r="A158" s="22" t="s">
+        <v>524</v>
+      </c>
+      <c r="B158" s="41" t="s">
+        <v>551</v>
+      </c>
+      <c r="C158" s="18" t="s">
+        <v>537</v>
+      </c>
+      <c r="D158" s="18" t="s">
+        <v>538</v>
+      </c>
+      <c r="E158" s="23"/>
+      <c r="F158" s="18" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="28">
+      <c r="A159" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="B159" s="41" t="s">
+        <v>521</v>
+      </c>
+      <c r="C159" s="47" t="s">
+        <v>552</v>
+      </c>
+      <c r="D159" s="18" t="s">
+        <v>553</v>
+      </c>
+      <c r="E159" s="23"/>
+      <c r="F159" s="18" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="28">
+      <c r="A160" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="B160" s="37" t="s">
+        <v>452</v>
+      </c>
+      <c r="C160" s="18" t="s">
+        <v>519</v>
+      </c>
+      <c r="D160" s="18" t="s">
+        <v>531</v>
+      </c>
+      <c r="E160" s="19"/>
+      <c r="F160" s="18" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="22"/>
+      <c r="B161" s="23"/>
+      <c r="C161" s="23"/>
+      <c r="E161" s="23"/>
+      <c r="F161" s="18"/>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="22"/>
+      <c r="B162" s="23"/>
+      <c r="C162" s="23"/>
+      <c r="E162" s="23"/>
+      <c r="F162" s="18"/>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="22"/>
+      <c r="B163" s="23"/>
+      <c r="C163" s="23"/>
+      <c r="E163" s="23"/>
+      <c r="F163" s="18"/>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="22"/>
+      <c r="B164" s="23"/>
+      <c r="C164" s="23"/>
+      <c r="E164" s="23"/>
+      <c r="F164" s="18"/>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" s="22"/>
+      <c r="B165" s="23"/>
+      <c r="C165" s="23"/>
+      <c r="E165" s="23"/>
+      <c r="F165" s="18"/>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" s="22"/>
+      <c r="B166" s="23"/>
+      <c r="C166" s="23"/>
+      <c r="E166" s="23"/>
+      <c r="F166" s="18"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>

</xml_diff>

<commit_message>
Add "Prosecutor Detail Mapping" tab.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/ProsecutionCaseQueryResults.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/ProsecutionCaseQueryResults.xlsx
@@ -1,16 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haiqiwei/git/main-upgrade/shared/ojb-resources-common/src/main/resources/ssp/Prosecution_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7323CD00-6002-A04A-87D5-ACE60C6FCD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="2540" windowWidth="28560" windowHeight="13740"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId1"/>
     <sheet name="Court Case Filing Update" sheetId="2" r:id="rId2"/>
+    <sheet name="Prosecutor  Detail Mapping " sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="622">
   <si>
     <t>ATN [Arrest Tracking Number]</t>
   </si>
@@ -1750,13 +1757,154 @@
   </si>
   <si>
     <t>/pcq-res-doc:ProsecutionCaseQueryResults/pcq-res-ext:ProsecutionCase/nc:PrimaryDocument/pcq-res-ext:LeadDocumentIndicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DETAILS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case Number </t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Xpath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case Docket ID? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">? </t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disposition </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disposition Code Description? </t>
+  </si>
+  <si>
+    <t>Disposition Final Date/Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prosecutor </t>
+  </si>
+  <si>
+    <t>Ref Agency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referral Agency?  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refrerral Date </t>
+  </si>
+  <si>
+    <t>CLOSED</t>
+  </si>
+  <si>
+    <t>ANC</t>
+  </si>
+  <si>
+    <t>2018-03-14 15:40:00</t>
+  </si>
+  <si>
+    <t>HPD</t>
+  </si>
+  <si>
+    <t>2016-11-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage Code </t>
+  </si>
+  <si>
+    <t>Judgement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">571-11(2)(B) HRS - Behavior injurious to the welfare of a minor </t>
+  </si>
+  <si>
+    <t>S/C</t>
+  </si>
+  <si>
+    <t>Charge Description?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count </t>
+  </si>
+  <si>
+    <t>Dispostion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DWP BY Prosecutor </t>
+  </si>
+  <si>
+    <t>Disposition Date/Time</t>
+  </si>
+  <si>
+    <t>Disposition Datetime</t>
+  </si>
+  <si>
+    <t>Sentencing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">709-906(1)(9) HRS Abuse of family or household members </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPNCP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison/Jail </t>
+  </si>
+  <si>
+    <t>Amt</t>
+  </si>
+  <si>
+    <t>Loc</t>
+  </si>
+  <si>
+    <t>OCCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start datetime </t>
+  </si>
+  <si>
+    <t>End Datetime</t>
+  </si>
+  <si>
+    <t>2019-03-14 15:40:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration </t>
+  </si>
+  <si>
+    <t>1 year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent Event </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arraignment? </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="35" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1901,40 +2049,48 @@
       <b/>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1942,20 +2098,24 @@
       <sz val="10"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1970,10 +2130,17 @@
       <sz val="12"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2058,6 +2225,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2463,172 +2636,196 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="393">
-    <cellStyle name="Accent1 - 20%" xfId="3"/>
-    <cellStyle name="Accent1 - 40%" xfId="4"/>
-    <cellStyle name="Accent1 - 60%" xfId="5"/>
-    <cellStyle name="Accent2 - 20%" xfId="6"/>
-    <cellStyle name="Accent2 - 40%" xfId="7"/>
-    <cellStyle name="Accent2 - 60%" xfId="8"/>
-    <cellStyle name="Accent3 - 20%" xfId="9"/>
-    <cellStyle name="Accent3 - 40%" xfId="10"/>
-    <cellStyle name="Accent3 - 60%" xfId="11"/>
-    <cellStyle name="Accent4 - 20%" xfId="12"/>
-    <cellStyle name="Accent4 - 40%" xfId="13"/>
-    <cellStyle name="Accent4 - 60%" xfId="14"/>
-    <cellStyle name="Accent5 - 20%" xfId="15"/>
-    <cellStyle name="Accent5 - 40%" xfId="16"/>
-    <cellStyle name="Accent5 - 60%" xfId="17"/>
-    <cellStyle name="Accent6 - 20%" xfId="18"/>
-    <cellStyle name="Accent6 - 40%" xfId="19"/>
-    <cellStyle name="Accent6 - 60%" xfId="20"/>
-    <cellStyle name="Emphasis 1" xfId="21"/>
-    <cellStyle name="Emphasis 2" xfId="22"/>
-    <cellStyle name="Emphasis 3" xfId="23"/>
+    <cellStyle name="Accent1 - 20%" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent1 - 40%" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent1 - 60%" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent2 - 20%" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Accent2 - 40%" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Accent2 - 60%" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Accent3 - 20%" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Accent3 - 40%" xfId="10" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Accent3 - 60%" xfId="11" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Accent4 - 20%" xfId="12" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Accent4 - 40%" xfId="13" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Accent4 - 60%" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Accent5 - 20%" xfId="15" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Accent5 - 40%" xfId="16" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Accent5 - 60%" xfId="17" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Accent6 - 20%" xfId="18" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Accent6 - 40%" xfId="19" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Accent6 - 60%" xfId="20" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Emphasis 1" xfId="21" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Emphasis 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Emphasis 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
@@ -2996,17 +3193,20 @@
     <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 2" xfId="90"/>
-    <cellStyle name="Normal 3" xfId="24"/>
-    <cellStyle name="Normal 4" xfId="1"/>
-    <cellStyle name="Sheet Title" xfId="25"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000084010000}"/>
+    <cellStyle name="Normal 2 2" xfId="90" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="Normal 3" xfId="24" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="Sheet Title" xfId="25" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3298,14 +3498,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E159" sqref="E159"/>
+    <sheetView topLeftCell="B91" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" style="15" customWidth="1"/>
     <col min="2" max="3" width="21" style="21" customWidth="1"/>
@@ -3315,14 +3515,14 @@
     <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-    </row>
-    <row r="2" spans="1:6" ht="49" customHeight="1">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+    </row>
+    <row r="2" spans="1:6" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
         <v>525</v>
       </c>
@@ -3342,14 +3542,14 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="D3" s="30" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="18" t="s">
         <v>11</v>
       </c>
@@ -3360,7 +3560,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D5" s="18" t="s">
         <v>10</v>
       </c>
@@ -3371,7 +3571,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D6" s="18" t="s">
         <v>160</v>
       </c>
@@ -3382,7 +3582,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="D7" s="18" t="s">
         <v>13</v>
       </c>
@@ -3393,7 +3593,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D8" s="18" t="s">
         <v>135</v>
       </c>
@@ -3404,7 +3604,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>4</v>
       </c>
@@ -3418,7 +3618,7 @@
       <c r="E9" s="27"/>
       <c r="F9" s="42"/>
     </row>
-    <row r="10" spans="1:6" ht="28">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>372</v>
       </c>
@@ -3436,7 +3636,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>374</v>
       </c>
@@ -3454,7 +3654,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="42">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>32</v>
       </c>
@@ -3472,7 +3672,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="42">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>373</v>
       </c>
@@ -3490,7 +3690,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>375</v>
       </c>
@@ -3508,7 +3708,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="D15" s="18" t="s">
         <v>34</v>
       </c>
@@ -3519,7 +3719,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="D16" s="18" t="s">
         <v>35</v>
       </c>
@@ -3530,7 +3730,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="42">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="D17" s="18" t="s">
         <v>36</v>
       </c>
@@ -3541,7 +3741,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="98">
+    <row r="18" spans="1:6" ht="105" x14ac:dyDescent="0.2">
       <c r="D18" s="18" t="s">
         <v>37</v>
       </c>
@@ -3552,7 +3752,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
@@ -3566,14 +3766,14 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D20" s="26" t="s">
         <v>376</v>
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="42"/>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>377</v>
       </c>
@@ -3589,14 +3789,14 @@
         <v>463</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D22" s="26" t="s">
         <v>142</v>
       </c>
       <c r="E22" s="27"/>
       <c r="F22" s="42"/>
     </row>
-    <row r="23" spans="1:6" s="2" customFormat="1">
+    <row r="23" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36"/>
       <c r="B23" s="38" t="s">
         <v>547</v>
@@ -3612,7 +3812,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="2" customFormat="1">
+    <row r="24" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="36"/>
       <c r="B24" s="38" t="s">
         <v>445</v>
@@ -3626,7 +3826,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
@@ -3640,7 +3840,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="26" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="25"/>
       <c r="C26" s="25"/>
@@ -3654,14 +3854,14 @@
         <v>258</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D27" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="27"/>
       <c r="F27" s="42"/>
     </row>
-    <row r="28" spans="1:6" s="2" customFormat="1">
+    <row r="28" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
       <c r="B28" s="25"/>
       <c r="C28" s="25"/>
@@ -3675,7 +3875,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>267</v>
       </c>
@@ -3693,7 +3893,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="20"/>
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
@@ -3707,7 +3907,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="31" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="20"/>
       <c r="B31" s="25"/>
       <c r="C31" s="25"/>
@@ -3721,7 +3921,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="2" customFormat="1">
+    <row r="32" spans="1:6" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
         <v>293</v>
       </c>
@@ -3735,7 +3935,7 @@
       </c>
       <c r="F32" s="24"/>
     </row>
-    <row r="33" spans="1:6" s="2" customFormat="1">
+    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
         <v>385</v>
       </c>
@@ -3751,7 +3951,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="34" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
         <v>347</v>
       </c>
@@ -3769,7 +3969,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="35" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
         <v>266</v>
       </c>
@@ -3787,7 +3987,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="36" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
         <v>265</v>
       </c>
@@ -3805,7 +4005,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="37" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
         <v>340</v>
       </c>
@@ -3823,7 +4023,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="38" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
         <v>341</v>
       </c>
@@ -3841,7 +4041,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="2" customFormat="1">
+    <row r="39" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
         <v>342</v>
       </c>
@@ -3859,7 +4059,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="2" customFormat="1">
+    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
         <v>268</v>
       </c>
@@ -3877,7 +4077,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="2" customFormat="1">
+    <row r="41" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
         <v>343</v>
       </c>
@@ -3895,14 +4095,14 @@
         <v>468</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D42" s="26" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="27"/>
       <c r="F42" s="42"/>
     </row>
-    <row r="43" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="20"/>
       <c r="B43" s="25"/>
       <c r="C43" s="25"/>
@@ -3916,7 +4116,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="44" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
         <v>386</v>
       </c>
@@ -3934,7 +4134,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="42">
+    <row r="45" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>289</v>
       </c>
@@ -3952,7 +4152,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D46" s="18" t="s">
         <v>337</v>
       </c>
@@ -3960,7 +4160,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="42">
+    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>9</v>
       </c>
@@ -3978,7 +4178,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="2" customFormat="1" ht="28">
+    <row r="48" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="20"/>
       <c r="B48" s="25"/>
       <c r="C48" s="25"/>
@@ -3992,7 +4192,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="2" customFormat="1" ht="28">
+    <row r="49" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="20"/>
       <c r="B49" s="25"/>
       <c r="C49" s="25"/>
@@ -4006,7 +4206,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="2" customFormat="1" ht="28">
+    <row r="50" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
         <v>380</v>
       </c>
@@ -4024,7 +4224,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="2" customFormat="1" ht="42">
+    <row r="51" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="D51" s="24" t="s">
         <v>18</v>
       </c>
@@ -4035,7 +4235,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="2" customFormat="1" ht="42">
+    <row r="52" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
         <v>381</v>
       </c>
@@ -4051,7 +4251,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="2" customFormat="1">
+    <row r="53" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="20"/>
       <c r="B53" s="25"/>
       <c r="C53" s="25"/>
@@ -4063,7 +4263,7 @@
       </c>
       <c r="F53" s="24"/>
     </row>
-    <row r="54" spans="1:11" s="2" customFormat="1" ht="42">
+    <row r="54" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
         <v>379</v>
       </c>
@@ -4081,7 +4281,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="2" customFormat="1" ht="42">
+    <row r="55" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A55" s="20"/>
       <c r="B55" s="25"/>
       <c r="C55" s="25"/>
@@ -4095,7 +4295,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="2" customFormat="1" ht="42">
+    <row r="56" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A56" s="20"/>
       <c r="B56" s="25"/>
       <c r="C56" s="25"/>
@@ -4109,7 +4309,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="2" customFormat="1" ht="28">
+    <row r="57" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="20"/>
       <c r="B57" s="25"/>
       <c r="C57" s="25"/>
@@ -4123,7 +4323,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="2" customFormat="1" ht="56">
+    <row r="58" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A58" s="20"/>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
@@ -4137,7 +4337,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="2" customFormat="1" ht="28">
+    <row r="59" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="20"/>
       <c r="B59" s="25"/>
       <c r="C59" s="25"/>
@@ -4154,7 +4354,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="2" customFormat="1" ht="38" customHeight="1">
+    <row r="60" spans="1:11" s="2" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20"/>
       <c r="B60" s="25"/>
       <c r="C60" s="25"/>
@@ -4168,14 +4368,14 @@
         <v>248</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D61" s="26" t="s">
         <v>474</v>
       </c>
       <c r="E61" s="27"/>
       <c r="F61" s="42"/>
     </row>
-    <row r="62" spans="1:11" ht="42">
+    <row r="62" spans="1:11" ht="45" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
         <v>353</v>
       </c>
@@ -4191,7 +4391,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="2" customFormat="1" ht="42">
+    <row r="63" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
         <v>52</v>
       </c>
@@ -4209,7 +4409,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="2" customFormat="1" ht="42">
+    <row r="64" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
         <v>53</v>
       </c>
@@ -4227,7 +4427,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="65" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
         <v>196</v>
       </c>
@@ -4245,7 +4445,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="66" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
         <v>457</v>
       </c>
@@ -4263,7 +4463,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="67" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
         <v>359</v>
       </c>
@@ -4279,7 +4479,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="68" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
         <v>43</v>
       </c>
@@ -4297,7 +4497,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="69" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A69" s="20"/>
       <c r="B69" s="25"/>
       <c r="C69" s="25"/>
@@ -4311,7 +4511,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="70" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A70" s="20"/>
       <c r="B70" s="25"/>
       <c r="C70" s="25"/>
@@ -4325,7 +4525,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="2" customFormat="1">
+    <row r="71" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="20"/>
       <c r="B71" s="25"/>
       <c r="C71" s="25"/>
@@ -4337,7 +4537,7 @@
       </c>
       <c r="F71" s="24"/>
     </row>
-    <row r="72" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="72" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
         <v>454</v>
       </c>
@@ -4355,7 +4555,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="2" customFormat="1" ht="56">
+    <row r="73" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A73" s="20"/>
       <c r="B73" s="25"/>
       <c r="C73" s="25"/>
@@ -4369,7 +4569,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="74" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A74" s="20" t="s">
         <v>455</v>
       </c>
@@ -4387,7 +4587,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="2" customFormat="1" ht="56">
+    <row r="75" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
         <v>456</v>
       </c>
@@ -4405,7 +4605,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="76" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
         <v>269</v>
       </c>
@@ -4423,7 +4623,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="77" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="s">
         <v>271</v>
       </c>
@@ -4441,7 +4641,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="78" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A78" s="20"/>
       <c r="B78" s="25"/>
       <c r="C78" s="25"/>
@@ -4455,7 +4655,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="2" customFormat="1" ht="42">
+    <row r="79" spans="1:6" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A79" s="20" t="s">
         <v>272</v>
       </c>
@@ -4473,7 +4673,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="42">
+    <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="D80" s="18" t="s">
         <v>313</v>
       </c>
@@ -4484,7 +4684,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="2" customFormat="1" ht="42">
+    <row r="81" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A81" s="20" t="s">
         <v>274</v>
       </c>
@@ -4502,7 +4702,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="2" customFormat="1" ht="42">
+    <row r="82" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A82" s="20" t="s">
         <v>275</v>
       </c>
@@ -4520,7 +4720,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="2" customFormat="1" ht="42">
+    <row r="83" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A83" s="20" t="s">
         <v>276</v>
       </c>
@@ -4538,7 +4738,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="42">
+    <row r="84" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
         <v>288</v>
       </c>
@@ -4556,7 +4756,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B85" s="37" t="s">
         <v>430</v>
       </c>
@@ -4567,7 +4767,7 @@
       <c r="E85" s="27"/>
       <c r="F85" s="42"/>
     </row>
-    <row r="86" spans="1:10" s="2" customFormat="1" ht="42">
+    <row r="86" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A86" s="20" t="s">
         <v>427</v>
       </c>
@@ -4583,7 +4783,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="87" spans="1:10" s="2" customFormat="1" ht="42">
+    <row r="87" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A87" s="20" t="s">
         <v>428</v>
       </c>
@@ -4599,7 +4799,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="88" spans="1:10" s="2" customFormat="1" ht="42">
+    <row r="88" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A88" s="20" t="s">
         <v>429</v>
       </c>
@@ -4615,7 +4815,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D89" s="26" t="s">
         <v>358</v>
       </c>
@@ -4626,7 +4826,7 @@
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
     </row>
-    <row r="90" spans="1:10" ht="28">
+    <row r="90" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
         <v>350</v>
       </c>
@@ -4641,7 +4841,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="91" spans="1:10" s="2" customFormat="1" ht="28">
+    <row r="91" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A91" s="20" t="s">
         <v>277</v>
       </c>
@@ -4659,7 +4859,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="2" customFormat="1" ht="28">
+    <row r="92" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A92" s="20" t="s">
         <v>270</v>
       </c>
@@ -4677,7 +4877,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D93" s="26" t="s">
         <v>31</v>
       </c>
@@ -4688,7 +4888,7 @@
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
     </row>
-    <row r="94" spans="1:10" ht="28">
+    <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
         <v>350</v>
       </c>
@@ -4705,7 +4905,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="95" spans="1:10" s="2" customFormat="1" ht="28">
+    <row r="95" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A95" s="20" t="s">
         <v>277</v>
       </c>
@@ -4721,7 +4921,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="2" customFormat="1" ht="28">
+    <row r="96" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
         <v>270</v>
       </c>
@@ -4737,7 +4937,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="97" spans="4:10">
+    <row r="97" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D97" s="26" t="s">
         <v>318</v>
       </c>
@@ -4748,7 +4948,7 @@
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
     </row>
-    <row r="98" spans="4:10" ht="28">
+    <row r="98" spans="4:10" ht="30" x14ac:dyDescent="0.2">
       <c r="D98" s="18" t="s">
         <v>137</v>
       </c>
@@ -4763,14 +4963,14 @@
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
     </row>
-    <row r="99" spans="4:10">
+    <row r="99" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D99" s="26" t="s">
         <v>550</v>
       </c>
       <c r="E99" s="27"/>
       <c r="F99" s="42"/>
     </row>
-    <row r="100" spans="4:10" ht="42">
+    <row r="100" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D100" s="18" t="s">
         <v>69</v>
       </c>
@@ -4781,7 +4981,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="101" spans="4:10" ht="42">
+    <row r="101" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D101" s="24" t="s">
         <v>52</v>
       </c>
@@ -4792,7 +4992,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="102" spans="4:10" ht="42">
+    <row r="102" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D102" s="24" t="s">
         <v>53</v>
       </c>
@@ -4807,7 +5007,7 @@
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
     </row>
-    <row r="103" spans="4:10" ht="42">
+    <row r="103" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D103" s="24" t="s">
         <v>196</v>
       </c>
@@ -4822,7 +5022,7 @@
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
     </row>
-    <row r="104" spans="4:10" ht="42">
+    <row r="104" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D104" s="18" t="s">
         <v>58</v>
       </c>
@@ -4837,7 +5037,7 @@
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
     </row>
-    <row r="105" spans="4:10" ht="56">
+    <row r="105" spans="4:10" ht="60" x14ac:dyDescent="0.2">
       <c r="D105" s="18" t="s">
         <v>59</v>
       </c>
@@ -4852,7 +5052,7 @@
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
     </row>
-    <row r="106" spans="4:10" ht="42">
+    <row r="106" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D106" s="18" t="s">
         <v>60</v>
       </c>
@@ -4867,14 +5067,14 @@
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
     </row>
-    <row r="107" spans="4:10">
+    <row r="107" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D107" s="26" t="s">
         <v>221</v>
       </c>
       <c r="E107" s="27"/>
       <c r="F107" s="42"/>
     </row>
-    <row r="108" spans="4:10" ht="42">
+    <row r="108" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D108" s="18" t="s">
         <v>69</v>
       </c>
@@ -4885,7 +5085,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="109" spans="4:10" ht="42">
+    <row r="109" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D109" s="24" t="s">
         <v>52</v>
       </c>
@@ -4896,7 +5096,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="110" spans="4:10" ht="42">
+    <row r="110" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D110" s="24" t="s">
         <v>53</v>
       </c>
@@ -4911,7 +5111,7 @@
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
     </row>
-    <row r="111" spans="4:10" ht="42">
+    <row r="111" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D111" s="24" t="s">
         <v>196</v>
       </c>
@@ -4926,7 +5126,7 @@
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
     </row>
-    <row r="112" spans="4:10" ht="42">
+    <row r="112" spans="4:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D112" s="18" t="s">
         <v>58</v>
       </c>
@@ -4941,7 +5141,7 @@
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
     </row>
-    <row r="113" spans="1:10" ht="42">
+    <row r="113" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D113" s="18" t="s">
         <v>59</v>
       </c>
@@ -4956,7 +5156,7 @@
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
     </row>
-    <row r="114" spans="1:10" ht="28">
+    <row r="114" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="D114" s="18" t="s">
         <v>60</v>
       </c>
@@ -4971,14 +5171,14 @@
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D115" s="26" t="s">
         <v>235</v>
       </c>
       <c r="E115" s="27"/>
       <c r="F115" s="42"/>
     </row>
-    <row r="116" spans="1:10" ht="42">
+    <row r="116" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D116" s="18" t="s">
         <v>69</v>
       </c>
@@ -4989,7 +5189,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="42">
+    <row r="117" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D117" s="24" t="s">
         <v>52</v>
       </c>
@@ -5000,7 +5200,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="42">
+    <row r="118" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D118" s="24" t="s">
         <v>53</v>
       </c>
@@ -5015,7 +5215,7 @@
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
     </row>
-    <row r="119" spans="1:10" ht="42">
+    <row r="119" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D119" s="24" t="s">
         <v>196</v>
       </c>
@@ -5030,7 +5230,7 @@
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
     </row>
-    <row r="120" spans="1:10" ht="42">
+    <row r="120" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D120" s="18" t="s">
         <v>58</v>
       </c>
@@ -5045,7 +5245,7 @@
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
     </row>
-    <row r="121" spans="1:10" ht="42">
+    <row r="121" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="D121" s="18" t="s">
         <v>59</v>
       </c>
@@ -5060,7 +5260,7 @@
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
     </row>
-    <row r="122" spans="1:10" ht="28">
+    <row r="122" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="D122" s="18" t="s">
         <v>60</v>
       </c>
@@ -5075,7 +5275,7 @@
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B123" s="37" t="s">
         <v>413</v>
       </c>
@@ -5090,7 +5290,7 @@
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
     </row>
-    <row r="124" spans="1:10" ht="42">
+    <row r="124" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A124" s="15" t="s">
         <v>362</v>
       </c>
@@ -5112,7 +5312,7 @@
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
     </row>
-    <row r="125" spans="1:10" ht="42">
+    <row r="125" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A125" s="15" t="s">
         <v>364</v>
       </c>
@@ -5134,7 +5334,7 @@
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
     </row>
-    <row r="126" spans="1:10" ht="42">
+    <row r="126" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A126" s="15" t="s">
         <v>365</v>
       </c>
@@ -5156,7 +5356,7 @@
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
     </row>
-    <row r="127" spans="1:10" ht="42">
+    <row r="127" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B127" s="37" t="s">
         <v>417</v>
       </c>
@@ -5175,7 +5375,7 @@
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
     </row>
-    <row r="128" spans="1:10" ht="42">
+    <row r="128" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A128" s="15" t="s">
         <v>278</v>
       </c>
@@ -5197,7 +5397,7 @@
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
     </row>
-    <row r="129" spans="1:10" ht="42">
+    <row r="129" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A129" s="15" t="s">
         <v>139</v>
       </c>
@@ -5219,7 +5419,7 @@
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
     </row>
-    <row r="130" spans="1:10" ht="42">
+    <row r="130" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A130" s="15" t="s">
         <v>140</v>
       </c>
@@ -5241,7 +5441,7 @@
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
     </row>
-    <row r="131" spans="1:10" ht="42">
+    <row r="131" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A131" s="15" t="s">
         <v>368</v>
       </c>
@@ -5263,7 +5463,7 @@
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
     </row>
-    <row r="132" spans="1:10" ht="42">
+    <row r="132" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A132" s="15" t="s">
         <v>279</v>
       </c>
@@ -5285,7 +5485,7 @@
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D133" s="26" t="s">
         <v>320</v>
       </c>
@@ -5296,7 +5496,7 @@
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
     </row>
-    <row r="134" spans="1:10" s="2" customFormat="1" ht="42">
+    <row r="134" spans="1:10" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A134" s="20" t="s">
         <v>273</v>
       </c>
@@ -5314,7 +5514,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="56">
+    <row r="135" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A135" s="15" t="s">
         <v>280</v>
       </c>
@@ -5336,7 +5536,7 @@
       <c r="I135" s="3"/>
       <c r="J135" s="3"/>
     </row>
-    <row r="136" spans="1:10" ht="56">
+    <row r="136" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A136" s="15" t="s">
         <v>281</v>
       </c>
@@ -5358,7 +5558,7 @@
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
     </row>
-    <row r="137" spans="1:10" ht="56">
+    <row r="137" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A137" s="15" t="s">
         <v>282</v>
       </c>
@@ -5380,14 +5580,14 @@
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D138" s="26" t="s">
         <v>284</v>
       </c>
       <c r="E138" s="27"/>
       <c r="F138" s="42"/>
     </row>
-    <row r="139" spans="1:10" ht="36">
+    <row r="139" spans="1:10" ht="39" x14ac:dyDescent="0.2">
       <c r="A139" s="15" t="s">
         <v>286</v>
       </c>
@@ -5409,7 +5609,7 @@
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
     </row>
-    <row r="140" spans="1:10" ht="36">
+    <row r="140" spans="1:10" ht="39" x14ac:dyDescent="0.2">
       <c r="A140" s="15" t="s">
         <v>384</v>
       </c>
@@ -5431,14 +5631,14 @@
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D141" s="26" t="s">
         <v>383</v>
       </c>
       <c r="E141" s="27"/>
       <c r="F141" s="42"/>
     </row>
-    <row r="142" spans="1:10" ht="42">
+    <row r="142" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A142" s="22" t="s">
         <v>290</v>
       </c>
@@ -5453,7 +5653,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="42">
+    <row r="143" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A143" s="22" t="s">
         <v>291</v>
       </c>
@@ -5468,7 +5668,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="42">
+    <row r="144" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A144" s="22" t="s">
         <v>292</v>
       </c>
@@ -5483,7 +5683,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B145" s="37" t="s">
         <v>453</v>
       </c>
@@ -5494,7 +5694,7 @@
       <c r="E145" s="27"/>
       <c r="F145" s="42"/>
     </row>
-    <row r="146" spans="1:6" ht="28">
+    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A146" s="15" t="s">
         <v>387</v>
       </c>
@@ -5510,7 +5710,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="28">
+    <row r="147" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A147" s="15" t="s">
         <v>2</v>
       </c>
@@ -5526,7 +5726,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="28">
+    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A148" s="15" t="s">
         <v>388</v>
       </c>
@@ -5544,7 +5744,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="28">
+    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A149" s="15" t="s">
         <v>390</v>
       </c>
@@ -5562,7 +5762,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="42">
+    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A150" s="15" t="s">
         <v>523</v>
       </c>
@@ -5580,7 +5780,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="28">
+    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A151" s="22" t="s">
         <v>524</v>
       </c>
@@ -5598,7 +5798,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B152" s="37" t="s">
         <v>453</v>
       </c>
@@ -5609,7 +5809,7 @@
       <c r="E152" s="27"/>
       <c r="F152" s="42"/>
     </row>
-    <row r="153" spans="1:6" ht="28">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="15" t="s">
         <v>387</v>
       </c>
@@ -5625,7 +5825,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="28">
+    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A154" s="15" t="s">
         <v>2</v>
       </c>
@@ -5641,7 +5841,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="28">
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A155" s="15" t="s">
         <v>388</v>
       </c>
@@ -5659,7 +5859,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="28">
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A156" s="15" t="s">
         <v>390</v>
       </c>
@@ -5677,7 +5877,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="42">
+    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A157" s="15" t="s">
         <v>523</v>
       </c>
@@ -5695,7 +5895,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="28">
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A158" s="22" t="s">
         <v>524</v>
       </c>
@@ -5713,14 +5913,14 @@
         <v>574</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="28">
+    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A159" s="22" t="s">
         <v>522</v>
       </c>
       <c r="B159" s="41" t="s">
         <v>521</v>
       </c>
-      <c r="C159" s="47" t="s">
+      <c r="C159" s="45" t="s">
         <v>552</v>
       </c>
       <c r="D159" s="18" t="s">
@@ -5731,7 +5931,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="28">
+    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A160" s="15" t="s">
         <v>389</v>
       </c>
@@ -5749,42 +5949,42 @@
         <v>571</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="22"/>
       <c r="B161" s="23"/>
       <c r="C161" s="23"/>
       <c r="E161" s="23"/>
       <c r="F161" s="18"/>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="22"/>
       <c r="B162" s="23"/>
       <c r="C162" s="23"/>
       <c r="E162" s="23"/>
       <c r="F162" s="18"/>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="22"/>
       <c r="B163" s="23"/>
       <c r="C163" s="23"/>
       <c r="E163" s="23"/>
       <c r="F163" s="18"/>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="22"/>
       <c r="B164" s="23"/>
       <c r="C164" s="23"/>
       <c r="E164" s="23"/>
       <c r="F164" s="18"/>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="22"/>
       <c r="B165" s="23"/>
       <c r="C165" s="23"/>
       <c r="E165" s="23"/>
       <c r="F165" s="18"/>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="22"/>
       <c r="B166" s="23"/>
       <c r="C166" s="23"/>
@@ -5806,14 +6006,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.5" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" style="1" customWidth="1"/>
@@ -5821,7 +6021,7 @@
     <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
@@ -5832,14 +6032,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="12" customHeight="1">
+    <row r="3" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -5848,7 +6048,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12" customHeight="1">
+    <row r="4" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -5857,7 +6057,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12" customHeight="1">
+    <row r="5" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -5866,7 +6066,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12" customHeight="1">
+    <row r="6" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -5875,7 +6075,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="12" customHeight="1">
+    <row r="7" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -5884,14 +6084,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3" ht="12" customHeight="1">
+    <row r="9" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
@@ -5900,7 +6100,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="12" customHeight="1">
+    <row r="10" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
@@ -5909,7 +6109,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="12" customHeight="1">
+    <row r="11" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -5918,7 +6118,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="12" customHeight="1">
+    <row r="12" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>35</v>
       </c>
@@ -5927,7 +6127,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="12" customHeight="1">
+    <row r="13" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
@@ -5936,7 +6136,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="12" customHeight="1">
+    <row r="14" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
@@ -5945,7 +6145,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="15" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>0</v>
       </c>
@@ -5954,14 +6154,14 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="17" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>3</v>
       </c>
@@ -5970,7 +6170,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="18" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>27</v>
       </c>
@@ -5979,7 +6179,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="19" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>26</v>
       </c>
@@ -5988,7 +6188,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="20" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>28</v>
       </c>
@@ -5997,7 +6197,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="21" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>29</v>
       </c>
@@ -6006,7 +6206,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="22" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>30</v>
       </c>
@@ -6015,7 +6215,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="23" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>31</v>
       </c>
@@ -6024,7 +6224,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="24" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>64</v>
       </c>
@@ -6033,7 +6233,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="25" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>61</v>
       </c>
@@ -6042,7 +6242,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="26" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>62</v>
       </c>
@@ -6051,7 +6251,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="27" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>63</v>
       </c>
@@ -6060,7 +6260,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="28" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>65</v>
       </c>
@@ -6069,7 +6269,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="29" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>66</v>
       </c>
@@ -6078,7 +6278,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="30" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>67</v>
       </c>
@@ -6087,7 +6287,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="31" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>68</v>
       </c>
@@ -6096,14 +6296,14 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="9"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="33" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>14</v>
       </c>
@@ -6112,7 +6312,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="34" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>15</v>
       </c>
@@ -6121,7 +6321,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="35" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>16</v>
       </c>
@@ -6130,7 +6330,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="36" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>17</v>
       </c>
@@ -6139,7 +6339,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="37" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>18</v>
       </c>
@@ -6148,7 +6348,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="38" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>22</v>
       </c>
@@ -6157,7 +6357,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="39" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>19</v>
       </c>
@@ -6166,7 +6366,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="40" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>23</v>
       </c>
@@ -6175,7 +6375,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="41" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>24</v>
       </c>
@@ -6184,7 +6384,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="42" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>25</v>
       </c>
@@ -6193,14 +6393,14 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="9"/>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="44" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>38</v>
       </c>
@@ -6209,7 +6409,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="45" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>39</v>
       </c>
@@ -6218,7 +6418,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="46" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>40</v>
       </c>
@@ -6227,7 +6427,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="47" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A47" s="12" t="s">
         <v>41</v>
       </c>
@@ -6236,7 +6436,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="48" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>42</v>
       </c>
@@ -6245,7 +6445,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="49" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A49" s="12" t="s">
         <v>43</v>
       </c>
@@ -6254,7 +6454,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="50" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>44</v>
       </c>
@@ -6263,7 +6463,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="51" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A51" s="12" t="s">
         <v>45</v>
       </c>
@@ -6272,7 +6472,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="52" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A52" s="12" t="s">
         <v>48</v>
       </c>
@@ -6281,7 +6481,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="53" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>46</v>
       </c>
@@ -6290,7 +6490,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="54" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>47</v>
       </c>
@@ -6299,7 +6499,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="55" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>49</v>
       </c>
@@ -6308,7 +6508,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="56" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
         <v>50</v>
       </c>
@@ -6317,7 +6517,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="57" spans="1:3" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>51</v>
       </c>
@@ -6326,7 +6526,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>7</v>
       </c>
@@ -6335,7 +6535,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="12" customHeight="1">
+    <row r="59" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>69</v>
       </c>
@@ -6344,7 +6544,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="12" customHeight="1">
+    <row r="60" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
         <v>52</v>
       </c>
@@ -6353,7 +6553,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="12" customHeight="1">
+    <row r="61" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="12" t="s">
         <v>53</v>
       </c>
@@ -6362,7 +6562,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="12" customHeight="1">
+    <row r="62" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
         <v>54</v>
       </c>
@@ -6371,7 +6571,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="12" customHeight="1">
+    <row r="63" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
         <v>55</v>
       </c>
@@ -6380,7 +6580,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="12" customHeight="1">
+    <row r="64" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
         <v>56</v>
       </c>
@@ -6389,7 +6589,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
         <v>8</v>
       </c>
@@ -6398,7 +6598,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="12" customHeight="1">
+    <row r="66" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
         <v>57</v>
       </c>
@@ -6406,7 +6606,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="12" customHeight="1">
+    <row r="67" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
         <v>58</v>
       </c>
@@ -6414,7 +6614,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="12" customHeight="1">
+    <row r="68" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
         <v>59</v>
       </c>
@@ -6422,7 +6622,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="12" customHeight="1">
+    <row r="69" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
         <v>60</v>
       </c>
@@ -6430,51 +6630,51 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="10"/>
       <c r="C70" s="3"/>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="10"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="10"/>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="10"/>
       <c r="C73" s="3"/>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="10"/>
       <c r="C74" s="3"/>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C75" s="3"/>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C76" s="3"/>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C79" s="3"/>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C80" s="3"/>
     </row>
-    <row r="81" spans="3:3" s="1" customFormat="1">
+    <row r="81" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="3:3" s="1" customFormat="1">
+    <row r="82" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C82" s="3"/>
     </row>
-    <row r="83" spans="3:3" s="1" customFormat="1">
+    <row r="83" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C83" s="3"/>
     </row>
   </sheetData>
@@ -6485,4 +6685,603 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0D0565-A6AF-354A-8516-EA2DC08FED23}">
+  <dimension ref="A1:Q28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:M27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+    </row>
+    <row r="2" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>577</v>
+      </c>
+      <c r="B3" t="s">
+        <v>580</v>
+      </c>
+      <c r="C3" s="51">
+        <v>3159</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>581</v>
+      </c>
+      <c r="B4" t="s">
+        <v>582</v>
+      </c>
+      <c r="C4" t="s">
+        <v>591</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>583</v>
+      </c>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>584</v>
+      </c>
+      <c r="B5" t="s">
+        <v>585</v>
+      </c>
+      <c r="C5" t="s">
+        <v>592</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>583</v>
+      </c>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>586</v>
+      </c>
+      <c r="B6" t="s">
+        <v>583</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>593</v>
+      </c>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>587</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>588</v>
+      </c>
+      <c r="B8" t="s">
+        <v>589</v>
+      </c>
+      <c r="C8" t="s">
+        <v>594</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>583</v>
+      </c>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>590</v>
+      </c>
+      <c r="B9" t="s">
+        <v>590</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>595</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>583</v>
+      </c>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>596</v>
+      </c>
+      <c r="B10" t="s">
+        <v>583</v>
+      </c>
+      <c r="C10" t="s">
+        <v>583</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>583</v>
+      </c>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+    </row>
+    <row r="12" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
+        <v>597</v>
+      </c>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="53"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>598</v>
+      </c>
+      <c r="B13" t="s">
+        <v>601</v>
+      </c>
+      <c r="C13" t="s">
+        <v>599</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>470</v>
+      </c>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>600</v>
+      </c>
+      <c r="B14" t="s">
+        <v>583</v>
+      </c>
+      <c r="C14" t="s">
+        <v>583</v>
+      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>602</v>
+      </c>
+      <c r="B15" t="s">
+        <v>335</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>469</v>
+      </c>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>603</v>
+      </c>
+      <c r="B16" t="s">
+        <v>582</v>
+      </c>
+      <c r="C16" t="s">
+        <v>604</v>
+      </c>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>605</v>
+      </c>
+      <c r="B17" t="s">
+        <v>606</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>593</v>
+      </c>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+    </row>
+    <row r="19" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="53" t="s">
+        <v>607</v>
+      </c>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="53"/>
+    </row>
+    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>597</v>
+      </c>
+      <c r="B20" t="s">
+        <v>582</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>608</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>583</v>
+      </c>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>584</v>
+      </c>
+      <c r="B21" t="s">
+        <v>582</v>
+      </c>
+      <c r="C21" t="s">
+        <v>609</v>
+      </c>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>610</v>
+      </c>
+      <c r="B22" t="s">
+        <v>582</v>
+      </c>
+      <c r="C22" t="s">
+        <v>611</v>
+      </c>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>612</v>
+      </c>
+      <c r="B23" t="s">
+        <v>582</v>
+      </c>
+      <c r="C23" s="57">
+        <v>2000</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>613</v>
+      </c>
+      <c r="B24" t="s">
+        <v>583</v>
+      </c>
+      <c r="C24" t="s">
+        <v>614</v>
+      </c>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>615</v>
+      </c>
+      <c r="B25" t="s">
+        <v>582</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>593</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>616</v>
+      </c>
+      <c r="B26" t="s">
+        <v>583</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>617</v>
+      </c>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>618</v>
+      </c>
+      <c r="B27" t="s">
+        <v>583</v>
+      </c>
+      <c r="C27" t="s">
+        <v>619</v>
+      </c>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>620</v>
+      </c>
+      <c r="B28" t="s">
+        <v>582</v>
+      </c>
+      <c r="C28" t="s">
+        <v>621</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="D26:M26"/>
+    <mergeCell ref="D27:M27"/>
+    <mergeCell ref="D20:M20"/>
+    <mergeCell ref="D21:M21"/>
+    <mergeCell ref="D22:M22"/>
+    <mergeCell ref="D23:M23"/>
+    <mergeCell ref="D24:M24"/>
+    <mergeCell ref="D25:M25"/>
+    <mergeCell ref="D13:M13"/>
+    <mergeCell ref="D15:M15"/>
+    <mergeCell ref="D16:M16"/>
+    <mergeCell ref="D14:M14"/>
+    <mergeCell ref="D17:M17"/>
+    <mergeCell ref="A19:Q19"/>
+    <mergeCell ref="D6:M6"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="D8:M8"/>
+    <mergeCell ref="D9:M9"/>
+    <mergeCell ref="D10:M10"/>
+    <mergeCell ref="A12:Q12"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="D3:M3"/>
+    <mergeCell ref="D1:M1"/>
+    <mergeCell ref="D4:M4"/>
+    <mergeCell ref="D5:M5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>